<commit_message>
feat(dialog): update CN data and dialogue Excel files
Updated multiple binary Excel files in Original/CN/Data/ and Original/CN/Dialog/Drama/, including character talk, god talk, and various drama dialogues, to reflect latest content changes.
</commit_message>
<xml_diff>
--- a/Original/CN/Dialog/Drama/_main.xlsx
+++ b/Original/CN/Dialog/Drama/_main.xlsx
@@ -822,11 +822,11 @@
 I...well, I'll leave the rest to your imagination.</t>
   </si>
   <si>
-    <t xml:space="preserve">…我々ミシリアの者にとって、シェトラス様は父親であり、頭の上がらぬ先生だ。なにせ、200年もこの国を見守ってきたのだからね。さすがの君も、シェトラス様にはかなわなかったか。
+    <t xml:space="preserve">…我々ミシリアの者にとって、シェトラス様は父親であり、頭の上がらぬ先生だ。なにせ、100年以上もこの国を見守ってきたのだからね。さすがの君も、シェトラス様にはかなわなかったか。
 君が稽古に顔を見せなくなり、街外れの丘で一人リラの練習をしていると聞いたときは、恋の熱にでも浮かされたのかと皆勘ぐったものだ。だが、最近はリラを担いだ姿が板に付いてきている。</t>
   </si>
   <si>
-    <t xml:space="preserve">...For those of us in Mysilia, Master Cetrus is a father and a teacher we cannot look up to. After all, he has been watching over this country for 200 years. Even you are just like a spoiled child to him.
+    <t xml:space="preserve">...For those of us in Mysilia, Master Cetrus is a father and a teacher we cannot look up to. After all, he has been watching over this country for a hundred years and more. Even you are just like a spoiled child to him.
 We all wondered if you had been carried away by the fever of love when you had stopped showing up for practice and we heard that you were practicing lyra alone on a hill. But nowadays, you are getting used to carrying your lyra.</t>
   </si>
   <si>
@@ -1110,7 +1110,7 @@
 …その力を解放するすべは、長い時の流れの中で失われてしまいました。</t>
   </si>
   <si>
-    <t xml:space="preserve">O  daughter of the forest, a mortal, yet one who hears my voice. My name is Ornev, the companion of the great Unyielding Tree, the first being and the mother of all living things in Ylva.
+    <t xml:space="preserve">O  daughter of the forest, a mortal, yet one who hears my voice. My name is Onev, the companion of the great Unyielding Tree, the first being and the mother of all living things in Ylva.
 The crystal you see before you is a petrified form of an ancient tree together with ether. It is a crystal that contains immense power.
 ...The means to release the power has been lost in the long passage of time.</t>
   </si>
@@ -2023,15 +2023,15 @@
   </si>
   <si>
     <t xml:space="preserve">倒也没什么特别值得一说的。
-你也知道，我以前是扎南那边的人，因为做了些蠢事，在10年前逃亡到了米西利亚这边来。那时的我只懂舞刀弄剑的，加上人生地不熟，日子也不好过。</t>
+你也知道，我以前是泽纳恩那边的人，因为做了些蠢事，在10年前逃亡到了米西利亚这边来。那时的我只懂舞刀弄剑的，加上人生地不熟，日子也不好过。</t>
   </si>
   <si>
     <t xml:space="preserve">后来有一天，我在酒馆机缘巧合的遇到了一位弹着莱雅琴的男子。当然，我那时候并不知道他就是赛特拉斯大人。
-只是看大伙都觉得他那样玩弄乐器很优雅，就嘲讽说「乐器是给女人和孩子玩的东西」。后来你猜怎么着，他既不生气也不反驳，而是在看过我一眼后，没把我当回事的自顾自的演奏起了一曲扎南的牧歌。
+只是看大伙都觉得他那样玩弄乐器很优雅，就嘲讽说「乐器是给女人和孩子玩的东西」。后来你猜怎么着，他既不生气也不反驳，而是在看过我一眼后，没把我当回事的自顾自的演奏起了一曲泽纳恩的牧歌。
 然后我就…哎，算了，不跟你说了。后来的事就任你想象吧。</t>
   </si>
   <si>
-    <t xml:space="preserve">…对我们米西利亚人来说，赛特拉斯大人是一位让人感到亲近信任的慈祥父亲，也是一位让人不敢抬头直视的严厉老师。毕竟他已经守护了这个国家200年。你就是发飙也赢不过他吧。
+    <t xml:space="preserve">…对我们米西利亚人来说，赛特拉斯大人是一位让人感到亲近信任的慈祥父亲，也是一位让人不敢抬头直视的严厉老师。毕竟他已经守护了这个国家100多年。我看就算是你，也赢不过赛特拉斯大人吧。
 说起来，后来从人们口中得知你不练习剑术，而是跑到郊外的山丘上一个人练莱雅琴的时候，大家还以为你是爱上了哪个女人呢。不知不觉时间又过去那么久，现在看惯了你背着莱雅琴的样子，反而觉得这样才像你。</t>
   </si>
   <si>
@@ -2044,7 +2044,7 @@
   <si>
     <t xml:space="preserve">我喜欢米西利亚这个地方。
 虽然最开始在这里生活的那段日子里，人们看到我这么个大个子在扛着乐器四处走动都会笑话我，但后来米西利亚终究是接受了无家可归又性格偏激的我。不仅如此，我还在这里找到了毕生的挚友和美丽的妻子，有了个吵闹的秃头老丈人，每天的日子都变得热闹得很啊。
-让那又小又穷的扎南吃屎去吧！我，我要为我好不容易找寻到的故乡献出我的心脏。</t>
+让那又小又穷的泽纳恩吃屎去吧！我，我要为我好不容易找寻到的故乡献出我的心脏。</t>
   </si>
   <si>
     <t xml:space="preserve">…虽然算是借着酒劲说出来的话吧。但你能有这样的觉悟，是谁都会高看你一眼的。
@@ -2353,7 +2353,7 @@
     <t xml:space="preserve">他双手握住一个被扯断了的少女的手臂，蹲在地上。</t>
   </si>
   <si>
-    <t xml:space="preserve">在这场战斗中失去大部分主战斗力的扎南开始撤退。</t>
+    <t xml:space="preserve">在这场战斗中失去大部分主战斗力的泽纳恩开始撤退。</t>
   </si>
   <si>
     <t xml:space="preserve">贝里希失踪了。</t>
@@ -2362,7 +2362,7 @@
     <t xml:space="preserve">- 孤儿院地下 -</t>
   </si>
   <si>
-    <t xml:space="preserve">表现・测试效果。</t>
+    <t xml:space="preserve">表现·测试效果。</t>
   </si>
   <si>
     <t xml:space="preserve">呼唤风吧。</t>
@@ -3269,9 +3269,9 @@
   <dimension ref="A1:IW492"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K482" sqref="K482"/>
-      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
+      <selection pane="bottomLeft" activeCell="J153" sqref="J153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8"/>
@@ -29966,252 +29966,252 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52"/>
-      <c r="L52"/>
-      <c r="M52"/>
-      <c r="N52"/>
-      <c r="O52"/>
-      <c r="P52"/>
-      <c r="Q52"/>
-      <c r="R52"/>
-      <c r="S52"/>
-      <c r="T52"/>
-      <c r="U52"/>
-      <c r="V52"/>
-      <c r="W52"/>
-      <c r="X52"/>
-      <c r="Y52"/>
-      <c r="Z52"/>
-      <c r="AA52"/>
-      <c r="AB52"/>
-      <c r="AC52"/>
-      <c r="AD52"/>
-      <c r="AE52"/>
-      <c r="AF52"/>
-      <c r="AG52"/>
-      <c r="AH52"/>
-      <c r="AI52"/>
-      <c r="AJ52"/>
-      <c r="AK52"/>
-      <c r="AL52"/>
-      <c r="AM52"/>
-      <c r="AN52"/>
-      <c r="AO52"/>
-      <c r="AP52"/>
-      <c r="AQ52"/>
-      <c r="AR52"/>
-      <c r="AS52"/>
-      <c r="AT52"/>
-      <c r="AU52"/>
-      <c r="AV52"/>
-      <c r="AW52"/>
-      <c r="AX52"/>
-      <c r="AY52"/>
-      <c r="AZ52"/>
-      <c r="BA52"/>
-      <c r="BB52"/>
-      <c r="BC52"/>
-      <c r="BD52"/>
-      <c r="BE52"/>
-      <c r="BF52"/>
-      <c r="BG52"/>
-      <c r="BH52"/>
-      <c r="BI52"/>
-      <c r="BJ52"/>
-      <c r="BK52"/>
-      <c r="BL52"/>
-      <c r="BM52"/>
-      <c r="BN52"/>
-      <c r="BO52"/>
-      <c r="BP52"/>
-      <c r="BQ52"/>
-      <c r="BR52"/>
-      <c r="BS52"/>
-      <c r="BT52"/>
-      <c r="BU52"/>
-      <c r="BV52"/>
-      <c r="BW52"/>
-      <c r="BX52"/>
-      <c r="BY52"/>
-      <c r="BZ52"/>
-      <c r="CA52"/>
-      <c r="CB52"/>
-      <c r="CC52"/>
-      <c r="CD52"/>
-      <c r="CE52"/>
-      <c r="CF52"/>
-      <c r="CG52"/>
-      <c r="CH52"/>
-      <c r="CI52"/>
-      <c r="CJ52"/>
-      <c r="CK52"/>
-      <c r="CL52"/>
-      <c r="CM52"/>
-      <c r="CN52"/>
-      <c r="CO52"/>
-      <c r="CP52"/>
-      <c r="CQ52"/>
-      <c r="CR52"/>
-      <c r="CS52"/>
-      <c r="CT52"/>
-      <c r="CU52"/>
-      <c r="CV52"/>
-      <c r="CW52"/>
-      <c r="CX52"/>
-      <c r="CY52"/>
-      <c r="CZ52"/>
-      <c r="DA52"/>
-      <c r="DB52"/>
-      <c r="DC52"/>
-      <c r="DD52"/>
-      <c r="DE52"/>
-      <c r="DF52"/>
-      <c r="DG52"/>
-      <c r="DH52"/>
-      <c r="DI52"/>
-      <c r="DJ52"/>
-      <c r="DK52"/>
-      <c r="DL52"/>
-      <c r="DM52"/>
-      <c r="DN52"/>
-      <c r="DO52"/>
-      <c r="DP52"/>
-      <c r="DQ52"/>
-      <c r="DR52"/>
-      <c r="DS52"/>
-      <c r="DT52"/>
-      <c r="DU52"/>
-      <c r="DV52"/>
-      <c r="DW52"/>
-      <c r="DX52"/>
-      <c r="DY52"/>
-      <c r="DZ52"/>
-      <c r="EA52"/>
-      <c r="EB52"/>
-      <c r="EC52"/>
-      <c r="ED52"/>
-      <c r="EE52"/>
-      <c r="EF52"/>
-      <c r="EG52"/>
-      <c r="EH52"/>
-      <c r="EI52"/>
-      <c r="EJ52"/>
-      <c r="EK52"/>
-      <c r="EL52"/>
-      <c r="EM52"/>
-      <c r="EN52"/>
-      <c r="EO52"/>
-      <c r="EP52"/>
-      <c r="EQ52"/>
-      <c r="ER52"/>
-      <c r="ES52"/>
-      <c r="ET52"/>
-      <c r="EU52"/>
-      <c r="EV52"/>
-      <c r="EW52"/>
-      <c r="EX52"/>
-      <c r="EY52"/>
-      <c r="EZ52"/>
-      <c r="FA52"/>
-      <c r="FB52"/>
-      <c r="FC52"/>
-      <c r="FD52"/>
-      <c r="FE52"/>
-      <c r="FF52"/>
-      <c r="FG52"/>
-      <c r="FH52"/>
-      <c r="FI52"/>
-      <c r="FJ52"/>
-      <c r="FK52"/>
-      <c r="FL52"/>
-      <c r="FM52"/>
-      <c r="FN52"/>
-      <c r="FO52"/>
-      <c r="FP52"/>
-      <c r="FQ52"/>
-      <c r="FR52"/>
-      <c r="FS52"/>
-      <c r="FT52"/>
-      <c r="FU52"/>
-      <c r="FV52"/>
-      <c r="FW52"/>
-      <c r="FX52"/>
-      <c r="FY52"/>
-      <c r="FZ52"/>
-      <c r="GA52"/>
-      <c r="GB52"/>
-      <c r="GC52"/>
-      <c r="GD52"/>
-      <c r="GE52"/>
-      <c r="GF52"/>
-      <c r="GG52"/>
-      <c r="GH52"/>
-      <c r="GI52"/>
-      <c r="GJ52"/>
-      <c r="GK52"/>
-      <c r="GL52"/>
-      <c r="GM52"/>
-      <c r="GN52"/>
-      <c r="GO52"/>
-      <c r="GP52"/>
-      <c r="GQ52"/>
-      <c r="GR52"/>
-      <c r="GS52"/>
-      <c r="GT52"/>
-      <c r="GU52"/>
-      <c r="GV52"/>
-      <c r="GW52"/>
-      <c r="GX52"/>
-      <c r="GY52"/>
-      <c r="GZ52"/>
-      <c r="HA52"/>
-      <c r="HB52"/>
-      <c r="HC52"/>
-      <c r="HD52"/>
-      <c r="HE52"/>
-      <c r="HF52"/>
-      <c r="HG52"/>
-      <c r="HH52"/>
-      <c r="HI52"/>
-      <c r="HJ52"/>
-      <c r="HK52"/>
-      <c r="HL52"/>
-      <c r="HM52"/>
-      <c r="HN52"/>
-      <c r="HO52"/>
-      <c r="HP52"/>
-      <c r="HQ52"/>
-      <c r="HR52"/>
-      <c r="HS52"/>
-      <c r="HT52"/>
-      <c r="HU52"/>
-      <c r="HV52"/>
-      <c r="HW52"/>
-      <c r="HX52"/>
-      <c r="HY52"/>
-      <c r="HZ52"/>
-      <c r="IA52"/>
-      <c r="IB52"/>
-      <c r="IC52"/>
-      <c r="ID52"/>
-      <c r="IE52"/>
-      <c r="IF52"/>
-      <c r="IG52"/>
-      <c r="IH52"/>
-      <c r="II52"/>
-      <c r="IJ52"/>
-      <c r="IK52"/>
-      <c r="IL52"/>
-      <c r="IM52"/>
-      <c r="IN52"/>
-      <c r="IO52"/>
-      <c r="IP52"/>
-      <c r="IQ52"/>
-      <c r="IR52"/>
-      <c r="IS52"/>
-      <c r="IT52"/>
-      <c r="IU52"/>
-      <c r="IV52"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="1"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" s="1"/>
+      <c r="Y52" s="1"/>
+      <c r="Z52" s="1"/>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1"/>
+      <c r="AC52" s="1"/>
+      <c r="AD52" s="1"/>
+      <c r="AE52" s="1"/>
+      <c r="AF52" s="1"/>
+      <c r="AG52" s="1"/>
+      <c r="AH52" s="1"/>
+      <c r="AI52" s="1"/>
+      <c r="AJ52" s="1"/>
+      <c r="AK52" s="1"/>
+      <c r="AL52" s="1"/>
+      <c r="AM52" s="1"/>
+      <c r="AN52" s="1"/>
+      <c r="AO52" s="1"/>
+      <c r="AP52" s="1"/>
+      <c r="AQ52" s="1"/>
+      <c r="AR52" s="1"/>
+      <c r="AS52" s="1"/>
+      <c r="AT52" s="1"/>
+      <c r="AU52" s="1"/>
+      <c r="AV52" s="1"/>
+      <c r="AW52" s="1"/>
+      <c r="AX52" s="1"/>
+      <c r="AY52" s="1"/>
+      <c r="AZ52" s="1"/>
+      <c r="BA52" s="1"/>
+      <c r="BB52" s="1"/>
+      <c r="BC52" s="1"/>
+      <c r="BD52" s="1"/>
+      <c r="BE52" s="1"/>
+      <c r="BF52" s="1"/>
+      <c r="BG52" s="1"/>
+      <c r="BH52" s="1"/>
+      <c r="BI52" s="1"/>
+      <c r="BJ52" s="1"/>
+      <c r="BK52" s="1"/>
+      <c r="BL52" s="1"/>
+      <c r="BM52" s="1"/>
+      <c r="BN52" s="1"/>
+      <c r="BO52" s="1"/>
+      <c r="BP52" s="1"/>
+      <c r="BQ52" s="1"/>
+      <c r="BR52" s="1"/>
+      <c r="BS52" s="1"/>
+      <c r="BT52" s="1"/>
+      <c r="BU52" s="1"/>
+      <c r="BV52" s="1"/>
+      <c r="BW52" s="1"/>
+      <c r="BX52" s="1"/>
+      <c r="BY52" s="1"/>
+      <c r="BZ52" s="1"/>
+      <c r="CA52" s="1"/>
+      <c r="CB52" s="1"/>
+      <c r="CC52" s="1"/>
+      <c r="CD52" s="1"/>
+      <c r="CE52" s="1"/>
+      <c r="CF52" s="1"/>
+      <c r="CG52" s="1"/>
+      <c r="CH52" s="1"/>
+      <c r="CI52" s="1"/>
+      <c r="CJ52" s="1"/>
+      <c r="CK52" s="1"/>
+      <c r="CL52" s="1"/>
+      <c r="CM52" s="1"/>
+      <c r="CN52" s="1"/>
+      <c r="CO52" s="1"/>
+      <c r="CP52" s="1"/>
+      <c r="CQ52" s="1"/>
+      <c r="CR52" s="1"/>
+      <c r="CS52" s="1"/>
+      <c r="CT52" s="1"/>
+      <c r="CU52" s="1"/>
+      <c r="CV52" s="1"/>
+      <c r="CW52" s="1"/>
+      <c r="CX52" s="1"/>
+      <c r="CY52" s="1"/>
+      <c r="CZ52" s="1"/>
+      <c r="DA52" s="1"/>
+      <c r="DB52" s="1"/>
+      <c r="DC52" s="1"/>
+      <c r="DD52" s="1"/>
+      <c r="DE52" s="1"/>
+      <c r="DF52" s="1"/>
+      <c r="DG52" s="1"/>
+      <c r="DH52" s="1"/>
+      <c r="DI52" s="1"/>
+      <c r="DJ52" s="1"/>
+      <c r="DK52" s="1"/>
+      <c r="DL52" s="1"/>
+      <c r="DM52" s="1"/>
+      <c r="DN52" s="1"/>
+      <c r="DO52" s="1"/>
+      <c r="DP52" s="1"/>
+      <c r="DQ52" s="1"/>
+      <c r="DR52" s="1"/>
+      <c r="DS52" s="1"/>
+      <c r="DT52" s="1"/>
+      <c r="DU52" s="1"/>
+      <c r="DV52" s="1"/>
+      <c r="DW52" s="1"/>
+      <c r="DX52" s="1"/>
+      <c r="DY52" s="1"/>
+      <c r="DZ52" s="1"/>
+      <c r="EA52" s="1"/>
+      <c r="EB52" s="1"/>
+      <c r="EC52" s="1"/>
+      <c r="ED52" s="1"/>
+      <c r="EE52" s="1"/>
+      <c r="EF52" s="1"/>
+      <c r="EG52" s="1"/>
+      <c r="EH52" s="1"/>
+      <c r="EI52" s="1"/>
+      <c r="EJ52" s="1"/>
+      <c r="EK52" s="1"/>
+      <c r="EL52" s="1"/>
+      <c r="EM52" s="1"/>
+      <c r="EN52" s="1"/>
+      <c r="EO52" s="1"/>
+      <c r="EP52" s="1"/>
+      <c r="EQ52" s="1"/>
+      <c r="ER52" s="1"/>
+      <c r="ES52" s="1"/>
+      <c r="ET52" s="1"/>
+      <c r="EU52" s="1"/>
+      <c r="EV52" s="1"/>
+      <c r="EW52" s="1"/>
+      <c r="EX52" s="1"/>
+      <c r="EY52" s="1"/>
+      <c r="EZ52" s="1"/>
+      <c r="FA52" s="1"/>
+      <c r="FB52" s="1"/>
+      <c r="FC52" s="1"/>
+      <c r="FD52" s="1"/>
+      <c r="FE52" s="1"/>
+      <c r="FF52" s="1"/>
+      <c r="FG52" s="1"/>
+      <c r="FH52" s="1"/>
+      <c r="FI52" s="1"/>
+      <c r="FJ52" s="1"/>
+      <c r="FK52" s="1"/>
+      <c r="FL52" s="1"/>
+      <c r="FM52" s="1"/>
+      <c r="FN52" s="1"/>
+      <c r="FO52" s="1"/>
+      <c r="FP52" s="1"/>
+      <c r="FQ52" s="1"/>
+      <c r="FR52" s="1"/>
+      <c r="FS52" s="1"/>
+      <c r="FT52" s="1"/>
+      <c r="FU52" s="1"/>
+      <c r="FV52" s="1"/>
+      <c r="FW52" s="1"/>
+      <c r="FX52" s="1"/>
+      <c r="FY52" s="1"/>
+      <c r="FZ52" s="1"/>
+      <c r="GA52" s="1"/>
+      <c r="GB52" s="1"/>
+      <c r="GC52" s="1"/>
+      <c r="GD52" s="1"/>
+      <c r="GE52" s="1"/>
+      <c r="GF52" s="1"/>
+      <c r="GG52" s="1"/>
+      <c r="GH52" s="1"/>
+      <c r="GI52" s="1"/>
+      <c r="GJ52" s="1"/>
+      <c r="GK52" s="1"/>
+      <c r="GL52" s="1"/>
+      <c r="GM52" s="1"/>
+      <c r="GN52" s="1"/>
+      <c r="GO52" s="1"/>
+      <c r="GP52" s="1"/>
+      <c r="GQ52" s="1"/>
+      <c r="GR52" s="1"/>
+      <c r="GS52" s="1"/>
+      <c r="GT52" s="1"/>
+      <c r="GU52" s="1"/>
+      <c r="GV52" s="1"/>
+      <c r="GW52" s="1"/>
+      <c r="GX52" s="1"/>
+      <c r="GY52" s="1"/>
+      <c r="GZ52" s="1"/>
+      <c r="HA52" s="1"/>
+      <c r="HB52" s="1"/>
+      <c r="HC52" s="1"/>
+      <c r="HD52" s="1"/>
+      <c r="HE52" s="1"/>
+      <c r="HF52" s="1"/>
+      <c r="HG52" s="1"/>
+      <c r="HH52" s="1"/>
+      <c r="HI52" s="1"/>
+      <c r="HJ52" s="1"/>
+      <c r="HK52" s="1"/>
+      <c r="HL52" s="1"/>
+      <c r="HM52" s="1"/>
+      <c r="HN52" s="1"/>
+      <c r="HO52" s="1"/>
+      <c r="HP52" s="1"/>
+      <c r="HQ52" s="1"/>
+      <c r="HR52" s="1"/>
+      <c r="HS52" s="1"/>
+      <c r="HT52" s="1"/>
+      <c r="HU52" s="1"/>
+      <c r="HV52" s="1"/>
+      <c r="HW52" s="1"/>
+      <c r="HX52" s="1"/>
+      <c r="HY52" s="1"/>
+      <c r="HZ52" s="1"/>
+      <c r="IA52" s="1"/>
+      <c r="IB52" s="1"/>
+      <c r="IC52" s="1"/>
+      <c r="ID52" s="1"/>
+      <c r="IE52" s="1"/>
+      <c r="IF52" s="1"/>
+      <c r="IG52" s="1"/>
+      <c r="IH52" s="1"/>
+      <c r="II52" s="1"/>
+      <c r="IJ52" s="1"/>
+      <c r="IK52" s="1"/>
+      <c r="IL52" s="1"/>
+      <c r="IM52" s="1"/>
+      <c r="IN52" s="1"/>
+      <c r="IO52" s="1"/>
+      <c r="IP52" s="1"/>
+      <c r="IQ52" s="1"/>
+      <c r="IR52" s="1"/>
+      <c r="IS52" s="1"/>
+      <c r="IT52" s="1"/>
+      <c r="IU52" s="1"/>
+      <c r="IV52" s="1"/>
     </row>
     <row r="53" ht="12.8">
       <c r="K53" s="1"/>
@@ -31179,252 +31179,252 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
-      <c r="K80"/>
-      <c r="L80"/>
-      <c r="M80"/>
-      <c r="N80"/>
-      <c r="O80"/>
-      <c r="P80"/>
-      <c r="Q80"/>
-      <c r="R80"/>
-      <c r="S80"/>
-      <c r="T80"/>
-      <c r="U80"/>
-      <c r="V80"/>
-      <c r="W80"/>
-      <c r="X80"/>
-      <c r="Y80"/>
-      <c r="Z80"/>
-      <c r="AA80"/>
-      <c r="AB80"/>
-      <c r="AC80"/>
-      <c r="AD80"/>
-      <c r="AE80"/>
-      <c r="AF80"/>
-      <c r="AG80"/>
-      <c r="AH80"/>
-      <c r="AI80"/>
-      <c r="AJ80"/>
-      <c r="AK80"/>
-      <c r="AL80"/>
-      <c r="AM80"/>
-      <c r="AN80"/>
-      <c r="AO80"/>
-      <c r="AP80"/>
-      <c r="AQ80"/>
-      <c r="AR80"/>
-      <c r="AS80"/>
-      <c r="AT80"/>
-      <c r="AU80"/>
-      <c r="AV80"/>
-      <c r="AW80"/>
-      <c r="AX80"/>
-      <c r="AY80"/>
-      <c r="AZ80"/>
-      <c r="BA80"/>
-      <c r="BB80"/>
-      <c r="BC80"/>
-      <c r="BD80"/>
-      <c r="BE80"/>
-      <c r="BF80"/>
-      <c r="BG80"/>
-      <c r="BH80"/>
-      <c r="BI80"/>
-      <c r="BJ80"/>
-      <c r="BK80"/>
-      <c r="BL80"/>
-      <c r="BM80"/>
-      <c r="BN80"/>
-      <c r="BO80"/>
-      <c r="BP80"/>
-      <c r="BQ80"/>
-      <c r="BR80"/>
-      <c r="BS80"/>
-      <c r="BT80"/>
-      <c r="BU80"/>
-      <c r="BV80"/>
-      <c r="BW80"/>
-      <c r="BX80"/>
-      <c r="BY80"/>
-      <c r="BZ80"/>
-      <c r="CA80"/>
-      <c r="CB80"/>
-      <c r="CC80"/>
-      <c r="CD80"/>
-      <c r="CE80"/>
-      <c r="CF80"/>
-      <c r="CG80"/>
-      <c r="CH80"/>
-      <c r="CI80"/>
-      <c r="CJ80"/>
-      <c r="CK80"/>
-      <c r="CL80"/>
-      <c r="CM80"/>
-      <c r="CN80"/>
-      <c r="CO80"/>
-      <c r="CP80"/>
-      <c r="CQ80"/>
-      <c r="CR80"/>
-      <c r="CS80"/>
-      <c r="CT80"/>
-      <c r="CU80"/>
-      <c r="CV80"/>
-      <c r="CW80"/>
-      <c r="CX80"/>
-      <c r="CY80"/>
-      <c r="CZ80"/>
-      <c r="DA80"/>
-      <c r="DB80"/>
-      <c r="DC80"/>
-      <c r="DD80"/>
-      <c r="DE80"/>
-      <c r="DF80"/>
-      <c r="DG80"/>
-      <c r="DH80"/>
-      <c r="DI80"/>
-      <c r="DJ80"/>
-      <c r="DK80"/>
-      <c r="DL80"/>
-      <c r="DM80"/>
-      <c r="DN80"/>
-      <c r="DO80"/>
-      <c r="DP80"/>
-      <c r="DQ80"/>
-      <c r="DR80"/>
-      <c r="DS80"/>
-      <c r="DT80"/>
-      <c r="DU80"/>
-      <c r="DV80"/>
-      <c r="DW80"/>
-      <c r="DX80"/>
-      <c r="DY80"/>
-      <c r="DZ80"/>
-      <c r="EA80"/>
-      <c r="EB80"/>
-      <c r="EC80"/>
-      <c r="ED80"/>
-      <c r="EE80"/>
-      <c r="EF80"/>
-      <c r="EG80"/>
-      <c r="EH80"/>
-      <c r="EI80"/>
-      <c r="EJ80"/>
-      <c r="EK80"/>
-      <c r="EL80"/>
-      <c r="EM80"/>
-      <c r="EN80"/>
-      <c r="EO80"/>
-      <c r="EP80"/>
-      <c r="EQ80"/>
-      <c r="ER80"/>
-      <c r="ES80"/>
-      <c r="ET80"/>
-      <c r="EU80"/>
-      <c r="EV80"/>
-      <c r="EW80"/>
-      <c r="EX80"/>
-      <c r="EY80"/>
-      <c r="EZ80"/>
-      <c r="FA80"/>
-      <c r="FB80"/>
-      <c r="FC80"/>
-      <c r="FD80"/>
-      <c r="FE80"/>
-      <c r="FF80"/>
-      <c r="FG80"/>
-      <c r="FH80"/>
-      <c r="FI80"/>
-      <c r="FJ80"/>
-      <c r="FK80"/>
-      <c r="FL80"/>
-      <c r="FM80"/>
-      <c r="FN80"/>
-      <c r="FO80"/>
-      <c r="FP80"/>
-      <c r="FQ80"/>
-      <c r="FR80"/>
-      <c r="FS80"/>
-      <c r="FT80"/>
-      <c r="FU80"/>
-      <c r="FV80"/>
-      <c r="FW80"/>
-      <c r="FX80"/>
-      <c r="FY80"/>
-      <c r="FZ80"/>
-      <c r="GA80"/>
-      <c r="GB80"/>
-      <c r="GC80"/>
-      <c r="GD80"/>
-      <c r="GE80"/>
-      <c r="GF80"/>
-      <c r="GG80"/>
-      <c r="GH80"/>
-      <c r="GI80"/>
-      <c r="GJ80"/>
-      <c r="GK80"/>
-      <c r="GL80"/>
-      <c r="GM80"/>
-      <c r="GN80"/>
-      <c r="GO80"/>
-      <c r="GP80"/>
-      <c r="GQ80"/>
-      <c r="GR80"/>
-      <c r="GS80"/>
-      <c r="GT80"/>
-      <c r="GU80"/>
-      <c r="GV80"/>
-      <c r="GW80"/>
-      <c r="GX80"/>
-      <c r="GY80"/>
-      <c r="GZ80"/>
-      <c r="HA80"/>
-      <c r="HB80"/>
-      <c r="HC80"/>
-      <c r="HD80"/>
-      <c r="HE80"/>
-      <c r="HF80"/>
-      <c r="HG80"/>
-      <c r="HH80"/>
-      <c r="HI80"/>
-      <c r="HJ80"/>
-      <c r="HK80"/>
-      <c r="HL80"/>
-      <c r="HM80"/>
-      <c r="HN80"/>
-      <c r="HO80"/>
-      <c r="HP80"/>
-      <c r="HQ80"/>
-      <c r="HR80"/>
-      <c r="HS80"/>
-      <c r="HT80"/>
-      <c r="HU80"/>
-      <c r="HV80"/>
-      <c r="HW80"/>
-      <c r="HX80"/>
-      <c r="HY80"/>
-      <c r="HZ80"/>
-      <c r="IA80"/>
-      <c r="IB80"/>
-      <c r="IC80"/>
-      <c r="ID80"/>
-      <c r="IE80"/>
-      <c r="IF80"/>
-      <c r="IG80"/>
-      <c r="IH80"/>
-      <c r="II80"/>
-      <c r="IJ80"/>
-      <c r="IK80"/>
-      <c r="IL80"/>
-      <c r="IM80"/>
-      <c r="IN80"/>
-      <c r="IO80"/>
-      <c r="IP80"/>
-      <c r="IQ80"/>
-      <c r="IR80"/>
-      <c r="IS80"/>
-      <c r="IT80"/>
-      <c r="IU80"/>
-      <c r="IV80"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="W80" s="1"/>
+      <c r="X80" s="1"/>
+      <c r="Y80" s="1"/>
+      <c r="Z80" s="1"/>
+      <c r="AA80" s="1"/>
+      <c r="AB80" s="1"/>
+      <c r="AC80" s="1"/>
+      <c r="AD80" s="1"/>
+      <c r="AE80" s="1"/>
+      <c r="AF80" s="1"/>
+      <c r="AG80" s="1"/>
+      <c r="AH80" s="1"/>
+      <c r="AI80" s="1"/>
+      <c r="AJ80" s="1"/>
+      <c r="AK80" s="1"/>
+      <c r="AL80" s="1"/>
+      <c r="AM80" s="1"/>
+      <c r="AN80" s="1"/>
+      <c r="AO80" s="1"/>
+      <c r="AP80" s="1"/>
+      <c r="AQ80" s="1"/>
+      <c r="AR80" s="1"/>
+      <c r="AS80" s="1"/>
+      <c r="AT80" s="1"/>
+      <c r="AU80" s="1"/>
+      <c r="AV80" s="1"/>
+      <c r="AW80" s="1"/>
+      <c r="AX80" s="1"/>
+      <c r="AY80" s="1"/>
+      <c r="AZ80" s="1"/>
+      <c r="BA80" s="1"/>
+      <c r="BB80" s="1"/>
+      <c r="BC80" s="1"/>
+      <c r="BD80" s="1"/>
+      <c r="BE80" s="1"/>
+      <c r="BF80" s="1"/>
+      <c r="BG80" s="1"/>
+      <c r="BH80" s="1"/>
+      <c r="BI80" s="1"/>
+      <c r="BJ80" s="1"/>
+      <c r="BK80" s="1"/>
+      <c r="BL80" s="1"/>
+      <c r="BM80" s="1"/>
+      <c r="BN80" s="1"/>
+      <c r="BO80" s="1"/>
+      <c r="BP80" s="1"/>
+      <c r="BQ80" s="1"/>
+      <c r="BR80" s="1"/>
+      <c r="BS80" s="1"/>
+      <c r="BT80" s="1"/>
+      <c r="BU80" s="1"/>
+      <c r="BV80" s="1"/>
+      <c r="BW80" s="1"/>
+      <c r="BX80" s="1"/>
+      <c r="BY80" s="1"/>
+      <c r="BZ80" s="1"/>
+      <c r="CA80" s="1"/>
+      <c r="CB80" s="1"/>
+      <c r="CC80" s="1"/>
+      <c r="CD80" s="1"/>
+      <c r="CE80" s="1"/>
+      <c r="CF80" s="1"/>
+      <c r="CG80" s="1"/>
+      <c r="CH80" s="1"/>
+      <c r="CI80" s="1"/>
+      <c r="CJ80" s="1"/>
+      <c r="CK80" s="1"/>
+      <c r="CL80" s="1"/>
+      <c r="CM80" s="1"/>
+      <c r="CN80" s="1"/>
+      <c r="CO80" s="1"/>
+      <c r="CP80" s="1"/>
+      <c r="CQ80" s="1"/>
+      <c r="CR80" s="1"/>
+      <c r="CS80" s="1"/>
+      <c r="CT80" s="1"/>
+      <c r="CU80" s="1"/>
+      <c r="CV80" s="1"/>
+      <c r="CW80" s="1"/>
+      <c r="CX80" s="1"/>
+      <c r="CY80" s="1"/>
+      <c r="CZ80" s="1"/>
+      <c r="DA80" s="1"/>
+      <c r="DB80" s="1"/>
+      <c r="DC80" s="1"/>
+      <c r="DD80" s="1"/>
+      <c r="DE80" s="1"/>
+      <c r="DF80" s="1"/>
+      <c r="DG80" s="1"/>
+      <c r="DH80" s="1"/>
+      <c r="DI80" s="1"/>
+      <c r="DJ80" s="1"/>
+      <c r="DK80" s="1"/>
+      <c r="DL80" s="1"/>
+      <c r="DM80" s="1"/>
+      <c r="DN80" s="1"/>
+      <c r="DO80" s="1"/>
+      <c r="DP80" s="1"/>
+      <c r="DQ80" s="1"/>
+      <c r="DR80" s="1"/>
+      <c r="DS80" s="1"/>
+      <c r="DT80" s="1"/>
+      <c r="DU80" s="1"/>
+      <c r="DV80" s="1"/>
+      <c r="DW80" s="1"/>
+      <c r="DX80" s="1"/>
+      <c r="DY80" s="1"/>
+      <c r="DZ80" s="1"/>
+      <c r="EA80" s="1"/>
+      <c r="EB80" s="1"/>
+      <c r="EC80" s="1"/>
+      <c r="ED80" s="1"/>
+      <c r="EE80" s="1"/>
+      <c r="EF80" s="1"/>
+      <c r="EG80" s="1"/>
+      <c r="EH80" s="1"/>
+      <c r="EI80" s="1"/>
+      <c r="EJ80" s="1"/>
+      <c r="EK80" s="1"/>
+      <c r="EL80" s="1"/>
+      <c r="EM80" s="1"/>
+      <c r="EN80" s="1"/>
+      <c r="EO80" s="1"/>
+      <c r="EP80" s="1"/>
+      <c r="EQ80" s="1"/>
+      <c r="ER80" s="1"/>
+      <c r="ES80" s="1"/>
+      <c r="ET80" s="1"/>
+      <c r="EU80" s="1"/>
+      <c r="EV80" s="1"/>
+      <c r="EW80" s="1"/>
+      <c r="EX80" s="1"/>
+      <c r="EY80" s="1"/>
+      <c r="EZ80" s="1"/>
+      <c r="FA80" s="1"/>
+      <c r="FB80" s="1"/>
+      <c r="FC80" s="1"/>
+      <c r="FD80" s="1"/>
+      <c r="FE80" s="1"/>
+      <c r="FF80" s="1"/>
+      <c r="FG80" s="1"/>
+      <c r="FH80" s="1"/>
+      <c r="FI80" s="1"/>
+      <c r="FJ80" s="1"/>
+      <c r="FK80" s="1"/>
+      <c r="FL80" s="1"/>
+      <c r="FM80" s="1"/>
+      <c r="FN80" s="1"/>
+      <c r="FO80" s="1"/>
+      <c r="FP80" s="1"/>
+      <c r="FQ80" s="1"/>
+      <c r="FR80" s="1"/>
+      <c r="FS80" s="1"/>
+      <c r="FT80" s="1"/>
+      <c r="FU80" s="1"/>
+      <c r="FV80" s="1"/>
+      <c r="FW80" s="1"/>
+      <c r="FX80" s="1"/>
+      <c r="FY80" s="1"/>
+      <c r="FZ80" s="1"/>
+      <c r="GA80" s="1"/>
+      <c r="GB80" s="1"/>
+      <c r="GC80" s="1"/>
+      <c r="GD80" s="1"/>
+      <c r="GE80" s="1"/>
+      <c r="GF80" s="1"/>
+      <c r="GG80" s="1"/>
+      <c r="GH80" s="1"/>
+      <c r="GI80" s="1"/>
+      <c r="GJ80" s="1"/>
+      <c r="GK80" s="1"/>
+      <c r="GL80" s="1"/>
+      <c r="GM80" s="1"/>
+      <c r="GN80" s="1"/>
+      <c r="GO80" s="1"/>
+      <c r="GP80" s="1"/>
+      <c r="GQ80" s="1"/>
+      <c r="GR80" s="1"/>
+      <c r="GS80" s="1"/>
+      <c r="GT80" s="1"/>
+      <c r="GU80" s="1"/>
+      <c r="GV80" s="1"/>
+      <c r="GW80" s="1"/>
+      <c r="GX80" s="1"/>
+      <c r="GY80" s="1"/>
+      <c r="GZ80" s="1"/>
+      <c r="HA80" s="1"/>
+      <c r="HB80" s="1"/>
+      <c r="HC80" s="1"/>
+      <c r="HD80" s="1"/>
+      <c r="HE80" s="1"/>
+      <c r="HF80" s="1"/>
+      <c r="HG80" s="1"/>
+      <c r="HH80" s="1"/>
+      <c r="HI80" s="1"/>
+      <c r="HJ80" s="1"/>
+      <c r="HK80" s="1"/>
+      <c r="HL80" s="1"/>
+      <c r="HM80" s="1"/>
+      <c r="HN80" s="1"/>
+      <c r="HO80" s="1"/>
+      <c r="HP80" s="1"/>
+      <c r="HQ80" s="1"/>
+      <c r="HR80" s="1"/>
+      <c r="HS80" s="1"/>
+      <c r="HT80" s="1"/>
+      <c r="HU80" s="1"/>
+      <c r="HV80" s="1"/>
+      <c r="HW80" s="1"/>
+      <c r="HX80" s="1"/>
+      <c r="HY80" s="1"/>
+      <c r="HZ80" s="1"/>
+      <c r="IA80" s="1"/>
+      <c r="IB80" s="1"/>
+      <c r="IC80" s="1"/>
+      <c r="ID80" s="1"/>
+      <c r="IE80" s="1"/>
+      <c r="IF80" s="1"/>
+      <c r="IG80" s="1"/>
+      <c r="IH80" s="1"/>
+      <c r="II80" s="1"/>
+      <c r="IJ80" s="1"/>
+      <c r="IK80" s="1"/>
+      <c r="IL80" s="1"/>
+      <c r="IM80" s="1"/>
+      <c r="IN80" s="1"/>
+      <c r="IO80" s="1"/>
+      <c r="IP80" s="1"/>
+      <c r="IQ80" s="1"/>
+      <c r="IR80" s="1"/>
+      <c r="IS80" s="1"/>
+      <c r="IT80" s="1"/>
+      <c r="IU80" s="1"/>
+      <c r="IV80" s="1"/>
     </row>
     <row r="81" ht="12.8">
       <c r="K81" s="1"/>
@@ -32341,254 +32341,254 @@
         <v>472</v>
       </c>
       <c r="J105" s="1"/>
-      <c r="K105" t="s">
+      <c r="K105" s="1" t="s">
         <v>684</v>
       </c>
-      <c r="L105"/>
-      <c r="M105"/>
-      <c r="N105"/>
-      <c r="O105"/>
-      <c r="P105"/>
-      <c r="Q105"/>
-      <c r="R105"/>
-      <c r="S105"/>
-      <c r="T105"/>
-      <c r="U105"/>
-      <c r="V105"/>
-      <c r="W105"/>
-      <c r="X105"/>
-      <c r="Y105"/>
-      <c r="Z105"/>
-      <c r="AA105"/>
-      <c r="AB105"/>
-      <c r="AC105"/>
-      <c r="AD105"/>
-      <c r="AE105"/>
-      <c r="AF105"/>
-      <c r="AG105"/>
-      <c r="AH105"/>
-      <c r="AI105"/>
-      <c r="AJ105"/>
-      <c r="AK105"/>
-      <c r="AL105"/>
-      <c r="AM105"/>
-      <c r="AN105"/>
-      <c r="AO105"/>
-      <c r="AP105"/>
-      <c r="AQ105"/>
-      <c r="AR105"/>
-      <c r="AS105"/>
-      <c r="AT105"/>
-      <c r="AU105"/>
-      <c r="AV105"/>
-      <c r="AW105"/>
-      <c r="AX105"/>
-      <c r="AY105"/>
-      <c r="AZ105"/>
-      <c r="BA105"/>
-      <c r="BB105"/>
-      <c r="BC105"/>
-      <c r="BD105"/>
-      <c r="BE105"/>
-      <c r="BF105"/>
-      <c r="BG105"/>
-      <c r="BH105"/>
-      <c r="BI105"/>
-      <c r="BJ105"/>
-      <c r="BK105"/>
-      <c r="BL105"/>
-      <c r="BM105"/>
-      <c r="BN105"/>
-      <c r="BO105"/>
-      <c r="BP105"/>
-      <c r="BQ105"/>
-      <c r="BR105"/>
-      <c r="BS105"/>
-      <c r="BT105"/>
-      <c r="BU105"/>
-      <c r="BV105"/>
-      <c r="BW105"/>
-      <c r="BX105"/>
-      <c r="BY105"/>
-      <c r="BZ105"/>
-      <c r="CA105"/>
-      <c r="CB105"/>
-      <c r="CC105"/>
-      <c r="CD105"/>
-      <c r="CE105"/>
-      <c r="CF105"/>
-      <c r="CG105"/>
-      <c r="CH105"/>
-      <c r="CI105"/>
-      <c r="CJ105"/>
-      <c r="CK105"/>
-      <c r="CL105"/>
-      <c r="CM105"/>
-      <c r="CN105"/>
-      <c r="CO105"/>
-      <c r="CP105"/>
-      <c r="CQ105"/>
-      <c r="CR105"/>
-      <c r="CS105"/>
-      <c r="CT105"/>
-      <c r="CU105"/>
-      <c r="CV105"/>
-      <c r="CW105"/>
-      <c r="CX105"/>
-      <c r="CY105"/>
-      <c r="CZ105"/>
-      <c r="DA105"/>
-      <c r="DB105"/>
-      <c r="DC105"/>
-      <c r="DD105"/>
-      <c r="DE105"/>
-      <c r="DF105"/>
-      <c r="DG105"/>
-      <c r="DH105"/>
-      <c r="DI105"/>
-      <c r="DJ105"/>
-      <c r="DK105"/>
-      <c r="DL105"/>
-      <c r="DM105"/>
-      <c r="DN105"/>
-      <c r="DO105"/>
-      <c r="DP105"/>
-      <c r="DQ105"/>
-      <c r="DR105"/>
-      <c r="DS105"/>
-      <c r="DT105"/>
-      <c r="DU105"/>
-      <c r="DV105"/>
-      <c r="DW105"/>
-      <c r="DX105"/>
-      <c r="DY105"/>
-      <c r="DZ105"/>
-      <c r="EA105"/>
-      <c r="EB105"/>
-      <c r="EC105"/>
-      <c r="ED105"/>
-      <c r="EE105"/>
-      <c r="EF105"/>
-      <c r="EG105"/>
-      <c r="EH105"/>
-      <c r="EI105"/>
-      <c r="EJ105"/>
-      <c r="EK105"/>
-      <c r="EL105"/>
-      <c r="EM105"/>
-      <c r="EN105"/>
-      <c r="EO105"/>
-      <c r="EP105"/>
-      <c r="EQ105"/>
-      <c r="ER105"/>
-      <c r="ES105"/>
-      <c r="ET105"/>
-      <c r="EU105"/>
-      <c r="EV105"/>
-      <c r="EW105"/>
-      <c r="EX105"/>
-      <c r="EY105"/>
-      <c r="EZ105"/>
-      <c r="FA105"/>
-      <c r="FB105"/>
-      <c r="FC105"/>
-      <c r="FD105"/>
-      <c r="FE105"/>
-      <c r="FF105"/>
-      <c r="FG105"/>
-      <c r="FH105"/>
-      <c r="FI105"/>
-      <c r="FJ105"/>
-      <c r="FK105"/>
-      <c r="FL105"/>
-      <c r="FM105"/>
-      <c r="FN105"/>
-      <c r="FO105"/>
-      <c r="FP105"/>
-      <c r="FQ105"/>
-      <c r="FR105"/>
-      <c r="FS105"/>
-      <c r="FT105"/>
-      <c r="FU105"/>
-      <c r="FV105"/>
-      <c r="FW105"/>
-      <c r="FX105"/>
-      <c r="FY105"/>
-      <c r="FZ105"/>
-      <c r="GA105"/>
-      <c r="GB105"/>
-      <c r="GC105"/>
-      <c r="GD105"/>
-      <c r="GE105"/>
-      <c r="GF105"/>
-      <c r="GG105"/>
-      <c r="GH105"/>
-      <c r="GI105"/>
-      <c r="GJ105"/>
-      <c r="GK105"/>
-      <c r="GL105"/>
-      <c r="GM105"/>
-      <c r="GN105"/>
-      <c r="GO105"/>
-      <c r="GP105"/>
-      <c r="GQ105"/>
-      <c r="GR105"/>
-      <c r="GS105"/>
-      <c r="GT105"/>
-      <c r="GU105"/>
-      <c r="GV105"/>
-      <c r="GW105"/>
-      <c r="GX105"/>
-      <c r="GY105"/>
-      <c r="GZ105"/>
-      <c r="HA105"/>
-      <c r="HB105"/>
-      <c r="HC105"/>
-      <c r="HD105"/>
-      <c r="HE105"/>
-      <c r="HF105"/>
-      <c r="HG105"/>
-      <c r="HH105"/>
-      <c r="HI105"/>
-      <c r="HJ105"/>
-      <c r="HK105"/>
-      <c r="HL105"/>
-      <c r="HM105"/>
-      <c r="HN105"/>
-      <c r="HO105"/>
-      <c r="HP105"/>
-      <c r="HQ105"/>
-      <c r="HR105"/>
-      <c r="HS105"/>
-      <c r="HT105"/>
-      <c r="HU105"/>
-      <c r="HV105"/>
-      <c r="HW105"/>
-      <c r="HX105"/>
-      <c r="HY105"/>
-      <c r="HZ105"/>
-      <c r="IA105"/>
-      <c r="IB105"/>
-      <c r="IC105"/>
-      <c r="ID105"/>
-      <c r="IE105"/>
-      <c r="IF105"/>
-      <c r="IG105"/>
-      <c r="IH105"/>
-      <c r="II105"/>
-      <c r="IJ105"/>
-      <c r="IK105"/>
-      <c r="IL105"/>
-      <c r="IM105"/>
-      <c r="IN105"/>
-      <c r="IO105"/>
-      <c r="IP105"/>
-      <c r="IQ105"/>
-      <c r="IR105"/>
-      <c r="IS105"/>
-      <c r="IT105"/>
-      <c r="IU105"/>
-      <c r="IV105"/>
+      <c r="L105" s="1"/>
+      <c r="M105" s="1"/>
+      <c r="N105" s="1"/>
+      <c r="O105" s="1"/>
+      <c r="P105" s="1"/>
+      <c r="Q105" s="1"/>
+      <c r="R105" s="1"/>
+      <c r="S105" s="1"/>
+      <c r="T105" s="1"/>
+      <c r="U105" s="1"/>
+      <c r="V105" s="1"/>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+      <c r="Y105" s="1"/>
+      <c r="Z105" s="1"/>
+      <c r="AA105" s="1"/>
+      <c r="AB105" s="1"/>
+      <c r="AC105" s="1"/>
+      <c r="AD105" s="1"/>
+      <c r="AE105" s="1"/>
+      <c r="AF105" s="1"/>
+      <c r="AG105" s="1"/>
+      <c r="AH105" s="1"/>
+      <c r="AI105" s="1"/>
+      <c r="AJ105" s="1"/>
+      <c r="AK105" s="1"/>
+      <c r="AL105" s="1"/>
+      <c r="AM105" s="1"/>
+      <c r="AN105" s="1"/>
+      <c r="AO105" s="1"/>
+      <c r="AP105" s="1"/>
+      <c r="AQ105" s="1"/>
+      <c r="AR105" s="1"/>
+      <c r="AS105" s="1"/>
+      <c r="AT105" s="1"/>
+      <c r="AU105" s="1"/>
+      <c r="AV105" s="1"/>
+      <c r="AW105" s="1"/>
+      <c r="AX105" s="1"/>
+      <c r="AY105" s="1"/>
+      <c r="AZ105" s="1"/>
+      <c r="BA105" s="1"/>
+      <c r="BB105" s="1"/>
+      <c r="BC105" s="1"/>
+      <c r="BD105" s="1"/>
+      <c r="BE105" s="1"/>
+      <c r="BF105" s="1"/>
+      <c r="BG105" s="1"/>
+      <c r="BH105" s="1"/>
+      <c r="BI105" s="1"/>
+      <c r="BJ105" s="1"/>
+      <c r="BK105" s="1"/>
+      <c r="BL105" s="1"/>
+      <c r="BM105" s="1"/>
+      <c r="BN105" s="1"/>
+      <c r="BO105" s="1"/>
+      <c r="BP105" s="1"/>
+      <c r="BQ105" s="1"/>
+      <c r="BR105" s="1"/>
+      <c r="BS105" s="1"/>
+      <c r="BT105" s="1"/>
+      <c r="BU105" s="1"/>
+      <c r="BV105" s="1"/>
+      <c r="BW105" s="1"/>
+      <c r="BX105" s="1"/>
+      <c r="BY105" s="1"/>
+      <c r="BZ105" s="1"/>
+      <c r="CA105" s="1"/>
+      <c r="CB105" s="1"/>
+      <c r="CC105" s="1"/>
+      <c r="CD105" s="1"/>
+      <c r="CE105" s="1"/>
+      <c r="CF105" s="1"/>
+      <c r="CG105" s="1"/>
+      <c r="CH105" s="1"/>
+      <c r="CI105" s="1"/>
+      <c r="CJ105" s="1"/>
+      <c r="CK105" s="1"/>
+      <c r="CL105" s="1"/>
+      <c r="CM105" s="1"/>
+      <c r="CN105" s="1"/>
+      <c r="CO105" s="1"/>
+      <c r="CP105" s="1"/>
+      <c r="CQ105" s="1"/>
+      <c r="CR105" s="1"/>
+      <c r="CS105" s="1"/>
+      <c r="CT105" s="1"/>
+      <c r="CU105" s="1"/>
+      <c r="CV105" s="1"/>
+      <c r="CW105" s="1"/>
+      <c r="CX105" s="1"/>
+      <c r="CY105" s="1"/>
+      <c r="CZ105" s="1"/>
+      <c r="DA105" s="1"/>
+      <c r="DB105" s="1"/>
+      <c r="DC105" s="1"/>
+      <c r="DD105" s="1"/>
+      <c r="DE105" s="1"/>
+      <c r="DF105" s="1"/>
+      <c r="DG105" s="1"/>
+      <c r="DH105" s="1"/>
+      <c r="DI105" s="1"/>
+      <c r="DJ105" s="1"/>
+      <c r="DK105" s="1"/>
+      <c r="DL105" s="1"/>
+      <c r="DM105" s="1"/>
+      <c r="DN105" s="1"/>
+      <c r="DO105" s="1"/>
+      <c r="DP105" s="1"/>
+      <c r="DQ105" s="1"/>
+      <c r="DR105" s="1"/>
+      <c r="DS105" s="1"/>
+      <c r="DT105" s="1"/>
+      <c r="DU105" s="1"/>
+      <c r="DV105" s="1"/>
+      <c r="DW105" s="1"/>
+      <c r="DX105" s="1"/>
+      <c r="DY105" s="1"/>
+      <c r="DZ105" s="1"/>
+      <c r="EA105" s="1"/>
+      <c r="EB105" s="1"/>
+      <c r="EC105" s="1"/>
+      <c r="ED105" s="1"/>
+      <c r="EE105" s="1"/>
+      <c r="EF105" s="1"/>
+      <c r="EG105" s="1"/>
+      <c r="EH105" s="1"/>
+      <c r="EI105" s="1"/>
+      <c r="EJ105" s="1"/>
+      <c r="EK105" s="1"/>
+      <c r="EL105" s="1"/>
+      <c r="EM105" s="1"/>
+      <c r="EN105" s="1"/>
+      <c r="EO105" s="1"/>
+      <c r="EP105" s="1"/>
+      <c r="EQ105" s="1"/>
+      <c r="ER105" s="1"/>
+      <c r="ES105" s="1"/>
+      <c r="ET105" s="1"/>
+      <c r="EU105" s="1"/>
+      <c r="EV105" s="1"/>
+      <c r="EW105" s="1"/>
+      <c r="EX105" s="1"/>
+      <c r="EY105" s="1"/>
+      <c r="EZ105" s="1"/>
+      <c r="FA105" s="1"/>
+      <c r="FB105" s="1"/>
+      <c r="FC105" s="1"/>
+      <c r="FD105" s="1"/>
+      <c r="FE105" s="1"/>
+      <c r="FF105" s="1"/>
+      <c r="FG105" s="1"/>
+      <c r="FH105" s="1"/>
+      <c r="FI105" s="1"/>
+      <c r="FJ105" s="1"/>
+      <c r="FK105" s="1"/>
+      <c r="FL105" s="1"/>
+      <c r="FM105" s="1"/>
+      <c r="FN105" s="1"/>
+      <c r="FO105" s="1"/>
+      <c r="FP105" s="1"/>
+      <c r="FQ105" s="1"/>
+      <c r="FR105" s="1"/>
+      <c r="FS105" s="1"/>
+      <c r="FT105" s="1"/>
+      <c r="FU105" s="1"/>
+      <c r="FV105" s="1"/>
+      <c r="FW105" s="1"/>
+      <c r="FX105" s="1"/>
+      <c r="FY105" s="1"/>
+      <c r="FZ105" s="1"/>
+      <c r="GA105" s="1"/>
+      <c r="GB105" s="1"/>
+      <c r="GC105" s="1"/>
+      <c r="GD105" s="1"/>
+      <c r="GE105" s="1"/>
+      <c r="GF105" s="1"/>
+      <c r="GG105" s="1"/>
+      <c r="GH105" s="1"/>
+      <c r="GI105" s="1"/>
+      <c r="GJ105" s="1"/>
+      <c r="GK105" s="1"/>
+      <c r="GL105" s="1"/>
+      <c r="GM105" s="1"/>
+      <c r="GN105" s="1"/>
+      <c r="GO105" s="1"/>
+      <c r="GP105" s="1"/>
+      <c r="GQ105" s="1"/>
+      <c r="GR105" s="1"/>
+      <c r="GS105" s="1"/>
+      <c r="GT105" s="1"/>
+      <c r="GU105" s="1"/>
+      <c r="GV105" s="1"/>
+      <c r="GW105" s="1"/>
+      <c r="GX105" s="1"/>
+      <c r="GY105" s="1"/>
+      <c r="GZ105" s="1"/>
+      <c r="HA105" s="1"/>
+      <c r="HB105" s="1"/>
+      <c r="HC105" s="1"/>
+      <c r="HD105" s="1"/>
+      <c r="HE105" s="1"/>
+      <c r="HF105" s="1"/>
+      <c r="HG105" s="1"/>
+      <c r="HH105" s="1"/>
+      <c r="HI105" s="1"/>
+      <c r="HJ105" s="1"/>
+      <c r="HK105" s="1"/>
+      <c r="HL105" s="1"/>
+      <c r="HM105" s="1"/>
+      <c r="HN105" s="1"/>
+      <c r="HO105" s="1"/>
+      <c r="HP105" s="1"/>
+      <c r="HQ105" s="1"/>
+      <c r="HR105" s="1"/>
+      <c r="HS105" s="1"/>
+      <c r="HT105" s="1"/>
+      <c r="HU105" s="1"/>
+      <c r="HV105" s="1"/>
+      <c r="HW105" s="1"/>
+      <c r="HX105" s="1"/>
+      <c r="HY105" s="1"/>
+      <c r="HZ105" s="1"/>
+      <c r="IA105" s="1"/>
+      <c r="IB105" s="1"/>
+      <c r="IC105" s="1"/>
+      <c r="ID105" s="1"/>
+      <c r="IE105" s="1"/>
+      <c r="IF105" s="1"/>
+      <c r="IG105" s="1"/>
+      <c r="IH105" s="1"/>
+      <c r="II105" s="1"/>
+      <c r="IJ105" s="1"/>
+      <c r="IK105" s="1"/>
+      <c r="IL105" s="1"/>
+      <c r="IM105" s="1"/>
+      <c r="IN105" s="1"/>
+      <c r="IO105" s="1"/>
+      <c r="IP105" s="1"/>
+      <c r="IQ105" s="1"/>
+      <c r="IR105" s="1"/>
+      <c r="IS105" s="1"/>
+      <c r="IT105" s="1"/>
+      <c r="IU105" s="1"/>
+      <c r="IV105" s="1"/>
     </row>
     <row r="106" ht="22.35">
       <c r="H106" s="1">
@@ -33582,252 +33582,252 @@
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
       <c r="J135" s="1"/>
-      <c r="K135"/>
-      <c r="L135"/>
-      <c r="M135"/>
-      <c r="N135"/>
-      <c r="O135"/>
-      <c r="P135"/>
-      <c r="Q135"/>
-      <c r="R135"/>
-      <c r="S135"/>
-      <c r="T135"/>
-      <c r="U135"/>
-      <c r="V135"/>
-      <c r="W135"/>
-      <c r="X135"/>
-      <c r="Y135"/>
-      <c r="Z135"/>
-      <c r="AA135"/>
-      <c r="AB135"/>
-      <c r="AC135"/>
-      <c r="AD135"/>
-      <c r="AE135"/>
-      <c r="AF135"/>
-      <c r="AG135"/>
-      <c r="AH135"/>
-      <c r="AI135"/>
-      <c r="AJ135"/>
-      <c r="AK135"/>
-      <c r="AL135"/>
-      <c r="AM135"/>
-      <c r="AN135"/>
-      <c r="AO135"/>
-      <c r="AP135"/>
-      <c r="AQ135"/>
-      <c r="AR135"/>
-      <c r="AS135"/>
-      <c r="AT135"/>
-      <c r="AU135"/>
-      <c r="AV135"/>
-      <c r="AW135"/>
-      <c r="AX135"/>
-      <c r="AY135"/>
-      <c r="AZ135"/>
-      <c r="BA135"/>
-      <c r="BB135"/>
-      <c r="BC135"/>
-      <c r="BD135"/>
-      <c r="BE135"/>
-      <c r="BF135"/>
-      <c r="BG135"/>
-      <c r="BH135"/>
-      <c r="BI135"/>
-      <c r="BJ135"/>
-      <c r="BK135"/>
-      <c r="BL135"/>
-      <c r="BM135"/>
-      <c r="BN135"/>
-      <c r="BO135"/>
-      <c r="BP135"/>
-      <c r="BQ135"/>
-      <c r="BR135"/>
-      <c r="BS135"/>
-      <c r="BT135"/>
-      <c r="BU135"/>
-      <c r="BV135"/>
-      <c r="BW135"/>
-      <c r="BX135"/>
-      <c r="BY135"/>
-      <c r="BZ135"/>
-      <c r="CA135"/>
-      <c r="CB135"/>
-      <c r="CC135"/>
-      <c r="CD135"/>
-      <c r="CE135"/>
-      <c r="CF135"/>
-      <c r="CG135"/>
-      <c r="CH135"/>
-      <c r="CI135"/>
-      <c r="CJ135"/>
-      <c r="CK135"/>
-      <c r="CL135"/>
-      <c r="CM135"/>
-      <c r="CN135"/>
-      <c r="CO135"/>
-      <c r="CP135"/>
-      <c r="CQ135"/>
-      <c r="CR135"/>
-      <c r="CS135"/>
-      <c r="CT135"/>
-      <c r="CU135"/>
-      <c r="CV135"/>
-      <c r="CW135"/>
-      <c r="CX135"/>
-      <c r="CY135"/>
-      <c r="CZ135"/>
-      <c r="DA135"/>
-      <c r="DB135"/>
-      <c r="DC135"/>
-      <c r="DD135"/>
-      <c r="DE135"/>
-      <c r="DF135"/>
-      <c r="DG135"/>
-      <c r="DH135"/>
-      <c r="DI135"/>
-      <c r="DJ135"/>
-      <c r="DK135"/>
-      <c r="DL135"/>
-      <c r="DM135"/>
-      <c r="DN135"/>
-      <c r="DO135"/>
-      <c r="DP135"/>
-      <c r="DQ135"/>
-      <c r="DR135"/>
-      <c r="DS135"/>
-      <c r="DT135"/>
-      <c r="DU135"/>
-      <c r="DV135"/>
-      <c r="DW135"/>
-      <c r="DX135"/>
-      <c r="DY135"/>
-      <c r="DZ135"/>
-      <c r="EA135"/>
-      <c r="EB135"/>
-      <c r="EC135"/>
-      <c r="ED135"/>
-      <c r="EE135"/>
-      <c r="EF135"/>
-      <c r="EG135"/>
-      <c r="EH135"/>
-      <c r="EI135"/>
-      <c r="EJ135"/>
-      <c r="EK135"/>
-      <c r="EL135"/>
-      <c r="EM135"/>
-      <c r="EN135"/>
-      <c r="EO135"/>
-      <c r="EP135"/>
-      <c r="EQ135"/>
-      <c r="ER135"/>
-      <c r="ES135"/>
-      <c r="ET135"/>
-      <c r="EU135"/>
-      <c r="EV135"/>
-      <c r="EW135"/>
-      <c r="EX135"/>
-      <c r="EY135"/>
-      <c r="EZ135"/>
-      <c r="FA135"/>
-      <c r="FB135"/>
-      <c r="FC135"/>
-      <c r="FD135"/>
-      <c r="FE135"/>
-      <c r="FF135"/>
-      <c r="FG135"/>
-      <c r="FH135"/>
-      <c r="FI135"/>
-      <c r="FJ135"/>
-      <c r="FK135"/>
-      <c r="FL135"/>
-      <c r="FM135"/>
-      <c r="FN135"/>
-      <c r="FO135"/>
-      <c r="FP135"/>
-      <c r="FQ135"/>
-      <c r="FR135"/>
-      <c r="FS135"/>
-      <c r="FT135"/>
-      <c r="FU135"/>
-      <c r="FV135"/>
-      <c r="FW135"/>
-      <c r="FX135"/>
-      <c r="FY135"/>
-      <c r="FZ135"/>
-      <c r="GA135"/>
-      <c r="GB135"/>
-      <c r="GC135"/>
-      <c r="GD135"/>
-      <c r="GE135"/>
-      <c r="GF135"/>
-      <c r="GG135"/>
-      <c r="GH135"/>
-      <c r="GI135"/>
-      <c r="GJ135"/>
-      <c r="GK135"/>
-      <c r="GL135"/>
-      <c r="GM135"/>
-      <c r="GN135"/>
-      <c r="GO135"/>
-      <c r="GP135"/>
-      <c r="GQ135"/>
-      <c r="GR135"/>
-      <c r="GS135"/>
-      <c r="GT135"/>
-      <c r="GU135"/>
-      <c r="GV135"/>
-      <c r="GW135"/>
-      <c r="GX135"/>
-      <c r="GY135"/>
-      <c r="GZ135"/>
-      <c r="HA135"/>
-      <c r="HB135"/>
-      <c r="HC135"/>
-      <c r="HD135"/>
-      <c r="HE135"/>
-      <c r="HF135"/>
-      <c r="HG135"/>
-      <c r="HH135"/>
-      <c r="HI135"/>
-      <c r="HJ135"/>
-      <c r="HK135"/>
-      <c r="HL135"/>
-      <c r="HM135"/>
-      <c r="HN135"/>
-      <c r="HO135"/>
-      <c r="HP135"/>
-      <c r="HQ135"/>
-      <c r="HR135"/>
-      <c r="HS135"/>
-      <c r="HT135"/>
-      <c r="HU135"/>
-      <c r="HV135"/>
-      <c r="HW135"/>
-      <c r="HX135"/>
-      <c r="HY135"/>
-      <c r="HZ135"/>
-      <c r="IA135"/>
-      <c r="IB135"/>
-      <c r="IC135"/>
-      <c r="ID135"/>
-      <c r="IE135"/>
-      <c r="IF135"/>
-      <c r="IG135"/>
-      <c r="IH135"/>
-      <c r="II135"/>
-      <c r="IJ135"/>
-      <c r="IK135"/>
-      <c r="IL135"/>
-      <c r="IM135"/>
-      <c r="IN135"/>
-      <c r="IO135"/>
-      <c r="IP135"/>
-      <c r="IQ135"/>
-      <c r="IR135"/>
-      <c r="IS135"/>
-      <c r="IT135"/>
-      <c r="IU135"/>
-      <c r="IV135"/>
+      <c r="K135" s="1"/>
+      <c r="L135" s="1"/>
+      <c r="M135" s="1"/>
+      <c r="N135" s="1"/>
+      <c r="O135" s="1"/>
+      <c r="P135" s="1"/>
+      <c r="Q135" s="1"/>
+      <c r="R135" s="1"/>
+      <c r="S135" s="1"/>
+      <c r="T135" s="1"/>
+      <c r="U135" s="1"/>
+      <c r="V135" s="1"/>
+      <c r="W135" s="1"/>
+      <c r="X135" s="1"/>
+      <c r="Y135" s="1"/>
+      <c r="Z135" s="1"/>
+      <c r="AA135" s="1"/>
+      <c r="AB135" s="1"/>
+      <c r="AC135" s="1"/>
+      <c r="AD135" s="1"/>
+      <c r="AE135" s="1"/>
+      <c r="AF135" s="1"/>
+      <c r="AG135" s="1"/>
+      <c r="AH135" s="1"/>
+      <c r="AI135" s="1"/>
+      <c r="AJ135" s="1"/>
+      <c r="AK135" s="1"/>
+      <c r="AL135" s="1"/>
+      <c r="AM135" s="1"/>
+      <c r="AN135" s="1"/>
+      <c r="AO135" s="1"/>
+      <c r="AP135" s="1"/>
+      <c r="AQ135" s="1"/>
+      <c r="AR135" s="1"/>
+      <c r="AS135" s="1"/>
+      <c r="AT135" s="1"/>
+      <c r="AU135" s="1"/>
+      <c r="AV135" s="1"/>
+      <c r="AW135" s="1"/>
+      <c r="AX135" s="1"/>
+      <c r="AY135" s="1"/>
+      <c r="AZ135" s="1"/>
+      <c r="BA135" s="1"/>
+      <c r="BB135" s="1"/>
+      <c r="BC135" s="1"/>
+      <c r="BD135" s="1"/>
+      <c r="BE135" s="1"/>
+      <c r="BF135" s="1"/>
+      <c r="BG135" s="1"/>
+      <c r="BH135" s="1"/>
+      <c r="BI135" s="1"/>
+      <c r="BJ135" s="1"/>
+      <c r="BK135" s="1"/>
+      <c r="BL135" s="1"/>
+      <c r="BM135" s="1"/>
+      <c r="BN135" s="1"/>
+      <c r="BO135" s="1"/>
+      <c r="BP135" s="1"/>
+      <c r="BQ135" s="1"/>
+      <c r="BR135" s="1"/>
+      <c r="BS135" s="1"/>
+      <c r="BT135" s="1"/>
+      <c r="BU135" s="1"/>
+      <c r="BV135" s="1"/>
+      <c r="BW135" s="1"/>
+      <c r="BX135" s="1"/>
+      <c r="BY135" s="1"/>
+      <c r="BZ135" s="1"/>
+      <c r="CA135" s="1"/>
+      <c r="CB135" s="1"/>
+      <c r="CC135" s="1"/>
+      <c r="CD135" s="1"/>
+      <c r="CE135" s="1"/>
+      <c r="CF135" s="1"/>
+      <c r="CG135" s="1"/>
+      <c r="CH135" s="1"/>
+      <c r="CI135" s="1"/>
+      <c r="CJ135" s="1"/>
+      <c r="CK135" s="1"/>
+      <c r="CL135" s="1"/>
+      <c r="CM135" s="1"/>
+      <c r="CN135" s="1"/>
+      <c r="CO135" s="1"/>
+      <c r="CP135" s="1"/>
+      <c r="CQ135" s="1"/>
+      <c r="CR135" s="1"/>
+      <c r="CS135" s="1"/>
+      <c r="CT135" s="1"/>
+      <c r="CU135" s="1"/>
+      <c r="CV135" s="1"/>
+      <c r="CW135" s="1"/>
+      <c r="CX135" s="1"/>
+      <c r="CY135" s="1"/>
+      <c r="CZ135" s="1"/>
+      <c r="DA135" s="1"/>
+      <c r="DB135" s="1"/>
+      <c r="DC135" s="1"/>
+      <c r="DD135" s="1"/>
+      <c r="DE135" s="1"/>
+      <c r="DF135" s="1"/>
+      <c r="DG135" s="1"/>
+      <c r="DH135" s="1"/>
+      <c r="DI135" s="1"/>
+      <c r="DJ135" s="1"/>
+      <c r="DK135" s="1"/>
+      <c r="DL135" s="1"/>
+      <c r="DM135" s="1"/>
+      <c r="DN135" s="1"/>
+      <c r="DO135" s="1"/>
+      <c r="DP135" s="1"/>
+      <c r="DQ135" s="1"/>
+      <c r="DR135" s="1"/>
+      <c r="DS135" s="1"/>
+      <c r="DT135" s="1"/>
+      <c r="DU135" s="1"/>
+      <c r="DV135" s="1"/>
+      <c r="DW135" s="1"/>
+      <c r="DX135" s="1"/>
+      <c r="DY135" s="1"/>
+      <c r="DZ135" s="1"/>
+      <c r="EA135" s="1"/>
+      <c r="EB135" s="1"/>
+      <c r="EC135" s="1"/>
+      <c r="ED135" s="1"/>
+      <c r="EE135" s="1"/>
+      <c r="EF135" s="1"/>
+      <c r="EG135" s="1"/>
+      <c r="EH135" s="1"/>
+      <c r="EI135" s="1"/>
+      <c r="EJ135" s="1"/>
+      <c r="EK135" s="1"/>
+      <c r="EL135" s="1"/>
+      <c r="EM135" s="1"/>
+      <c r="EN135" s="1"/>
+      <c r="EO135" s="1"/>
+      <c r="EP135" s="1"/>
+      <c r="EQ135" s="1"/>
+      <c r="ER135" s="1"/>
+      <c r="ES135" s="1"/>
+      <c r="ET135" s="1"/>
+      <c r="EU135" s="1"/>
+      <c r="EV135" s="1"/>
+      <c r="EW135" s="1"/>
+      <c r="EX135" s="1"/>
+      <c r="EY135" s="1"/>
+      <c r="EZ135" s="1"/>
+      <c r="FA135" s="1"/>
+      <c r="FB135" s="1"/>
+      <c r="FC135" s="1"/>
+      <c r="FD135" s="1"/>
+      <c r="FE135" s="1"/>
+      <c r="FF135" s="1"/>
+      <c r="FG135" s="1"/>
+      <c r="FH135" s="1"/>
+      <c r="FI135" s="1"/>
+      <c r="FJ135" s="1"/>
+      <c r="FK135" s="1"/>
+      <c r="FL135" s="1"/>
+      <c r="FM135" s="1"/>
+      <c r="FN135" s="1"/>
+      <c r="FO135" s="1"/>
+      <c r="FP135" s="1"/>
+      <c r="FQ135" s="1"/>
+      <c r="FR135" s="1"/>
+      <c r="FS135" s="1"/>
+      <c r="FT135" s="1"/>
+      <c r="FU135" s="1"/>
+      <c r="FV135" s="1"/>
+      <c r="FW135" s="1"/>
+      <c r="FX135" s="1"/>
+      <c r="FY135" s="1"/>
+      <c r="FZ135" s="1"/>
+      <c r="GA135" s="1"/>
+      <c r="GB135" s="1"/>
+      <c r="GC135" s="1"/>
+      <c r="GD135" s="1"/>
+      <c r="GE135" s="1"/>
+      <c r="GF135" s="1"/>
+      <c r="GG135" s="1"/>
+      <c r="GH135" s="1"/>
+      <c r="GI135" s="1"/>
+      <c r="GJ135" s="1"/>
+      <c r="GK135" s="1"/>
+      <c r="GL135" s="1"/>
+      <c r="GM135" s="1"/>
+      <c r="GN135" s="1"/>
+      <c r="GO135" s="1"/>
+      <c r="GP135" s="1"/>
+      <c r="GQ135" s="1"/>
+      <c r="GR135" s="1"/>
+      <c r="GS135" s="1"/>
+      <c r="GT135" s="1"/>
+      <c r="GU135" s="1"/>
+      <c r="GV135" s="1"/>
+      <c r="GW135" s="1"/>
+      <c r="GX135" s="1"/>
+      <c r="GY135" s="1"/>
+      <c r="GZ135" s="1"/>
+      <c r="HA135" s="1"/>
+      <c r="HB135" s="1"/>
+      <c r="HC135" s="1"/>
+      <c r="HD135" s="1"/>
+      <c r="HE135" s="1"/>
+      <c r="HF135" s="1"/>
+      <c r="HG135" s="1"/>
+      <c r="HH135" s="1"/>
+      <c r="HI135" s="1"/>
+      <c r="HJ135" s="1"/>
+      <c r="HK135" s="1"/>
+      <c r="HL135" s="1"/>
+      <c r="HM135" s="1"/>
+      <c r="HN135" s="1"/>
+      <c r="HO135" s="1"/>
+      <c r="HP135" s="1"/>
+      <c r="HQ135" s="1"/>
+      <c r="HR135" s="1"/>
+      <c r="HS135" s="1"/>
+      <c r="HT135" s="1"/>
+      <c r="HU135" s="1"/>
+      <c r="HV135" s="1"/>
+      <c r="HW135" s="1"/>
+      <c r="HX135" s="1"/>
+      <c r="HY135" s="1"/>
+      <c r="HZ135" s="1"/>
+      <c r="IA135" s="1"/>
+      <c r="IB135" s="1"/>
+      <c r="IC135" s="1"/>
+      <c r="ID135" s="1"/>
+      <c r="IE135" s="1"/>
+      <c r="IF135" s="1"/>
+      <c r="IG135" s="1"/>
+      <c r="IH135" s="1"/>
+      <c r="II135" s="1"/>
+      <c r="IJ135" s="1"/>
+      <c r="IK135" s="1"/>
+      <c r="IL135" s="1"/>
+      <c r="IM135" s="1"/>
+      <c r="IN135" s="1"/>
+      <c r="IO135" s="1"/>
+      <c r="IP135" s="1"/>
+      <c r="IQ135" s="1"/>
+      <c r="IR135" s="1"/>
+      <c r="IS135" s="1"/>
+      <c r="IT135" s="1"/>
+      <c r="IU135" s="1"/>
+      <c r="IV135" s="1"/>
     </row>
     <row r="136" ht="12.8">
       <c r="K136" s="1"/>
@@ -34877,252 +34877,252 @@
       <c r="H150" s="1"/>
       <c r="I150" s="1"/>
       <c r="J150" s="1"/>
-      <c r="K150"/>
-      <c r="L150"/>
-      <c r="M150"/>
-      <c r="N150"/>
-      <c r="O150"/>
-      <c r="P150"/>
-      <c r="Q150"/>
-      <c r="R150"/>
-      <c r="S150"/>
-      <c r="T150"/>
-      <c r="U150"/>
-      <c r="V150"/>
-      <c r="W150"/>
-      <c r="X150"/>
-      <c r="Y150"/>
-      <c r="Z150"/>
-      <c r="AA150"/>
-      <c r="AB150"/>
-      <c r="AC150"/>
-      <c r="AD150"/>
-      <c r="AE150"/>
-      <c r="AF150"/>
-      <c r="AG150"/>
-      <c r="AH150"/>
-      <c r="AI150"/>
-      <c r="AJ150"/>
-      <c r="AK150"/>
-      <c r="AL150"/>
-      <c r="AM150"/>
-      <c r="AN150"/>
-      <c r="AO150"/>
-      <c r="AP150"/>
-      <c r="AQ150"/>
-      <c r="AR150"/>
-      <c r="AS150"/>
-      <c r="AT150"/>
-      <c r="AU150"/>
-      <c r="AV150"/>
-      <c r="AW150"/>
-      <c r="AX150"/>
-      <c r="AY150"/>
-      <c r="AZ150"/>
-      <c r="BA150"/>
-      <c r="BB150"/>
-      <c r="BC150"/>
-      <c r="BD150"/>
-      <c r="BE150"/>
-      <c r="BF150"/>
-      <c r="BG150"/>
-      <c r="BH150"/>
-      <c r="BI150"/>
-      <c r="BJ150"/>
-      <c r="BK150"/>
-      <c r="BL150"/>
-      <c r="BM150"/>
-      <c r="BN150"/>
-      <c r="BO150"/>
-      <c r="BP150"/>
-      <c r="BQ150"/>
-      <c r="BR150"/>
-      <c r="BS150"/>
-      <c r="BT150"/>
-      <c r="BU150"/>
-      <c r="BV150"/>
-      <c r="BW150"/>
-      <c r="BX150"/>
-      <c r="BY150"/>
-      <c r="BZ150"/>
-      <c r="CA150"/>
-      <c r="CB150"/>
-      <c r="CC150"/>
-      <c r="CD150"/>
-      <c r="CE150"/>
-      <c r="CF150"/>
-      <c r="CG150"/>
-      <c r="CH150"/>
-      <c r="CI150"/>
-      <c r="CJ150"/>
-      <c r="CK150"/>
-      <c r="CL150"/>
-      <c r="CM150"/>
-      <c r="CN150"/>
-      <c r="CO150"/>
-      <c r="CP150"/>
-      <c r="CQ150"/>
-      <c r="CR150"/>
-      <c r="CS150"/>
-      <c r="CT150"/>
-      <c r="CU150"/>
-      <c r="CV150"/>
-      <c r="CW150"/>
-      <c r="CX150"/>
-      <c r="CY150"/>
-      <c r="CZ150"/>
-      <c r="DA150"/>
-      <c r="DB150"/>
-      <c r="DC150"/>
-      <c r="DD150"/>
-      <c r="DE150"/>
-      <c r="DF150"/>
-      <c r="DG150"/>
-      <c r="DH150"/>
-      <c r="DI150"/>
-      <c r="DJ150"/>
-      <c r="DK150"/>
-      <c r="DL150"/>
-      <c r="DM150"/>
-      <c r="DN150"/>
-      <c r="DO150"/>
-      <c r="DP150"/>
-      <c r="DQ150"/>
-      <c r="DR150"/>
-      <c r="DS150"/>
-      <c r="DT150"/>
-      <c r="DU150"/>
-      <c r="DV150"/>
-      <c r="DW150"/>
-      <c r="DX150"/>
-      <c r="DY150"/>
-      <c r="DZ150"/>
-      <c r="EA150"/>
-      <c r="EB150"/>
-      <c r="EC150"/>
-      <c r="ED150"/>
-      <c r="EE150"/>
-      <c r="EF150"/>
-      <c r="EG150"/>
-      <c r="EH150"/>
-      <c r="EI150"/>
-      <c r="EJ150"/>
-      <c r="EK150"/>
-      <c r="EL150"/>
-      <c r="EM150"/>
-      <c r="EN150"/>
-      <c r="EO150"/>
-      <c r="EP150"/>
-      <c r="EQ150"/>
-      <c r="ER150"/>
-      <c r="ES150"/>
-      <c r="ET150"/>
-      <c r="EU150"/>
-      <c r="EV150"/>
-      <c r="EW150"/>
-      <c r="EX150"/>
-      <c r="EY150"/>
-      <c r="EZ150"/>
-      <c r="FA150"/>
-      <c r="FB150"/>
-      <c r="FC150"/>
-      <c r="FD150"/>
-      <c r="FE150"/>
-      <c r="FF150"/>
-      <c r="FG150"/>
-      <c r="FH150"/>
-      <c r="FI150"/>
-      <c r="FJ150"/>
-      <c r="FK150"/>
-      <c r="FL150"/>
-      <c r="FM150"/>
-      <c r="FN150"/>
-      <c r="FO150"/>
-      <c r="FP150"/>
-      <c r="FQ150"/>
-      <c r="FR150"/>
-      <c r="FS150"/>
-      <c r="FT150"/>
-      <c r="FU150"/>
-      <c r="FV150"/>
-      <c r="FW150"/>
-      <c r="FX150"/>
-      <c r="FY150"/>
-      <c r="FZ150"/>
-      <c r="GA150"/>
-      <c r="GB150"/>
-      <c r="GC150"/>
-      <c r="GD150"/>
-      <c r="GE150"/>
-      <c r="GF150"/>
-      <c r="GG150"/>
-      <c r="GH150"/>
-      <c r="GI150"/>
-      <c r="GJ150"/>
-      <c r="GK150"/>
-      <c r="GL150"/>
-      <c r="GM150"/>
-      <c r="GN150"/>
-      <c r="GO150"/>
-      <c r="GP150"/>
-      <c r="GQ150"/>
-      <c r="GR150"/>
-      <c r="GS150"/>
-      <c r="GT150"/>
-      <c r="GU150"/>
-      <c r="GV150"/>
-      <c r="GW150"/>
-      <c r="GX150"/>
-      <c r="GY150"/>
-      <c r="GZ150"/>
-      <c r="HA150"/>
-      <c r="HB150"/>
-      <c r="HC150"/>
-      <c r="HD150"/>
-      <c r="HE150"/>
-      <c r="HF150"/>
-      <c r="HG150"/>
-      <c r="HH150"/>
-      <c r="HI150"/>
-      <c r="HJ150"/>
-      <c r="HK150"/>
-      <c r="HL150"/>
-      <c r="HM150"/>
-      <c r="HN150"/>
-      <c r="HO150"/>
-      <c r="HP150"/>
-      <c r="HQ150"/>
-      <c r="HR150"/>
-      <c r="HS150"/>
-      <c r="HT150"/>
-      <c r="HU150"/>
-      <c r="HV150"/>
-      <c r="HW150"/>
-      <c r="HX150"/>
-      <c r="HY150"/>
-      <c r="HZ150"/>
-      <c r="IA150"/>
-      <c r="IB150"/>
-      <c r="IC150"/>
-      <c r="ID150"/>
-      <c r="IE150"/>
-      <c r="IF150"/>
-      <c r="IG150"/>
-      <c r="IH150"/>
-      <c r="II150"/>
-      <c r="IJ150"/>
-      <c r="IK150"/>
-      <c r="IL150"/>
-      <c r="IM150"/>
-      <c r="IN150"/>
-      <c r="IO150"/>
-      <c r="IP150"/>
-      <c r="IQ150"/>
-      <c r="IR150"/>
-      <c r="IS150"/>
-      <c r="IT150"/>
-      <c r="IU150"/>
-      <c r="IV150"/>
+      <c r="K150" s="1"/>
+      <c r="L150" s="1"/>
+      <c r="M150" s="1"/>
+      <c r="N150" s="1"/>
+      <c r="O150" s="1"/>
+      <c r="P150" s="1"/>
+      <c r="Q150" s="1"/>
+      <c r="R150" s="1"/>
+      <c r="S150" s="1"/>
+      <c r="T150" s="1"/>
+      <c r="U150" s="1"/>
+      <c r="V150" s="1"/>
+      <c r="W150" s="1"/>
+      <c r="X150" s="1"/>
+      <c r="Y150" s="1"/>
+      <c r="Z150" s="1"/>
+      <c r="AA150" s="1"/>
+      <c r="AB150" s="1"/>
+      <c r="AC150" s="1"/>
+      <c r="AD150" s="1"/>
+      <c r="AE150" s="1"/>
+      <c r="AF150" s="1"/>
+      <c r="AG150" s="1"/>
+      <c r="AH150" s="1"/>
+      <c r="AI150" s="1"/>
+      <c r="AJ150" s="1"/>
+      <c r="AK150" s="1"/>
+      <c r="AL150" s="1"/>
+      <c r="AM150" s="1"/>
+      <c r="AN150" s="1"/>
+      <c r="AO150" s="1"/>
+      <c r="AP150" s="1"/>
+      <c r="AQ150" s="1"/>
+      <c r="AR150" s="1"/>
+      <c r="AS150" s="1"/>
+      <c r="AT150" s="1"/>
+      <c r="AU150" s="1"/>
+      <c r="AV150" s="1"/>
+      <c r="AW150" s="1"/>
+      <c r="AX150" s="1"/>
+      <c r="AY150" s="1"/>
+      <c r="AZ150" s="1"/>
+      <c r="BA150" s="1"/>
+      <c r="BB150" s="1"/>
+      <c r="BC150" s="1"/>
+      <c r="BD150" s="1"/>
+      <c r="BE150" s="1"/>
+      <c r="BF150" s="1"/>
+      <c r="BG150" s="1"/>
+      <c r="BH150" s="1"/>
+      <c r="BI150" s="1"/>
+      <c r="BJ150" s="1"/>
+      <c r="BK150" s="1"/>
+      <c r="BL150" s="1"/>
+      <c r="BM150" s="1"/>
+      <c r="BN150" s="1"/>
+      <c r="BO150" s="1"/>
+      <c r="BP150" s="1"/>
+      <c r="BQ150" s="1"/>
+      <c r="BR150" s="1"/>
+      <c r="BS150" s="1"/>
+      <c r="BT150" s="1"/>
+      <c r="BU150" s="1"/>
+      <c r="BV150" s="1"/>
+      <c r="BW150" s="1"/>
+      <c r="BX150" s="1"/>
+      <c r="BY150" s="1"/>
+      <c r="BZ150" s="1"/>
+      <c r="CA150" s="1"/>
+      <c r="CB150" s="1"/>
+      <c r="CC150" s="1"/>
+      <c r="CD150" s="1"/>
+      <c r="CE150" s="1"/>
+      <c r="CF150" s="1"/>
+      <c r="CG150" s="1"/>
+      <c r="CH150" s="1"/>
+      <c r="CI150" s="1"/>
+      <c r="CJ150" s="1"/>
+      <c r="CK150" s="1"/>
+      <c r="CL150" s="1"/>
+      <c r="CM150" s="1"/>
+      <c r="CN150" s="1"/>
+      <c r="CO150" s="1"/>
+      <c r="CP150" s="1"/>
+      <c r="CQ150" s="1"/>
+      <c r="CR150" s="1"/>
+      <c r="CS150" s="1"/>
+      <c r="CT150" s="1"/>
+      <c r="CU150" s="1"/>
+      <c r="CV150" s="1"/>
+      <c r="CW150" s="1"/>
+      <c r="CX150" s="1"/>
+      <c r="CY150" s="1"/>
+      <c r="CZ150" s="1"/>
+      <c r="DA150" s="1"/>
+      <c r="DB150" s="1"/>
+      <c r="DC150" s="1"/>
+      <c r="DD150" s="1"/>
+      <c r="DE150" s="1"/>
+      <c r="DF150" s="1"/>
+      <c r="DG150" s="1"/>
+      <c r="DH150" s="1"/>
+      <c r="DI150" s="1"/>
+      <c r="DJ150" s="1"/>
+      <c r="DK150" s="1"/>
+      <c r="DL150" s="1"/>
+      <c r="DM150" s="1"/>
+      <c r="DN150" s="1"/>
+      <c r="DO150" s="1"/>
+      <c r="DP150" s="1"/>
+      <c r="DQ150" s="1"/>
+      <c r="DR150" s="1"/>
+      <c r="DS150" s="1"/>
+      <c r="DT150" s="1"/>
+      <c r="DU150" s="1"/>
+      <c r="DV150" s="1"/>
+      <c r="DW150" s="1"/>
+      <c r="DX150" s="1"/>
+      <c r="DY150" s="1"/>
+      <c r="DZ150" s="1"/>
+      <c r="EA150" s="1"/>
+      <c r="EB150" s="1"/>
+      <c r="EC150" s="1"/>
+      <c r="ED150" s="1"/>
+      <c r="EE150" s="1"/>
+      <c r="EF150" s="1"/>
+      <c r="EG150" s="1"/>
+      <c r="EH150" s="1"/>
+      <c r="EI150" s="1"/>
+      <c r="EJ150" s="1"/>
+      <c r="EK150" s="1"/>
+      <c r="EL150" s="1"/>
+      <c r="EM150" s="1"/>
+      <c r="EN150" s="1"/>
+      <c r="EO150" s="1"/>
+      <c r="EP150" s="1"/>
+      <c r="EQ150" s="1"/>
+      <c r="ER150" s="1"/>
+      <c r="ES150" s="1"/>
+      <c r="ET150" s="1"/>
+      <c r="EU150" s="1"/>
+      <c r="EV150" s="1"/>
+      <c r="EW150" s="1"/>
+      <c r="EX150" s="1"/>
+      <c r="EY150" s="1"/>
+      <c r="EZ150" s="1"/>
+      <c r="FA150" s="1"/>
+      <c r="FB150" s="1"/>
+      <c r="FC150" s="1"/>
+      <c r="FD150" s="1"/>
+      <c r="FE150" s="1"/>
+      <c r="FF150" s="1"/>
+      <c r="FG150" s="1"/>
+      <c r="FH150" s="1"/>
+      <c r="FI150" s="1"/>
+      <c r="FJ150" s="1"/>
+      <c r="FK150" s="1"/>
+      <c r="FL150" s="1"/>
+      <c r="FM150" s="1"/>
+      <c r="FN150" s="1"/>
+      <c r="FO150" s="1"/>
+      <c r="FP150" s="1"/>
+      <c r="FQ150" s="1"/>
+      <c r="FR150" s="1"/>
+      <c r="FS150" s="1"/>
+      <c r="FT150" s="1"/>
+      <c r="FU150" s="1"/>
+      <c r="FV150" s="1"/>
+      <c r="FW150" s="1"/>
+      <c r="FX150" s="1"/>
+      <c r="FY150" s="1"/>
+      <c r="FZ150" s="1"/>
+      <c r="GA150" s="1"/>
+      <c r="GB150" s="1"/>
+      <c r="GC150" s="1"/>
+      <c r="GD150" s="1"/>
+      <c r="GE150" s="1"/>
+      <c r="GF150" s="1"/>
+      <c r="GG150" s="1"/>
+      <c r="GH150" s="1"/>
+      <c r="GI150" s="1"/>
+      <c r="GJ150" s="1"/>
+      <c r="GK150" s="1"/>
+      <c r="GL150" s="1"/>
+      <c r="GM150" s="1"/>
+      <c r="GN150" s="1"/>
+      <c r="GO150" s="1"/>
+      <c r="GP150" s="1"/>
+      <c r="GQ150" s="1"/>
+      <c r="GR150" s="1"/>
+      <c r="GS150" s="1"/>
+      <c r="GT150" s="1"/>
+      <c r="GU150" s="1"/>
+      <c r="GV150" s="1"/>
+      <c r="GW150" s="1"/>
+      <c r="GX150" s="1"/>
+      <c r="GY150" s="1"/>
+      <c r="GZ150" s="1"/>
+      <c r="HA150" s="1"/>
+      <c r="HB150" s="1"/>
+      <c r="HC150" s="1"/>
+      <c r="HD150" s="1"/>
+      <c r="HE150" s="1"/>
+      <c r="HF150" s="1"/>
+      <c r="HG150" s="1"/>
+      <c r="HH150" s="1"/>
+      <c r="HI150" s="1"/>
+      <c r="HJ150" s="1"/>
+      <c r="HK150" s="1"/>
+      <c r="HL150" s="1"/>
+      <c r="HM150" s="1"/>
+      <c r="HN150" s="1"/>
+      <c r="HO150" s="1"/>
+      <c r="HP150" s="1"/>
+      <c r="HQ150" s="1"/>
+      <c r="HR150" s="1"/>
+      <c r="HS150" s="1"/>
+      <c r="HT150" s="1"/>
+      <c r="HU150" s="1"/>
+      <c r="HV150" s="1"/>
+      <c r="HW150" s="1"/>
+      <c r="HX150" s="1"/>
+      <c r="HY150" s="1"/>
+      <c r="HZ150" s="1"/>
+      <c r="IA150" s="1"/>
+      <c r="IB150" s="1"/>
+      <c r="IC150" s="1"/>
+      <c r="ID150" s="1"/>
+      <c r="IE150" s="1"/>
+      <c r="IF150" s="1"/>
+      <c r="IG150" s="1"/>
+      <c r="IH150" s="1"/>
+      <c r="II150" s="1"/>
+      <c r="IJ150" s="1"/>
+      <c r="IK150" s="1"/>
+      <c r="IL150" s="1"/>
+      <c r="IM150" s="1"/>
+      <c r="IN150" s="1"/>
+      <c r="IO150" s="1"/>
+      <c r="IP150" s="1"/>
+      <c r="IQ150" s="1"/>
+      <c r="IR150" s="1"/>
+      <c r="IS150" s="1"/>
+      <c r="IT150" s="1"/>
+      <c r="IU150" s="1"/>
+      <c r="IV150" s="1"/>
     </row>
     <row r="151" ht="12.8">
       <c r="K151" s="1"/>
@@ -35631,252 +35631,252 @@
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
       <c r="J157" s="1"/>
-      <c r="K157"/>
-      <c r="L157"/>
-      <c r="M157"/>
-      <c r="N157"/>
-      <c r="O157"/>
-      <c r="P157"/>
-      <c r="Q157"/>
-      <c r="R157"/>
-      <c r="S157"/>
-      <c r="T157"/>
-      <c r="U157"/>
-      <c r="V157"/>
-      <c r="W157"/>
-      <c r="X157"/>
-      <c r="Y157"/>
-      <c r="Z157"/>
-      <c r="AA157"/>
-      <c r="AB157"/>
-      <c r="AC157"/>
-      <c r="AD157"/>
-      <c r="AE157"/>
-      <c r="AF157"/>
-      <c r="AG157"/>
-      <c r="AH157"/>
-      <c r="AI157"/>
-      <c r="AJ157"/>
-      <c r="AK157"/>
-      <c r="AL157"/>
-      <c r="AM157"/>
-      <c r="AN157"/>
-      <c r="AO157"/>
-      <c r="AP157"/>
-      <c r="AQ157"/>
-      <c r="AR157"/>
-      <c r="AS157"/>
-      <c r="AT157"/>
-      <c r="AU157"/>
-      <c r="AV157"/>
-      <c r="AW157"/>
-      <c r="AX157"/>
-      <c r="AY157"/>
-      <c r="AZ157"/>
-      <c r="BA157"/>
-      <c r="BB157"/>
-      <c r="BC157"/>
-      <c r="BD157"/>
-      <c r="BE157"/>
-      <c r="BF157"/>
-      <c r="BG157"/>
-      <c r="BH157"/>
-      <c r="BI157"/>
-      <c r="BJ157"/>
-      <c r="BK157"/>
-      <c r="BL157"/>
-      <c r="BM157"/>
-      <c r="BN157"/>
-      <c r="BO157"/>
-      <c r="BP157"/>
-      <c r="BQ157"/>
-      <c r="BR157"/>
-      <c r="BS157"/>
-      <c r="BT157"/>
-      <c r="BU157"/>
-      <c r="BV157"/>
-      <c r="BW157"/>
-      <c r="BX157"/>
-      <c r="BY157"/>
-      <c r="BZ157"/>
-      <c r="CA157"/>
-      <c r="CB157"/>
-      <c r="CC157"/>
-      <c r="CD157"/>
-      <c r="CE157"/>
-      <c r="CF157"/>
-      <c r="CG157"/>
-      <c r="CH157"/>
-      <c r="CI157"/>
-      <c r="CJ157"/>
-      <c r="CK157"/>
-      <c r="CL157"/>
-      <c r="CM157"/>
-      <c r="CN157"/>
-      <c r="CO157"/>
-      <c r="CP157"/>
-      <c r="CQ157"/>
-      <c r="CR157"/>
-      <c r="CS157"/>
-      <c r="CT157"/>
-      <c r="CU157"/>
-      <c r="CV157"/>
-      <c r="CW157"/>
-      <c r="CX157"/>
-      <c r="CY157"/>
-      <c r="CZ157"/>
-      <c r="DA157"/>
-      <c r="DB157"/>
-      <c r="DC157"/>
-      <c r="DD157"/>
-      <c r="DE157"/>
-      <c r="DF157"/>
-      <c r="DG157"/>
-      <c r="DH157"/>
-      <c r="DI157"/>
-      <c r="DJ157"/>
-      <c r="DK157"/>
-      <c r="DL157"/>
-      <c r="DM157"/>
-      <c r="DN157"/>
-      <c r="DO157"/>
-      <c r="DP157"/>
-      <c r="DQ157"/>
-      <c r="DR157"/>
-      <c r="DS157"/>
-      <c r="DT157"/>
-      <c r="DU157"/>
-      <c r="DV157"/>
-      <c r="DW157"/>
-      <c r="DX157"/>
-      <c r="DY157"/>
-      <c r="DZ157"/>
-      <c r="EA157"/>
-      <c r="EB157"/>
-      <c r="EC157"/>
-      <c r="ED157"/>
-      <c r="EE157"/>
-      <c r="EF157"/>
-      <c r="EG157"/>
-      <c r="EH157"/>
-      <c r="EI157"/>
-      <c r="EJ157"/>
-      <c r="EK157"/>
-      <c r="EL157"/>
-      <c r="EM157"/>
-      <c r="EN157"/>
-      <c r="EO157"/>
-      <c r="EP157"/>
-      <c r="EQ157"/>
-      <c r="ER157"/>
-      <c r="ES157"/>
-      <c r="ET157"/>
-      <c r="EU157"/>
-      <c r="EV157"/>
-      <c r="EW157"/>
-      <c r="EX157"/>
-      <c r="EY157"/>
-      <c r="EZ157"/>
-      <c r="FA157"/>
-      <c r="FB157"/>
-      <c r="FC157"/>
-      <c r="FD157"/>
-      <c r="FE157"/>
-      <c r="FF157"/>
-      <c r="FG157"/>
-      <c r="FH157"/>
-      <c r="FI157"/>
-      <c r="FJ157"/>
-      <c r="FK157"/>
-      <c r="FL157"/>
-      <c r="FM157"/>
-      <c r="FN157"/>
-      <c r="FO157"/>
-      <c r="FP157"/>
-      <c r="FQ157"/>
-      <c r="FR157"/>
-      <c r="FS157"/>
-      <c r="FT157"/>
-      <c r="FU157"/>
-      <c r="FV157"/>
-      <c r="FW157"/>
-      <c r="FX157"/>
-      <c r="FY157"/>
-      <c r="FZ157"/>
-      <c r="GA157"/>
-      <c r="GB157"/>
-      <c r="GC157"/>
-      <c r="GD157"/>
-      <c r="GE157"/>
-      <c r="GF157"/>
-      <c r="GG157"/>
-      <c r="GH157"/>
-      <c r="GI157"/>
-      <c r="GJ157"/>
-      <c r="GK157"/>
-      <c r="GL157"/>
-      <c r="GM157"/>
-      <c r="GN157"/>
-      <c r="GO157"/>
-      <c r="GP157"/>
-      <c r="GQ157"/>
-      <c r="GR157"/>
-      <c r="GS157"/>
-      <c r="GT157"/>
-      <c r="GU157"/>
-      <c r="GV157"/>
-      <c r="GW157"/>
-      <c r="GX157"/>
-      <c r="GY157"/>
-      <c r="GZ157"/>
-      <c r="HA157"/>
-      <c r="HB157"/>
-      <c r="HC157"/>
-      <c r="HD157"/>
-      <c r="HE157"/>
-      <c r="HF157"/>
-      <c r="HG157"/>
-      <c r="HH157"/>
-      <c r="HI157"/>
-      <c r="HJ157"/>
-      <c r="HK157"/>
-      <c r="HL157"/>
-      <c r="HM157"/>
-      <c r="HN157"/>
-      <c r="HO157"/>
-      <c r="HP157"/>
-      <c r="HQ157"/>
-      <c r="HR157"/>
-      <c r="HS157"/>
-      <c r="HT157"/>
-      <c r="HU157"/>
-      <c r="HV157"/>
-      <c r="HW157"/>
-      <c r="HX157"/>
-      <c r="HY157"/>
-      <c r="HZ157"/>
-      <c r="IA157"/>
-      <c r="IB157"/>
-      <c r="IC157"/>
-      <c r="ID157"/>
-      <c r="IE157"/>
-      <c r="IF157"/>
-      <c r="IG157"/>
-      <c r="IH157"/>
-      <c r="II157"/>
-      <c r="IJ157"/>
-      <c r="IK157"/>
-      <c r="IL157"/>
-      <c r="IM157"/>
-      <c r="IN157"/>
-      <c r="IO157"/>
-      <c r="IP157"/>
-      <c r="IQ157"/>
-      <c r="IR157"/>
-      <c r="IS157"/>
-      <c r="IT157"/>
-      <c r="IU157"/>
-      <c r="IV157"/>
+      <c r="K157" s="1"/>
+      <c r="L157" s="1"/>
+      <c r="M157" s="1"/>
+      <c r="N157" s="1"/>
+      <c r="O157" s="1"/>
+      <c r="P157" s="1"/>
+      <c r="Q157" s="1"/>
+      <c r="R157" s="1"/>
+      <c r="S157" s="1"/>
+      <c r="T157" s="1"/>
+      <c r="U157" s="1"/>
+      <c r="V157" s="1"/>
+      <c r="W157" s="1"/>
+      <c r="X157" s="1"/>
+      <c r="Y157" s="1"/>
+      <c r="Z157" s="1"/>
+      <c r="AA157" s="1"/>
+      <c r="AB157" s="1"/>
+      <c r="AC157" s="1"/>
+      <c r="AD157" s="1"/>
+      <c r="AE157" s="1"/>
+      <c r="AF157" s="1"/>
+      <c r="AG157" s="1"/>
+      <c r="AH157" s="1"/>
+      <c r="AI157" s="1"/>
+      <c r="AJ157" s="1"/>
+      <c r="AK157" s="1"/>
+      <c r="AL157" s="1"/>
+      <c r="AM157" s="1"/>
+      <c r="AN157" s="1"/>
+      <c r="AO157" s="1"/>
+      <c r="AP157" s="1"/>
+      <c r="AQ157" s="1"/>
+      <c r="AR157" s="1"/>
+      <c r="AS157" s="1"/>
+      <c r="AT157" s="1"/>
+      <c r="AU157" s="1"/>
+      <c r="AV157" s="1"/>
+      <c r="AW157" s="1"/>
+      <c r="AX157" s="1"/>
+      <c r="AY157" s="1"/>
+      <c r="AZ157" s="1"/>
+      <c r="BA157" s="1"/>
+      <c r="BB157" s="1"/>
+      <c r="BC157" s="1"/>
+      <c r="BD157" s="1"/>
+      <c r="BE157" s="1"/>
+      <c r="BF157" s="1"/>
+      <c r="BG157" s="1"/>
+      <c r="BH157" s="1"/>
+      <c r="BI157" s="1"/>
+      <c r="BJ157" s="1"/>
+      <c r="BK157" s="1"/>
+      <c r="BL157" s="1"/>
+      <c r="BM157" s="1"/>
+      <c r="BN157" s="1"/>
+      <c r="BO157" s="1"/>
+      <c r="BP157" s="1"/>
+      <c r="BQ157" s="1"/>
+      <c r="BR157" s="1"/>
+      <c r="BS157" s="1"/>
+      <c r="BT157" s="1"/>
+      <c r="BU157" s="1"/>
+      <c r="BV157" s="1"/>
+      <c r="BW157" s="1"/>
+      <c r="BX157" s="1"/>
+      <c r="BY157" s="1"/>
+      <c r="BZ157" s="1"/>
+      <c r="CA157" s="1"/>
+      <c r="CB157" s="1"/>
+      <c r="CC157" s="1"/>
+      <c r="CD157" s="1"/>
+      <c r="CE157" s="1"/>
+      <c r="CF157" s="1"/>
+      <c r="CG157" s="1"/>
+      <c r="CH157" s="1"/>
+      <c r="CI157" s="1"/>
+      <c r="CJ157" s="1"/>
+      <c r="CK157" s="1"/>
+      <c r="CL157" s="1"/>
+      <c r="CM157" s="1"/>
+      <c r="CN157" s="1"/>
+      <c r="CO157" s="1"/>
+      <c r="CP157" s="1"/>
+      <c r="CQ157" s="1"/>
+      <c r="CR157" s="1"/>
+      <c r="CS157" s="1"/>
+      <c r="CT157" s="1"/>
+      <c r="CU157" s="1"/>
+      <c r="CV157" s="1"/>
+      <c r="CW157" s="1"/>
+      <c r="CX157" s="1"/>
+      <c r="CY157" s="1"/>
+      <c r="CZ157" s="1"/>
+      <c r="DA157" s="1"/>
+      <c r="DB157" s="1"/>
+      <c r="DC157" s="1"/>
+      <c r="DD157" s="1"/>
+      <c r="DE157" s="1"/>
+      <c r="DF157" s="1"/>
+      <c r="DG157" s="1"/>
+      <c r="DH157" s="1"/>
+      <c r="DI157" s="1"/>
+      <c r="DJ157" s="1"/>
+      <c r="DK157" s="1"/>
+      <c r="DL157" s="1"/>
+      <c r="DM157" s="1"/>
+      <c r="DN157" s="1"/>
+      <c r="DO157" s="1"/>
+      <c r="DP157" s="1"/>
+      <c r="DQ157" s="1"/>
+      <c r="DR157" s="1"/>
+      <c r="DS157" s="1"/>
+      <c r="DT157" s="1"/>
+      <c r="DU157" s="1"/>
+      <c r="DV157" s="1"/>
+      <c r="DW157" s="1"/>
+      <c r="DX157" s="1"/>
+      <c r="DY157" s="1"/>
+      <c r="DZ157" s="1"/>
+      <c r="EA157" s="1"/>
+      <c r="EB157" s="1"/>
+      <c r="EC157" s="1"/>
+      <c r="ED157" s="1"/>
+      <c r="EE157" s="1"/>
+      <c r="EF157" s="1"/>
+      <c r="EG157" s="1"/>
+      <c r="EH157" s="1"/>
+      <c r="EI157" s="1"/>
+      <c r="EJ157" s="1"/>
+      <c r="EK157" s="1"/>
+      <c r="EL157" s="1"/>
+      <c r="EM157" s="1"/>
+      <c r="EN157" s="1"/>
+      <c r="EO157" s="1"/>
+      <c r="EP157" s="1"/>
+      <c r="EQ157" s="1"/>
+      <c r="ER157" s="1"/>
+      <c r="ES157" s="1"/>
+      <c r="ET157" s="1"/>
+      <c r="EU157" s="1"/>
+      <c r="EV157" s="1"/>
+      <c r="EW157" s="1"/>
+      <c r="EX157" s="1"/>
+      <c r="EY157" s="1"/>
+      <c r="EZ157" s="1"/>
+      <c r="FA157" s="1"/>
+      <c r="FB157" s="1"/>
+      <c r="FC157" s="1"/>
+      <c r="FD157" s="1"/>
+      <c r="FE157" s="1"/>
+      <c r="FF157" s="1"/>
+      <c r="FG157" s="1"/>
+      <c r="FH157" s="1"/>
+      <c r="FI157" s="1"/>
+      <c r="FJ157" s="1"/>
+      <c r="FK157" s="1"/>
+      <c r="FL157" s="1"/>
+      <c r="FM157" s="1"/>
+      <c r="FN157" s="1"/>
+      <c r="FO157" s="1"/>
+      <c r="FP157" s="1"/>
+      <c r="FQ157" s="1"/>
+      <c r="FR157" s="1"/>
+      <c r="FS157" s="1"/>
+      <c r="FT157" s="1"/>
+      <c r="FU157" s="1"/>
+      <c r="FV157" s="1"/>
+      <c r="FW157" s="1"/>
+      <c r="FX157" s="1"/>
+      <c r="FY157" s="1"/>
+      <c r="FZ157" s="1"/>
+      <c r="GA157" s="1"/>
+      <c r="GB157" s="1"/>
+      <c r="GC157" s="1"/>
+      <c r="GD157" s="1"/>
+      <c r="GE157" s="1"/>
+      <c r="GF157" s="1"/>
+      <c r="GG157" s="1"/>
+      <c r="GH157" s="1"/>
+      <c r="GI157" s="1"/>
+      <c r="GJ157" s="1"/>
+      <c r="GK157" s="1"/>
+      <c r="GL157" s="1"/>
+      <c r="GM157" s="1"/>
+      <c r="GN157" s="1"/>
+      <c r="GO157" s="1"/>
+      <c r="GP157" s="1"/>
+      <c r="GQ157" s="1"/>
+      <c r="GR157" s="1"/>
+      <c r="GS157" s="1"/>
+      <c r="GT157" s="1"/>
+      <c r="GU157" s="1"/>
+      <c r="GV157" s="1"/>
+      <c r="GW157" s="1"/>
+      <c r="GX157" s="1"/>
+      <c r="GY157" s="1"/>
+      <c r="GZ157" s="1"/>
+      <c r="HA157" s="1"/>
+      <c r="HB157" s="1"/>
+      <c r="HC157" s="1"/>
+      <c r="HD157" s="1"/>
+      <c r="HE157" s="1"/>
+      <c r="HF157" s="1"/>
+      <c r="HG157" s="1"/>
+      <c r="HH157" s="1"/>
+      <c r="HI157" s="1"/>
+      <c r="HJ157" s="1"/>
+      <c r="HK157" s="1"/>
+      <c r="HL157" s="1"/>
+      <c r="HM157" s="1"/>
+      <c r="HN157" s="1"/>
+      <c r="HO157" s="1"/>
+      <c r="HP157" s="1"/>
+      <c r="HQ157" s="1"/>
+      <c r="HR157" s="1"/>
+      <c r="HS157" s="1"/>
+      <c r="HT157" s="1"/>
+      <c r="HU157" s="1"/>
+      <c r="HV157" s="1"/>
+      <c r="HW157" s="1"/>
+      <c r="HX157" s="1"/>
+      <c r="HY157" s="1"/>
+      <c r="HZ157" s="1"/>
+      <c r="IA157" s="1"/>
+      <c r="IB157" s="1"/>
+      <c r="IC157" s="1"/>
+      <c r="ID157" s="1"/>
+      <c r="IE157" s="1"/>
+      <c r="IF157" s="1"/>
+      <c r="IG157" s="1"/>
+      <c r="IH157" s="1"/>
+      <c r="II157" s="1"/>
+      <c r="IJ157" s="1"/>
+      <c r="IK157" s="1"/>
+      <c r="IL157" s="1"/>
+      <c r="IM157" s="1"/>
+      <c r="IN157" s="1"/>
+      <c r="IO157" s="1"/>
+      <c r="IP157" s="1"/>
+      <c r="IQ157" s="1"/>
+      <c r="IR157" s="1"/>
+      <c r="IS157" s="1"/>
+      <c r="IT157" s="1"/>
+      <c r="IU157" s="1"/>
+      <c r="IV157" s="1"/>
     </row>
     <row r="158" ht="12.8">
       <c r="K158" s="1"/>

</xml_diff>

<commit_message>
Revert "feat(dialog): update CN data and dialogue Excel files"
This reverts commit 6e92b9ce6ea970d77f1880eb08b69162b48182d4.
</commit_message>
<xml_diff>
--- a/Original/CN/Dialog/Drama/_main.xlsx
+++ b/Original/CN/Dialog/Drama/_main.xlsx
@@ -822,11 +822,11 @@
 I...well, I'll leave the rest to your imagination.</t>
   </si>
   <si>
-    <t xml:space="preserve">…我々ミシリアの者にとって、シェトラス様は父親であり、頭の上がらぬ先生だ。なにせ、100年以上もこの国を見守ってきたのだからね。さすがの君も、シェトラス様にはかなわなかったか。
+    <t xml:space="preserve">…我々ミシリアの者にとって、シェトラス様は父親であり、頭の上がらぬ先生だ。なにせ、200年もこの国を見守ってきたのだからね。さすがの君も、シェトラス様にはかなわなかったか。
 君が稽古に顔を見せなくなり、街外れの丘で一人リラの練習をしていると聞いたときは、恋の熱にでも浮かされたのかと皆勘ぐったものだ。だが、最近はリラを担いだ姿が板に付いてきている。</t>
   </si>
   <si>
-    <t xml:space="preserve">...For those of us in Mysilia, Master Cetrus is a father and a teacher we cannot look up to. After all, he has been watching over this country for a hundred years and more. Even you are just like a spoiled child to him.
+    <t xml:space="preserve">...For those of us in Mysilia, Master Cetrus is a father and a teacher we cannot look up to. After all, he has been watching over this country for 200 years. Even you are just like a spoiled child to him.
 We all wondered if you had been carried away by the fever of love when you had stopped showing up for practice and we heard that you were practicing lyra alone on a hill. But nowadays, you are getting used to carrying your lyra.</t>
   </si>
   <si>
@@ -1110,7 +1110,7 @@
 …その力を解放するすべは、長い時の流れの中で失われてしまいました。</t>
   </si>
   <si>
-    <t xml:space="preserve">O  daughter of the forest, a mortal, yet one who hears my voice. My name is Onev, the companion of the great Unyielding Tree, the first being and the mother of all living things in Ylva.
+    <t xml:space="preserve">O  daughter of the forest, a mortal, yet one who hears my voice. My name is Ornev, the companion of the great Unyielding Tree, the first being and the mother of all living things in Ylva.
 The crystal you see before you is a petrified form of an ancient tree together with ether. It is a crystal that contains immense power.
 ...The means to release the power has been lost in the long passage of time.</t>
   </si>
@@ -2023,15 +2023,15 @@
   </si>
   <si>
     <t xml:space="preserve">倒也没什么特别值得一说的。
-你也知道，我以前是泽纳恩那边的人，因为做了些蠢事，在10年前逃亡到了米西利亚这边来。那时的我只懂舞刀弄剑的，加上人生地不熟，日子也不好过。</t>
+你也知道，我以前是扎南那边的人，因为做了些蠢事，在10年前逃亡到了米西利亚这边来。那时的我只懂舞刀弄剑的，加上人生地不熟，日子也不好过。</t>
   </si>
   <si>
     <t xml:space="preserve">后来有一天，我在酒馆机缘巧合的遇到了一位弹着莱雅琴的男子。当然，我那时候并不知道他就是赛特拉斯大人。
-只是看大伙都觉得他那样玩弄乐器很优雅，就嘲讽说「乐器是给女人和孩子玩的东西」。后来你猜怎么着，他既不生气也不反驳，而是在看过我一眼后，没把我当回事的自顾自的演奏起了一曲泽纳恩的牧歌。
+只是看大伙都觉得他那样玩弄乐器很优雅，就嘲讽说「乐器是给女人和孩子玩的东西」。后来你猜怎么着，他既不生气也不反驳，而是在看过我一眼后，没把我当回事的自顾自的演奏起了一曲扎南的牧歌。
 然后我就…哎，算了，不跟你说了。后来的事就任你想象吧。</t>
   </si>
   <si>
-    <t xml:space="preserve">…对我们米西利亚人来说，赛特拉斯大人是一位让人感到亲近信任的慈祥父亲，也是一位让人不敢抬头直视的严厉老师。毕竟他已经守护了这个国家100多年。我看就算是你，也赢不过赛特拉斯大人吧。
+    <t xml:space="preserve">…对我们米西利亚人来说，赛特拉斯大人是一位让人感到亲近信任的慈祥父亲，也是一位让人不敢抬头直视的严厉老师。毕竟他已经守护了这个国家200年。你就是发飙也赢不过他吧。
 说起来，后来从人们口中得知你不练习剑术，而是跑到郊外的山丘上一个人练莱雅琴的时候，大家还以为你是爱上了哪个女人呢。不知不觉时间又过去那么久，现在看惯了你背着莱雅琴的样子，反而觉得这样才像你。</t>
   </si>
   <si>
@@ -2044,7 +2044,7 @@
   <si>
     <t xml:space="preserve">我喜欢米西利亚这个地方。
 虽然最开始在这里生活的那段日子里，人们看到我这么个大个子在扛着乐器四处走动都会笑话我，但后来米西利亚终究是接受了无家可归又性格偏激的我。不仅如此，我还在这里找到了毕生的挚友和美丽的妻子，有了个吵闹的秃头老丈人，每天的日子都变得热闹得很啊。
-让那又小又穷的泽纳恩吃屎去吧！我，我要为我好不容易找寻到的故乡献出我的心脏。</t>
+让那又小又穷的扎南吃屎去吧！我，我要为我好不容易找寻到的故乡献出我的心脏。</t>
   </si>
   <si>
     <t xml:space="preserve">…虽然算是借着酒劲说出来的话吧。但你能有这样的觉悟，是谁都会高看你一眼的。
@@ -2353,7 +2353,7 @@
     <t xml:space="preserve">他双手握住一个被扯断了的少女的手臂，蹲在地上。</t>
   </si>
   <si>
-    <t xml:space="preserve">在这场战斗中失去大部分主战斗力的泽纳恩开始撤退。</t>
+    <t xml:space="preserve">在这场战斗中失去大部分主战斗力的扎南开始撤退。</t>
   </si>
   <si>
     <t xml:space="preserve">贝里希失踪了。</t>
@@ -2362,7 +2362,7 @@
     <t xml:space="preserve">- 孤儿院地下 -</t>
   </si>
   <si>
-    <t xml:space="preserve">表现·测试效果。</t>
+    <t xml:space="preserve">表现・测试效果。</t>
   </si>
   <si>
     <t xml:space="preserve">呼唤风吧。</t>
@@ -3269,9 +3269,9 @@
   <dimension ref="A1:IW492"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K482" sqref="K482"/>
-      <selection pane="bottomLeft" activeCell="J153" sqref="J153"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.8"/>
@@ -29966,252 +29966,252 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
-      <c r="S52" s="1"/>
-      <c r="T52" s="1"/>
-      <c r="U52" s="1"/>
-      <c r="V52" s="1"/>
-      <c r="W52" s="1"/>
-      <c r="X52" s="1"/>
-      <c r="Y52" s="1"/>
-      <c r="Z52" s="1"/>
-      <c r="AA52" s="1"/>
-      <c r="AB52" s="1"/>
-      <c r="AC52" s="1"/>
-      <c r="AD52" s="1"/>
-      <c r="AE52" s="1"/>
-      <c r="AF52" s="1"/>
-      <c r="AG52" s="1"/>
-      <c r="AH52" s="1"/>
-      <c r="AI52" s="1"/>
-      <c r="AJ52" s="1"/>
-      <c r="AK52" s="1"/>
-      <c r="AL52" s="1"/>
-      <c r="AM52" s="1"/>
-      <c r="AN52" s="1"/>
-      <c r="AO52" s="1"/>
-      <c r="AP52" s="1"/>
-      <c r="AQ52" s="1"/>
-      <c r="AR52" s="1"/>
-      <c r="AS52" s="1"/>
-      <c r="AT52" s="1"/>
-      <c r="AU52" s="1"/>
-      <c r="AV52" s="1"/>
-      <c r="AW52" s="1"/>
-      <c r="AX52" s="1"/>
-      <c r="AY52" s="1"/>
-      <c r="AZ52" s="1"/>
-      <c r="BA52" s="1"/>
-      <c r="BB52" s="1"/>
-      <c r="BC52" s="1"/>
-      <c r="BD52" s="1"/>
-      <c r="BE52" s="1"/>
-      <c r="BF52" s="1"/>
-      <c r="BG52" s="1"/>
-      <c r="BH52" s="1"/>
-      <c r="BI52" s="1"/>
-      <c r="BJ52" s="1"/>
-      <c r="BK52" s="1"/>
-      <c r="BL52" s="1"/>
-      <c r="BM52" s="1"/>
-      <c r="BN52" s="1"/>
-      <c r="BO52" s="1"/>
-      <c r="BP52" s="1"/>
-      <c r="BQ52" s="1"/>
-      <c r="BR52" s="1"/>
-      <c r="BS52" s="1"/>
-      <c r="BT52" s="1"/>
-      <c r="BU52" s="1"/>
-      <c r="BV52" s="1"/>
-      <c r="BW52" s="1"/>
-      <c r="BX52" s="1"/>
-      <c r="BY52" s="1"/>
-      <c r="BZ52" s="1"/>
-      <c r="CA52" s="1"/>
-      <c r="CB52" s="1"/>
-      <c r="CC52" s="1"/>
-      <c r="CD52" s="1"/>
-      <c r="CE52" s="1"/>
-      <c r="CF52" s="1"/>
-      <c r="CG52" s="1"/>
-      <c r="CH52" s="1"/>
-      <c r="CI52" s="1"/>
-      <c r="CJ52" s="1"/>
-      <c r="CK52" s="1"/>
-      <c r="CL52" s="1"/>
-      <c r="CM52" s="1"/>
-      <c r="CN52" s="1"/>
-      <c r="CO52" s="1"/>
-      <c r="CP52" s="1"/>
-      <c r="CQ52" s="1"/>
-      <c r="CR52" s="1"/>
-      <c r="CS52" s="1"/>
-      <c r="CT52" s="1"/>
-      <c r="CU52" s="1"/>
-      <c r="CV52" s="1"/>
-      <c r="CW52" s="1"/>
-      <c r="CX52" s="1"/>
-      <c r="CY52" s="1"/>
-      <c r="CZ52" s="1"/>
-      <c r="DA52" s="1"/>
-      <c r="DB52" s="1"/>
-      <c r="DC52" s="1"/>
-      <c r="DD52" s="1"/>
-      <c r="DE52" s="1"/>
-      <c r="DF52" s="1"/>
-      <c r="DG52" s="1"/>
-      <c r="DH52" s="1"/>
-      <c r="DI52" s="1"/>
-      <c r="DJ52" s="1"/>
-      <c r="DK52" s="1"/>
-      <c r="DL52" s="1"/>
-      <c r="DM52" s="1"/>
-      <c r="DN52" s="1"/>
-      <c r="DO52" s="1"/>
-      <c r="DP52" s="1"/>
-      <c r="DQ52" s="1"/>
-      <c r="DR52" s="1"/>
-      <c r="DS52" s="1"/>
-      <c r="DT52" s="1"/>
-      <c r="DU52" s="1"/>
-      <c r="DV52" s="1"/>
-      <c r="DW52" s="1"/>
-      <c r="DX52" s="1"/>
-      <c r="DY52" s="1"/>
-      <c r="DZ52" s="1"/>
-      <c r="EA52" s="1"/>
-      <c r="EB52" s="1"/>
-      <c r="EC52" s="1"/>
-      <c r="ED52" s="1"/>
-      <c r="EE52" s="1"/>
-      <c r="EF52" s="1"/>
-      <c r="EG52" s="1"/>
-      <c r="EH52" s="1"/>
-      <c r="EI52" s="1"/>
-      <c r="EJ52" s="1"/>
-      <c r="EK52" s="1"/>
-      <c r="EL52" s="1"/>
-      <c r="EM52" s="1"/>
-      <c r="EN52" s="1"/>
-      <c r="EO52" s="1"/>
-      <c r="EP52" s="1"/>
-      <c r="EQ52" s="1"/>
-      <c r="ER52" s="1"/>
-      <c r="ES52" s="1"/>
-      <c r="ET52" s="1"/>
-      <c r="EU52" s="1"/>
-      <c r="EV52" s="1"/>
-      <c r="EW52" s="1"/>
-      <c r="EX52" s="1"/>
-      <c r="EY52" s="1"/>
-      <c r="EZ52" s="1"/>
-      <c r="FA52" s="1"/>
-      <c r="FB52" s="1"/>
-      <c r="FC52" s="1"/>
-      <c r="FD52" s="1"/>
-      <c r="FE52" s="1"/>
-      <c r="FF52" s="1"/>
-      <c r="FG52" s="1"/>
-      <c r="FH52" s="1"/>
-      <c r="FI52" s="1"/>
-      <c r="FJ52" s="1"/>
-      <c r="FK52" s="1"/>
-      <c r="FL52" s="1"/>
-      <c r="FM52" s="1"/>
-      <c r="FN52" s="1"/>
-      <c r="FO52" s="1"/>
-      <c r="FP52" s="1"/>
-      <c r="FQ52" s="1"/>
-      <c r="FR52" s="1"/>
-      <c r="FS52" s="1"/>
-      <c r="FT52" s="1"/>
-      <c r="FU52" s="1"/>
-      <c r="FV52" s="1"/>
-      <c r="FW52" s="1"/>
-      <c r="FX52" s="1"/>
-      <c r="FY52" s="1"/>
-      <c r="FZ52" s="1"/>
-      <c r="GA52" s="1"/>
-      <c r="GB52" s="1"/>
-      <c r="GC52" s="1"/>
-      <c r="GD52" s="1"/>
-      <c r="GE52" s="1"/>
-      <c r="GF52" s="1"/>
-      <c r="GG52" s="1"/>
-      <c r="GH52" s="1"/>
-      <c r="GI52" s="1"/>
-      <c r="GJ52" s="1"/>
-      <c r="GK52" s="1"/>
-      <c r="GL52" s="1"/>
-      <c r="GM52" s="1"/>
-      <c r="GN52" s="1"/>
-      <c r="GO52" s="1"/>
-      <c r="GP52" s="1"/>
-      <c r="GQ52" s="1"/>
-      <c r="GR52" s="1"/>
-      <c r="GS52" s="1"/>
-      <c r="GT52" s="1"/>
-      <c r="GU52" s="1"/>
-      <c r="GV52" s="1"/>
-      <c r="GW52" s="1"/>
-      <c r="GX52" s="1"/>
-      <c r="GY52" s="1"/>
-      <c r="GZ52" s="1"/>
-      <c r="HA52" s="1"/>
-      <c r="HB52" s="1"/>
-      <c r="HC52" s="1"/>
-      <c r="HD52" s="1"/>
-      <c r="HE52" s="1"/>
-      <c r="HF52" s="1"/>
-      <c r="HG52" s="1"/>
-      <c r="HH52" s="1"/>
-      <c r="HI52" s="1"/>
-      <c r="HJ52" s="1"/>
-      <c r="HK52" s="1"/>
-      <c r="HL52" s="1"/>
-      <c r="HM52" s="1"/>
-      <c r="HN52" s="1"/>
-      <c r="HO52" s="1"/>
-      <c r="HP52" s="1"/>
-      <c r="HQ52" s="1"/>
-      <c r="HR52" s="1"/>
-      <c r="HS52" s="1"/>
-      <c r="HT52" s="1"/>
-      <c r="HU52" s="1"/>
-      <c r="HV52" s="1"/>
-      <c r="HW52" s="1"/>
-      <c r="HX52" s="1"/>
-      <c r="HY52" s="1"/>
-      <c r="HZ52" s="1"/>
-      <c r="IA52" s="1"/>
-      <c r="IB52" s="1"/>
-      <c r="IC52" s="1"/>
-      <c r="ID52" s="1"/>
-      <c r="IE52" s="1"/>
-      <c r="IF52" s="1"/>
-      <c r="IG52" s="1"/>
-      <c r="IH52" s="1"/>
-      <c r="II52" s="1"/>
-      <c r="IJ52" s="1"/>
-      <c r="IK52" s="1"/>
-      <c r="IL52" s="1"/>
-      <c r="IM52" s="1"/>
-      <c r="IN52" s="1"/>
-      <c r="IO52" s="1"/>
-      <c r="IP52" s="1"/>
-      <c r="IQ52" s="1"/>
-      <c r="IR52" s="1"/>
-      <c r="IS52" s="1"/>
-      <c r="IT52" s="1"/>
-      <c r="IU52" s="1"/>
-      <c r="IV52" s="1"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+      <c r="V52"/>
+      <c r="W52"/>
+      <c r="X52"/>
+      <c r="Y52"/>
+      <c r="Z52"/>
+      <c r="AA52"/>
+      <c r="AB52"/>
+      <c r="AC52"/>
+      <c r="AD52"/>
+      <c r="AE52"/>
+      <c r="AF52"/>
+      <c r="AG52"/>
+      <c r="AH52"/>
+      <c r="AI52"/>
+      <c r="AJ52"/>
+      <c r="AK52"/>
+      <c r="AL52"/>
+      <c r="AM52"/>
+      <c r="AN52"/>
+      <c r="AO52"/>
+      <c r="AP52"/>
+      <c r="AQ52"/>
+      <c r="AR52"/>
+      <c r="AS52"/>
+      <c r="AT52"/>
+      <c r="AU52"/>
+      <c r="AV52"/>
+      <c r="AW52"/>
+      <c r="AX52"/>
+      <c r="AY52"/>
+      <c r="AZ52"/>
+      <c r="BA52"/>
+      <c r="BB52"/>
+      <c r="BC52"/>
+      <c r="BD52"/>
+      <c r="BE52"/>
+      <c r="BF52"/>
+      <c r="BG52"/>
+      <c r="BH52"/>
+      <c r="BI52"/>
+      <c r="BJ52"/>
+      <c r="BK52"/>
+      <c r="BL52"/>
+      <c r="BM52"/>
+      <c r="BN52"/>
+      <c r="BO52"/>
+      <c r="BP52"/>
+      <c r="BQ52"/>
+      <c r="BR52"/>
+      <c r="BS52"/>
+      <c r="BT52"/>
+      <c r="BU52"/>
+      <c r="BV52"/>
+      <c r="BW52"/>
+      <c r="BX52"/>
+      <c r="BY52"/>
+      <c r="BZ52"/>
+      <c r="CA52"/>
+      <c r="CB52"/>
+      <c r="CC52"/>
+      <c r="CD52"/>
+      <c r="CE52"/>
+      <c r="CF52"/>
+      <c r="CG52"/>
+      <c r="CH52"/>
+      <c r="CI52"/>
+      <c r="CJ52"/>
+      <c r="CK52"/>
+      <c r="CL52"/>
+      <c r="CM52"/>
+      <c r="CN52"/>
+      <c r="CO52"/>
+      <c r="CP52"/>
+      <c r="CQ52"/>
+      <c r="CR52"/>
+      <c r="CS52"/>
+      <c r="CT52"/>
+      <c r="CU52"/>
+      <c r="CV52"/>
+      <c r="CW52"/>
+      <c r="CX52"/>
+      <c r="CY52"/>
+      <c r="CZ52"/>
+      <c r="DA52"/>
+      <c r="DB52"/>
+      <c r="DC52"/>
+      <c r="DD52"/>
+      <c r="DE52"/>
+      <c r="DF52"/>
+      <c r="DG52"/>
+      <c r="DH52"/>
+      <c r="DI52"/>
+      <c r="DJ52"/>
+      <c r="DK52"/>
+      <c r="DL52"/>
+      <c r="DM52"/>
+      <c r="DN52"/>
+      <c r="DO52"/>
+      <c r="DP52"/>
+      <c r="DQ52"/>
+      <c r="DR52"/>
+      <c r="DS52"/>
+      <c r="DT52"/>
+      <c r="DU52"/>
+      <c r="DV52"/>
+      <c r="DW52"/>
+      <c r="DX52"/>
+      <c r="DY52"/>
+      <c r="DZ52"/>
+      <c r="EA52"/>
+      <c r="EB52"/>
+      <c r="EC52"/>
+      <c r="ED52"/>
+      <c r="EE52"/>
+      <c r="EF52"/>
+      <c r="EG52"/>
+      <c r="EH52"/>
+      <c r="EI52"/>
+      <c r="EJ52"/>
+      <c r="EK52"/>
+      <c r="EL52"/>
+      <c r="EM52"/>
+      <c r="EN52"/>
+      <c r="EO52"/>
+      <c r="EP52"/>
+      <c r="EQ52"/>
+      <c r="ER52"/>
+      <c r="ES52"/>
+      <c r="ET52"/>
+      <c r="EU52"/>
+      <c r="EV52"/>
+      <c r="EW52"/>
+      <c r="EX52"/>
+      <c r="EY52"/>
+      <c r="EZ52"/>
+      <c r="FA52"/>
+      <c r="FB52"/>
+      <c r="FC52"/>
+      <c r="FD52"/>
+      <c r="FE52"/>
+      <c r="FF52"/>
+      <c r="FG52"/>
+      <c r="FH52"/>
+      <c r="FI52"/>
+      <c r="FJ52"/>
+      <c r="FK52"/>
+      <c r="FL52"/>
+      <c r="FM52"/>
+      <c r="FN52"/>
+      <c r="FO52"/>
+      <c r="FP52"/>
+      <c r="FQ52"/>
+      <c r="FR52"/>
+      <c r="FS52"/>
+      <c r="FT52"/>
+      <c r="FU52"/>
+      <c r="FV52"/>
+      <c r="FW52"/>
+      <c r="FX52"/>
+      <c r="FY52"/>
+      <c r="FZ52"/>
+      <c r="GA52"/>
+      <c r="GB52"/>
+      <c r="GC52"/>
+      <c r="GD52"/>
+      <c r="GE52"/>
+      <c r="GF52"/>
+      <c r="GG52"/>
+      <c r="GH52"/>
+      <c r="GI52"/>
+      <c r="GJ52"/>
+      <c r="GK52"/>
+      <c r="GL52"/>
+      <c r="GM52"/>
+      <c r="GN52"/>
+      <c r="GO52"/>
+      <c r="GP52"/>
+      <c r="GQ52"/>
+      <c r="GR52"/>
+      <c r="GS52"/>
+      <c r="GT52"/>
+      <c r="GU52"/>
+      <c r="GV52"/>
+      <c r="GW52"/>
+      <c r="GX52"/>
+      <c r="GY52"/>
+      <c r="GZ52"/>
+      <c r="HA52"/>
+      <c r="HB52"/>
+      <c r="HC52"/>
+      <c r="HD52"/>
+      <c r="HE52"/>
+      <c r="HF52"/>
+      <c r="HG52"/>
+      <c r="HH52"/>
+      <c r="HI52"/>
+      <c r="HJ52"/>
+      <c r="HK52"/>
+      <c r="HL52"/>
+      <c r="HM52"/>
+      <c r="HN52"/>
+      <c r="HO52"/>
+      <c r="HP52"/>
+      <c r="HQ52"/>
+      <c r="HR52"/>
+      <c r="HS52"/>
+      <c r="HT52"/>
+      <c r="HU52"/>
+      <c r="HV52"/>
+      <c r="HW52"/>
+      <c r="HX52"/>
+      <c r="HY52"/>
+      <c r="HZ52"/>
+      <c r="IA52"/>
+      <c r="IB52"/>
+      <c r="IC52"/>
+      <c r="ID52"/>
+      <c r="IE52"/>
+      <c r="IF52"/>
+      <c r="IG52"/>
+      <c r="IH52"/>
+      <c r="II52"/>
+      <c r="IJ52"/>
+      <c r="IK52"/>
+      <c r="IL52"/>
+      <c r="IM52"/>
+      <c r="IN52"/>
+      <c r="IO52"/>
+      <c r="IP52"/>
+      <c r="IQ52"/>
+      <c r="IR52"/>
+      <c r="IS52"/>
+      <c r="IT52"/>
+      <c r="IU52"/>
+      <c r="IV52"/>
     </row>
     <row r="53" ht="12.8">
       <c r="K53" s="1"/>
@@ -31179,252 +31179,252 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
-      <c r="N80" s="1"/>
-      <c r="O80" s="1"/>
-      <c r="P80" s="1"/>
-      <c r="Q80" s="1"/>
-      <c r="R80" s="1"/>
-      <c r="S80" s="1"/>
-      <c r="T80" s="1"/>
-      <c r="U80" s="1"/>
-      <c r="V80" s="1"/>
-      <c r="W80" s="1"/>
-      <c r="X80" s="1"/>
-      <c r="Y80" s="1"/>
-      <c r="Z80" s="1"/>
-      <c r="AA80" s="1"/>
-      <c r="AB80" s="1"/>
-      <c r="AC80" s="1"/>
-      <c r="AD80" s="1"/>
-      <c r="AE80" s="1"/>
-      <c r="AF80" s="1"/>
-      <c r="AG80" s="1"/>
-      <c r="AH80" s="1"/>
-      <c r="AI80" s="1"/>
-      <c r="AJ80" s="1"/>
-      <c r="AK80" s="1"/>
-      <c r="AL80" s="1"/>
-      <c r="AM80" s="1"/>
-      <c r="AN80" s="1"/>
-      <c r="AO80" s="1"/>
-      <c r="AP80" s="1"/>
-      <c r="AQ80" s="1"/>
-      <c r="AR80" s="1"/>
-      <c r="AS80" s="1"/>
-      <c r="AT80" s="1"/>
-      <c r="AU80" s="1"/>
-      <c r="AV80" s="1"/>
-      <c r="AW80" s="1"/>
-      <c r="AX80" s="1"/>
-      <c r="AY80" s="1"/>
-      <c r="AZ80" s="1"/>
-      <c r="BA80" s="1"/>
-      <c r="BB80" s="1"/>
-      <c r="BC80" s="1"/>
-      <c r="BD80" s="1"/>
-      <c r="BE80" s="1"/>
-      <c r="BF80" s="1"/>
-      <c r="BG80" s="1"/>
-      <c r="BH80" s="1"/>
-      <c r="BI80" s="1"/>
-      <c r="BJ80" s="1"/>
-      <c r="BK80" s="1"/>
-      <c r="BL80" s="1"/>
-      <c r="BM80" s="1"/>
-      <c r="BN80" s="1"/>
-      <c r="BO80" s="1"/>
-      <c r="BP80" s="1"/>
-      <c r="BQ80" s="1"/>
-      <c r="BR80" s="1"/>
-      <c r="BS80" s="1"/>
-      <c r="BT80" s="1"/>
-      <c r="BU80" s="1"/>
-      <c r="BV80" s="1"/>
-      <c r="BW80" s="1"/>
-      <c r="BX80" s="1"/>
-      <c r="BY80" s="1"/>
-      <c r="BZ80" s="1"/>
-      <c r="CA80" s="1"/>
-      <c r="CB80" s="1"/>
-      <c r="CC80" s="1"/>
-      <c r="CD80" s="1"/>
-      <c r="CE80" s="1"/>
-      <c r="CF80" s="1"/>
-      <c r="CG80" s="1"/>
-      <c r="CH80" s="1"/>
-      <c r="CI80" s="1"/>
-      <c r="CJ80" s="1"/>
-      <c r="CK80" s="1"/>
-      <c r="CL80" s="1"/>
-      <c r="CM80" s="1"/>
-      <c r="CN80" s="1"/>
-      <c r="CO80" s="1"/>
-      <c r="CP80" s="1"/>
-      <c r="CQ80" s="1"/>
-      <c r="CR80" s="1"/>
-      <c r="CS80" s="1"/>
-      <c r="CT80" s="1"/>
-      <c r="CU80" s="1"/>
-      <c r="CV80" s="1"/>
-      <c r="CW80" s="1"/>
-      <c r="CX80" s="1"/>
-      <c r="CY80" s="1"/>
-      <c r="CZ80" s="1"/>
-      <c r="DA80" s="1"/>
-      <c r="DB80" s="1"/>
-      <c r="DC80" s="1"/>
-      <c r="DD80" s="1"/>
-      <c r="DE80" s="1"/>
-      <c r="DF80" s="1"/>
-      <c r="DG80" s="1"/>
-      <c r="DH80" s="1"/>
-      <c r="DI80" s="1"/>
-      <c r="DJ80" s="1"/>
-      <c r="DK80" s="1"/>
-      <c r="DL80" s="1"/>
-      <c r="DM80" s="1"/>
-      <c r="DN80" s="1"/>
-      <c r="DO80" s="1"/>
-      <c r="DP80" s="1"/>
-      <c r="DQ80" s="1"/>
-      <c r="DR80" s="1"/>
-      <c r="DS80" s="1"/>
-      <c r="DT80" s="1"/>
-      <c r="DU80" s="1"/>
-      <c r="DV80" s="1"/>
-      <c r="DW80" s="1"/>
-      <c r="DX80" s="1"/>
-      <c r="DY80" s="1"/>
-      <c r="DZ80" s="1"/>
-      <c r="EA80" s="1"/>
-      <c r="EB80" s="1"/>
-      <c r="EC80" s="1"/>
-      <c r="ED80" s="1"/>
-      <c r="EE80" s="1"/>
-      <c r="EF80" s="1"/>
-      <c r="EG80" s="1"/>
-      <c r="EH80" s="1"/>
-      <c r="EI80" s="1"/>
-      <c r="EJ80" s="1"/>
-      <c r="EK80" s="1"/>
-      <c r="EL80" s="1"/>
-      <c r="EM80" s="1"/>
-      <c r="EN80" s="1"/>
-      <c r="EO80" s="1"/>
-      <c r="EP80" s="1"/>
-      <c r="EQ80" s="1"/>
-      <c r="ER80" s="1"/>
-      <c r="ES80" s="1"/>
-      <c r="ET80" s="1"/>
-      <c r="EU80" s="1"/>
-      <c r="EV80" s="1"/>
-      <c r="EW80" s="1"/>
-      <c r="EX80" s="1"/>
-      <c r="EY80" s="1"/>
-      <c r="EZ80" s="1"/>
-      <c r="FA80" s="1"/>
-      <c r="FB80" s="1"/>
-      <c r="FC80" s="1"/>
-      <c r="FD80" s="1"/>
-      <c r="FE80" s="1"/>
-      <c r="FF80" s="1"/>
-      <c r="FG80" s="1"/>
-      <c r="FH80" s="1"/>
-      <c r="FI80" s="1"/>
-      <c r="FJ80" s="1"/>
-      <c r="FK80" s="1"/>
-      <c r="FL80" s="1"/>
-      <c r="FM80" s="1"/>
-      <c r="FN80" s="1"/>
-      <c r="FO80" s="1"/>
-      <c r="FP80" s="1"/>
-      <c r="FQ80" s="1"/>
-      <c r="FR80" s="1"/>
-      <c r="FS80" s="1"/>
-      <c r="FT80" s="1"/>
-      <c r="FU80" s="1"/>
-      <c r="FV80" s="1"/>
-      <c r="FW80" s="1"/>
-      <c r="FX80" s="1"/>
-      <c r="FY80" s="1"/>
-      <c r="FZ80" s="1"/>
-      <c r="GA80" s="1"/>
-      <c r="GB80" s="1"/>
-      <c r="GC80" s="1"/>
-      <c r="GD80" s="1"/>
-      <c r="GE80" s="1"/>
-      <c r="GF80" s="1"/>
-      <c r="GG80" s="1"/>
-      <c r="GH80" s="1"/>
-      <c r="GI80" s="1"/>
-      <c r="GJ80" s="1"/>
-      <c r="GK80" s="1"/>
-      <c r="GL80" s="1"/>
-      <c r="GM80" s="1"/>
-      <c r="GN80" s="1"/>
-      <c r="GO80" s="1"/>
-      <c r="GP80" s="1"/>
-      <c r="GQ80" s="1"/>
-      <c r="GR80" s="1"/>
-      <c r="GS80" s="1"/>
-      <c r="GT80" s="1"/>
-      <c r="GU80" s="1"/>
-      <c r="GV80" s="1"/>
-      <c r="GW80" s="1"/>
-      <c r="GX80" s="1"/>
-      <c r="GY80" s="1"/>
-      <c r="GZ80" s="1"/>
-      <c r="HA80" s="1"/>
-      <c r="HB80" s="1"/>
-      <c r="HC80" s="1"/>
-      <c r="HD80" s="1"/>
-      <c r="HE80" s="1"/>
-      <c r="HF80" s="1"/>
-      <c r="HG80" s="1"/>
-      <c r="HH80" s="1"/>
-      <c r="HI80" s="1"/>
-      <c r="HJ80" s="1"/>
-      <c r="HK80" s="1"/>
-      <c r="HL80" s="1"/>
-      <c r="HM80" s="1"/>
-      <c r="HN80" s="1"/>
-      <c r="HO80" s="1"/>
-      <c r="HP80" s="1"/>
-      <c r="HQ80" s="1"/>
-      <c r="HR80" s="1"/>
-      <c r="HS80" s="1"/>
-      <c r="HT80" s="1"/>
-      <c r="HU80" s="1"/>
-      <c r="HV80" s="1"/>
-      <c r="HW80" s="1"/>
-      <c r="HX80" s="1"/>
-      <c r="HY80" s="1"/>
-      <c r="HZ80" s="1"/>
-      <c r="IA80" s="1"/>
-      <c r="IB80" s="1"/>
-      <c r="IC80" s="1"/>
-      <c r="ID80" s="1"/>
-      <c r="IE80" s="1"/>
-      <c r="IF80" s="1"/>
-      <c r="IG80" s="1"/>
-      <c r="IH80" s="1"/>
-      <c r="II80" s="1"/>
-      <c r="IJ80" s="1"/>
-      <c r="IK80" s="1"/>
-      <c r="IL80" s="1"/>
-      <c r="IM80" s="1"/>
-      <c r="IN80" s="1"/>
-      <c r="IO80" s="1"/>
-      <c r="IP80" s="1"/>
-      <c r="IQ80" s="1"/>
-      <c r="IR80" s="1"/>
-      <c r="IS80" s="1"/>
-      <c r="IT80" s="1"/>
-      <c r="IU80" s="1"/>
-      <c r="IV80" s="1"/>
+      <c r="K80"/>
+      <c r="L80"/>
+      <c r="M80"/>
+      <c r="N80"/>
+      <c r="O80"/>
+      <c r="P80"/>
+      <c r="Q80"/>
+      <c r="R80"/>
+      <c r="S80"/>
+      <c r="T80"/>
+      <c r="U80"/>
+      <c r="V80"/>
+      <c r="W80"/>
+      <c r="X80"/>
+      <c r="Y80"/>
+      <c r="Z80"/>
+      <c r="AA80"/>
+      <c r="AB80"/>
+      <c r="AC80"/>
+      <c r="AD80"/>
+      <c r="AE80"/>
+      <c r="AF80"/>
+      <c r="AG80"/>
+      <c r="AH80"/>
+      <c r="AI80"/>
+      <c r="AJ80"/>
+      <c r="AK80"/>
+      <c r="AL80"/>
+      <c r="AM80"/>
+      <c r="AN80"/>
+      <c r="AO80"/>
+      <c r="AP80"/>
+      <c r="AQ80"/>
+      <c r="AR80"/>
+      <c r="AS80"/>
+      <c r="AT80"/>
+      <c r="AU80"/>
+      <c r="AV80"/>
+      <c r="AW80"/>
+      <c r="AX80"/>
+      <c r="AY80"/>
+      <c r="AZ80"/>
+      <c r="BA80"/>
+      <c r="BB80"/>
+      <c r="BC80"/>
+      <c r="BD80"/>
+      <c r="BE80"/>
+      <c r="BF80"/>
+      <c r="BG80"/>
+      <c r="BH80"/>
+      <c r="BI80"/>
+      <c r="BJ80"/>
+      <c r="BK80"/>
+      <c r="BL80"/>
+      <c r="BM80"/>
+      <c r="BN80"/>
+      <c r="BO80"/>
+      <c r="BP80"/>
+      <c r="BQ80"/>
+      <c r="BR80"/>
+      <c r="BS80"/>
+      <c r="BT80"/>
+      <c r="BU80"/>
+      <c r="BV80"/>
+      <c r="BW80"/>
+      <c r="BX80"/>
+      <c r="BY80"/>
+      <c r="BZ80"/>
+      <c r="CA80"/>
+      <c r="CB80"/>
+      <c r="CC80"/>
+      <c r="CD80"/>
+      <c r="CE80"/>
+      <c r="CF80"/>
+      <c r="CG80"/>
+      <c r="CH80"/>
+      <c r="CI80"/>
+      <c r="CJ80"/>
+      <c r="CK80"/>
+      <c r="CL80"/>
+      <c r="CM80"/>
+      <c r="CN80"/>
+      <c r="CO80"/>
+      <c r="CP80"/>
+      <c r="CQ80"/>
+      <c r="CR80"/>
+      <c r="CS80"/>
+      <c r="CT80"/>
+      <c r="CU80"/>
+      <c r="CV80"/>
+      <c r="CW80"/>
+      <c r="CX80"/>
+      <c r="CY80"/>
+      <c r="CZ80"/>
+      <c r="DA80"/>
+      <c r="DB80"/>
+      <c r="DC80"/>
+      <c r="DD80"/>
+      <c r="DE80"/>
+      <c r="DF80"/>
+      <c r="DG80"/>
+      <c r="DH80"/>
+      <c r="DI80"/>
+      <c r="DJ80"/>
+      <c r="DK80"/>
+      <c r="DL80"/>
+      <c r="DM80"/>
+      <c r="DN80"/>
+      <c r="DO80"/>
+      <c r="DP80"/>
+      <c r="DQ80"/>
+      <c r="DR80"/>
+      <c r="DS80"/>
+      <c r="DT80"/>
+      <c r="DU80"/>
+      <c r="DV80"/>
+      <c r="DW80"/>
+      <c r="DX80"/>
+      <c r="DY80"/>
+      <c r="DZ80"/>
+      <c r="EA80"/>
+      <c r="EB80"/>
+      <c r="EC80"/>
+      <c r="ED80"/>
+      <c r="EE80"/>
+      <c r="EF80"/>
+      <c r="EG80"/>
+      <c r="EH80"/>
+      <c r="EI80"/>
+      <c r="EJ80"/>
+      <c r="EK80"/>
+      <c r="EL80"/>
+      <c r="EM80"/>
+      <c r="EN80"/>
+      <c r="EO80"/>
+      <c r="EP80"/>
+      <c r="EQ80"/>
+      <c r="ER80"/>
+      <c r="ES80"/>
+      <c r="ET80"/>
+      <c r="EU80"/>
+      <c r="EV80"/>
+      <c r="EW80"/>
+      <c r="EX80"/>
+      <c r="EY80"/>
+      <c r="EZ80"/>
+      <c r="FA80"/>
+      <c r="FB80"/>
+      <c r="FC80"/>
+      <c r="FD80"/>
+      <c r="FE80"/>
+      <c r="FF80"/>
+      <c r="FG80"/>
+      <c r="FH80"/>
+      <c r="FI80"/>
+      <c r="FJ80"/>
+      <c r="FK80"/>
+      <c r="FL80"/>
+      <c r="FM80"/>
+      <c r="FN80"/>
+      <c r="FO80"/>
+      <c r="FP80"/>
+      <c r="FQ80"/>
+      <c r="FR80"/>
+      <c r="FS80"/>
+      <c r="FT80"/>
+      <c r="FU80"/>
+      <c r="FV80"/>
+      <c r="FW80"/>
+      <c r="FX80"/>
+      <c r="FY80"/>
+      <c r="FZ80"/>
+      <c r="GA80"/>
+      <c r="GB80"/>
+      <c r="GC80"/>
+      <c r="GD80"/>
+      <c r="GE80"/>
+      <c r="GF80"/>
+      <c r="GG80"/>
+      <c r="GH80"/>
+      <c r="GI80"/>
+      <c r="GJ80"/>
+      <c r="GK80"/>
+      <c r="GL80"/>
+      <c r="GM80"/>
+      <c r="GN80"/>
+      <c r="GO80"/>
+      <c r="GP80"/>
+      <c r="GQ80"/>
+      <c r="GR80"/>
+      <c r="GS80"/>
+      <c r="GT80"/>
+      <c r="GU80"/>
+      <c r="GV80"/>
+      <c r="GW80"/>
+      <c r="GX80"/>
+      <c r="GY80"/>
+      <c r="GZ80"/>
+      <c r="HA80"/>
+      <c r="HB80"/>
+      <c r="HC80"/>
+      <c r="HD80"/>
+      <c r="HE80"/>
+      <c r="HF80"/>
+      <c r="HG80"/>
+      <c r="HH80"/>
+      <c r="HI80"/>
+      <c r="HJ80"/>
+      <c r="HK80"/>
+      <c r="HL80"/>
+      <c r="HM80"/>
+      <c r="HN80"/>
+      <c r="HO80"/>
+      <c r="HP80"/>
+      <c r="HQ80"/>
+      <c r="HR80"/>
+      <c r="HS80"/>
+      <c r="HT80"/>
+      <c r="HU80"/>
+      <c r="HV80"/>
+      <c r="HW80"/>
+      <c r="HX80"/>
+      <c r="HY80"/>
+      <c r="HZ80"/>
+      <c r="IA80"/>
+      <c r="IB80"/>
+      <c r="IC80"/>
+      <c r="ID80"/>
+      <c r="IE80"/>
+      <c r="IF80"/>
+      <c r="IG80"/>
+      <c r="IH80"/>
+      <c r="II80"/>
+      <c r="IJ80"/>
+      <c r="IK80"/>
+      <c r="IL80"/>
+      <c r="IM80"/>
+      <c r="IN80"/>
+      <c r="IO80"/>
+      <c r="IP80"/>
+      <c r="IQ80"/>
+      <c r="IR80"/>
+      <c r="IS80"/>
+      <c r="IT80"/>
+      <c r="IU80"/>
+      <c r="IV80"/>
     </row>
     <row r="81" ht="12.8">
       <c r="K81" s="1"/>
@@ -32341,254 +32341,254 @@
         <v>472</v>
       </c>
       <c r="J105" s="1"/>
-      <c r="K105" s="1" t="s">
+      <c r="K105" t="s">
         <v>684</v>
       </c>
-      <c r="L105" s="1"/>
-      <c r="M105" s="1"/>
-      <c r="N105" s="1"/>
-      <c r="O105" s="1"/>
-      <c r="P105" s="1"/>
-      <c r="Q105" s="1"/>
-      <c r="R105" s="1"/>
-      <c r="S105" s="1"/>
-      <c r="T105" s="1"/>
-      <c r="U105" s="1"/>
-      <c r="V105" s="1"/>
-      <c r="W105" s="1"/>
-      <c r="X105" s="1"/>
-      <c r="Y105" s="1"/>
-      <c r="Z105" s="1"/>
-      <c r="AA105" s="1"/>
-      <c r="AB105" s="1"/>
-      <c r="AC105" s="1"/>
-      <c r="AD105" s="1"/>
-      <c r="AE105" s="1"/>
-      <c r="AF105" s="1"/>
-      <c r="AG105" s="1"/>
-      <c r="AH105" s="1"/>
-      <c r="AI105" s="1"/>
-      <c r="AJ105" s="1"/>
-      <c r="AK105" s="1"/>
-      <c r="AL105" s="1"/>
-      <c r="AM105" s="1"/>
-      <c r="AN105" s="1"/>
-      <c r="AO105" s="1"/>
-      <c r="AP105" s="1"/>
-      <c r="AQ105" s="1"/>
-      <c r="AR105" s="1"/>
-      <c r="AS105" s="1"/>
-      <c r="AT105" s="1"/>
-      <c r="AU105" s="1"/>
-      <c r="AV105" s="1"/>
-      <c r="AW105" s="1"/>
-      <c r="AX105" s="1"/>
-      <c r="AY105" s="1"/>
-      <c r="AZ105" s="1"/>
-      <c r="BA105" s="1"/>
-      <c r="BB105" s="1"/>
-      <c r="BC105" s="1"/>
-      <c r="BD105" s="1"/>
-      <c r="BE105" s="1"/>
-      <c r="BF105" s="1"/>
-      <c r="BG105" s="1"/>
-      <c r="BH105" s="1"/>
-      <c r="BI105" s="1"/>
-      <c r="BJ105" s="1"/>
-      <c r="BK105" s="1"/>
-      <c r="BL105" s="1"/>
-      <c r="BM105" s="1"/>
-      <c r="BN105" s="1"/>
-      <c r="BO105" s="1"/>
-      <c r="BP105" s="1"/>
-      <c r="BQ105" s="1"/>
-      <c r="BR105" s="1"/>
-      <c r="BS105" s="1"/>
-      <c r="BT105" s="1"/>
-      <c r="BU105" s="1"/>
-      <c r="BV105" s="1"/>
-      <c r="BW105" s="1"/>
-      <c r="BX105" s="1"/>
-      <c r="BY105" s="1"/>
-      <c r="BZ105" s="1"/>
-      <c r="CA105" s="1"/>
-      <c r="CB105" s="1"/>
-      <c r="CC105" s="1"/>
-      <c r="CD105" s="1"/>
-      <c r="CE105" s="1"/>
-      <c r="CF105" s="1"/>
-      <c r="CG105" s="1"/>
-      <c r="CH105" s="1"/>
-      <c r="CI105" s="1"/>
-      <c r="CJ105" s="1"/>
-      <c r="CK105" s="1"/>
-      <c r="CL105" s="1"/>
-      <c r="CM105" s="1"/>
-      <c r="CN105" s="1"/>
-      <c r="CO105" s="1"/>
-      <c r="CP105" s="1"/>
-      <c r="CQ105" s="1"/>
-      <c r="CR105" s="1"/>
-      <c r="CS105" s="1"/>
-      <c r="CT105" s="1"/>
-      <c r="CU105" s="1"/>
-      <c r="CV105" s="1"/>
-      <c r="CW105" s="1"/>
-      <c r="CX105" s="1"/>
-      <c r="CY105" s="1"/>
-      <c r="CZ105" s="1"/>
-      <c r="DA105" s="1"/>
-      <c r="DB105" s="1"/>
-      <c r="DC105" s="1"/>
-      <c r="DD105" s="1"/>
-      <c r="DE105" s="1"/>
-      <c r="DF105" s="1"/>
-      <c r="DG105" s="1"/>
-      <c r="DH105" s="1"/>
-      <c r="DI105" s="1"/>
-      <c r="DJ105" s="1"/>
-      <c r="DK105" s="1"/>
-      <c r="DL105" s="1"/>
-      <c r="DM105" s="1"/>
-      <c r="DN105" s="1"/>
-      <c r="DO105" s="1"/>
-      <c r="DP105" s="1"/>
-      <c r="DQ105" s="1"/>
-      <c r="DR105" s="1"/>
-      <c r="DS105" s="1"/>
-      <c r="DT105" s="1"/>
-      <c r="DU105" s="1"/>
-      <c r="DV105" s="1"/>
-      <c r="DW105" s="1"/>
-      <c r="DX105" s="1"/>
-      <c r="DY105" s="1"/>
-      <c r="DZ105" s="1"/>
-      <c r="EA105" s="1"/>
-      <c r="EB105" s="1"/>
-      <c r="EC105" s="1"/>
-      <c r="ED105" s="1"/>
-      <c r="EE105" s="1"/>
-      <c r="EF105" s="1"/>
-      <c r="EG105" s="1"/>
-      <c r="EH105" s="1"/>
-      <c r="EI105" s="1"/>
-      <c r="EJ105" s="1"/>
-      <c r="EK105" s="1"/>
-      <c r="EL105" s="1"/>
-      <c r="EM105" s="1"/>
-      <c r="EN105" s="1"/>
-      <c r="EO105" s="1"/>
-      <c r="EP105" s="1"/>
-      <c r="EQ105" s="1"/>
-      <c r="ER105" s="1"/>
-      <c r="ES105" s="1"/>
-      <c r="ET105" s="1"/>
-      <c r="EU105" s="1"/>
-      <c r="EV105" s="1"/>
-      <c r="EW105" s="1"/>
-      <c r="EX105" s="1"/>
-      <c r="EY105" s="1"/>
-      <c r="EZ105" s="1"/>
-      <c r="FA105" s="1"/>
-      <c r="FB105" s="1"/>
-      <c r="FC105" s="1"/>
-      <c r="FD105" s="1"/>
-      <c r="FE105" s="1"/>
-      <c r="FF105" s="1"/>
-      <c r="FG105" s="1"/>
-      <c r="FH105" s="1"/>
-      <c r="FI105" s="1"/>
-      <c r="FJ105" s="1"/>
-      <c r="FK105" s="1"/>
-      <c r="FL105" s="1"/>
-      <c r="FM105" s="1"/>
-      <c r="FN105" s="1"/>
-      <c r="FO105" s="1"/>
-      <c r="FP105" s="1"/>
-      <c r="FQ105" s="1"/>
-      <c r="FR105" s="1"/>
-      <c r="FS105" s="1"/>
-      <c r="FT105" s="1"/>
-      <c r="FU105" s="1"/>
-      <c r="FV105" s="1"/>
-      <c r="FW105" s="1"/>
-      <c r="FX105" s="1"/>
-      <c r="FY105" s="1"/>
-      <c r="FZ105" s="1"/>
-      <c r="GA105" s="1"/>
-      <c r="GB105" s="1"/>
-      <c r="GC105" s="1"/>
-      <c r="GD105" s="1"/>
-      <c r="GE105" s="1"/>
-      <c r="GF105" s="1"/>
-      <c r="GG105" s="1"/>
-      <c r="GH105" s="1"/>
-      <c r="GI105" s="1"/>
-      <c r="GJ105" s="1"/>
-      <c r="GK105" s="1"/>
-      <c r="GL105" s="1"/>
-      <c r="GM105" s="1"/>
-      <c r="GN105" s="1"/>
-      <c r="GO105" s="1"/>
-      <c r="GP105" s="1"/>
-      <c r="GQ105" s="1"/>
-      <c r="GR105" s="1"/>
-      <c r="GS105" s="1"/>
-      <c r="GT105" s="1"/>
-      <c r="GU105" s="1"/>
-      <c r="GV105" s="1"/>
-      <c r="GW105" s="1"/>
-      <c r="GX105" s="1"/>
-      <c r="GY105" s="1"/>
-      <c r="GZ105" s="1"/>
-      <c r="HA105" s="1"/>
-      <c r="HB105" s="1"/>
-      <c r="HC105" s="1"/>
-      <c r="HD105" s="1"/>
-      <c r="HE105" s="1"/>
-      <c r="HF105" s="1"/>
-      <c r="HG105" s="1"/>
-      <c r="HH105" s="1"/>
-      <c r="HI105" s="1"/>
-      <c r="HJ105" s="1"/>
-      <c r="HK105" s="1"/>
-      <c r="HL105" s="1"/>
-      <c r="HM105" s="1"/>
-      <c r="HN105" s="1"/>
-      <c r="HO105" s="1"/>
-      <c r="HP105" s="1"/>
-      <c r="HQ105" s="1"/>
-      <c r="HR105" s="1"/>
-      <c r="HS105" s="1"/>
-      <c r="HT105" s="1"/>
-      <c r="HU105" s="1"/>
-      <c r="HV105" s="1"/>
-      <c r="HW105" s="1"/>
-      <c r="HX105" s="1"/>
-      <c r="HY105" s="1"/>
-      <c r="HZ105" s="1"/>
-      <c r="IA105" s="1"/>
-      <c r="IB105" s="1"/>
-      <c r="IC105" s="1"/>
-      <c r="ID105" s="1"/>
-      <c r="IE105" s="1"/>
-      <c r="IF105" s="1"/>
-      <c r="IG105" s="1"/>
-      <c r="IH105" s="1"/>
-      <c r="II105" s="1"/>
-      <c r="IJ105" s="1"/>
-      <c r="IK105" s="1"/>
-      <c r="IL105" s="1"/>
-      <c r="IM105" s="1"/>
-      <c r="IN105" s="1"/>
-      <c r="IO105" s="1"/>
-      <c r="IP105" s="1"/>
-      <c r="IQ105" s="1"/>
-      <c r="IR105" s="1"/>
-      <c r="IS105" s="1"/>
-      <c r="IT105" s="1"/>
-      <c r="IU105" s="1"/>
-      <c r="IV105" s="1"/>
+      <c r="L105"/>
+      <c r="M105"/>
+      <c r="N105"/>
+      <c r="O105"/>
+      <c r="P105"/>
+      <c r="Q105"/>
+      <c r="R105"/>
+      <c r="S105"/>
+      <c r="T105"/>
+      <c r="U105"/>
+      <c r="V105"/>
+      <c r="W105"/>
+      <c r="X105"/>
+      <c r="Y105"/>
+      <c r="Z105"/>
+      <c r="AA105"/>
+      <c r="AB105"/>
+      <c r="AC105"/>
+      <c r="AD105"/>
+      <c r="AE105"/>
+      <c r="AF105"/>
+      <c r="AG105"/>
+      <c r="AH105"/>
+      <c r="AI105"/>
+      <c r="AJ105"/>
+      <c r="AK105"/>
+      <c r="AL105"/>
+      <c r="AM105"/>
+      <c r="AN105"/>
+      <c r="AO105"/>
+      <c r="AP105"/>
+      <c r="AQ105"/>
+      <c r="AR105"/>
+      <c r="AS105"/>
+      <c r="AT105"/>
+      <c r="AU105"/>
+      <c r="AV105"/>
+      <c r="AW105"/>
+      <c r="AX105"/>
+      <c r="AY105"/>
+      <c r="AZ105"/>
+      <c r="BA105"/>
+      <c r="BB105"/>
+      <c r="BC105"/>
+      <c r="BD105"/>
+      <c r="BE105"/>
+      <c r="BF105"/>
+      <c r="BG105"/>
+      <c r="BH105"/>
+      <c r="BI105"/>
+      <c r="BJ105"/>
+      <c r="BK105"/>
+      <c r="BL105"/>
+      <c r="BM105"/>
+      <c r="BN105"/>
+      <c r="BO105"/>
+      <c r="BP105"/>
+      <c r="BQ105"/>
+      <c r="BR105"/>
+      <c r="BS105"/>
+      <c r="BT105"/>
+      <c r="BU105"/>
+      <c r="BV105"/>
+      <c r="BW105"/>
+      <c r="BX105"/>
+      <c r="BY105"/>
+      <c r="BZ105"/>
+      <c r="CA105"/>
+      <c r="CB105"/>
+      <c r="CC105"/>
+      <c r="CD105"/>
+      <c r="CE105"/>
+      <c r="CF105"/>
+      <c r="CG105"/>
+      <c r="CH105"/>
+      <c r="CI105"/>
+      <c r="CJ105"/>
+      <c r="CK105"/>
+      <c r="CL105"/>
+      <c r="CM105"/>
+      <c r="CN105"/>
+      <c r="CO105"/>
+      <c r="CP105"/>
+      <c r="CQ105"/>
+      <c r="CR105"/>
+      <c r="CS105"/>
+      <c r="CT105"/>
+      <c r="CU105"/>
+      <c r="CV105"/>
+      <c r="CW105"/>
+      <c r="CX105"/>
+      <c r="CY105"/>
+      <c r="CZ105"/>
+      <c r="DA105"/>
+      <c r="DB105"/>
+      <c r="DC105"/>
+      <c r="DD105"/>
+      <c r="DE105"/>
+      <c r="DF105"/>
+      <c r="DG105"/>
+      <c r="DH105"/>
+      <c r="DI105"/>
+      <c r="DJ105"/>
+      <c r="DK105"/>
+      <c r="DL105"/>
+      <c r="DM105"/>
+      <c r="DN105"/>
+      <c r="DO105"/>
+      <c r="DP105"/>
+      <c r="DQ105"/>
+      <c r="DR105"/>
+      <c r="DS105"/>
+      <c r="DT105"/>
+      <c r="DU105"/>
+      <c r="DV105"/>
+      <c r="DW105"/>
+      <c r="DX105"/>
+      <c r="DY105"/>
+      <c r="DZ105"/>
+      <c r="EA105"/>
+      <c r="EB105"/>
+      <c r="EC105"/>
+      <c r="ED105"/>
+      <c r="EE105"/>
+      <c r="EF105"/>
+      <c r="EG105"/>
+      <c r="EH105"/>
+      <c r="EI105"/>
+      <c r="EJ105"/>
+      <c r="EK105"/>
+      <c r="EL105"/>
+      <c r="EM105"/>
+      <c r="EN105"/>
+      <c r="EO105"/>
+      <c r="EP105"/>
+      <c r="EQ105"/>
+      <c r="ER105"/>
+      <c r="ES105"/>
+      <c r="ET105"/>
+      <c r="EU105"/>
+      <c r="EV105"/>
+      <c r="EW105"/>
+      <c r="EX105"/>
+      <c r="EY105"/>
+      <c r="EZ105"/>
+      <c r="FA105"/>
+      <c r="FB105"/>
+      <c r="FC105"/>
+      <c r="FD105"/>
+      <c r="FE105"/>
+      <c r="FF105"/>
+      <c r="FG105"/>
+      <c r="FH105"/>
+      <c r="FI105"/>
+      <c r="FJ105"/>
+      <c r="FK105"/>
+      <c r="FL105"/>
+      <c r="FM105"/>
+      <c r="FN105"/>
+      <c r="FO105"/>
+      <c r="FP105"/>
+      <c r="FQ105"/>
+      <c r="FR105"/>
+      <c r="FS105"/>
+      <c r="FT105"/>
+      <c r="FU105"/>
+      <c r="FV105"/>
+      <c r="FW105"/>
+      <c r="FX105"/>
+      <c r="FY105"/>
+      <c r="FZ105"/>
+      <c r="GA105"/>
+      <c r="GB105"/>
+      <c r="GC105"/>
+      <c r="GD105"/>
+      <c r="GE105"/>
+      <c r="GF105"/>
+      <c r="GG105"/>
+      <c r="GH105"/>
+      <c r="GI105"/>
+      <c r="GJ105"/>
+      <c r="GK105"/>
+      <c r="GL105"/>
+      <c r="GM105"/>
+      <c r="GN105"/>
+      <c r="GO105"/>
+      <c r="GP105"/>
+      <c r="GQ105"/>
+      <c r="GR105"/>
+      <c r="GS105"/>
+      <c r="GT105"/>
+      <c r="GU105"/>
+      <c r="GV105"/>
+      <c r="GW105"/>
+      <c r="GX105"/>
+      <c r="GY105"/>
+      <c r="GZ105"/>
+      <c r="HA105"/>
+      <c r="HB105"/>
+      <c r="HC105"/>
+      <c r="HD105"/>
+      <c r="HE105"/>
+      <c r="HF105"/>
+      <c r="HG105"/>
+      <c r="HH105"/>
+      <c r="HI105"/>
+      <c r="HJ105"/>
+      <c r="HK105"/>
+      <c r="HL105"/>
+      <c r="HM105"/>
+      <c r="HN105"/>
+      <c r="HO105"/>
+      <c r="HP105"/>
+      <c r="HQ105"/>
+      <c r="HR105"/>
+      <c r="HS105"/>
+      <c r="HT105"/>
+      <c r="HU105"/>
+      <c r="HV105"/>
+      <c r="HW105"/>
+      <c r="HX105"/>
+      <c r="HY105"/>
+      <c r="HZ105"/>
+      <c r="IA105"/>
+      <c r="IB105"/>
+      <c r="IC105"/>
+      <c r="ID105"/>
+      <c r="IE105"/>
+      <c r="IF105"/>
+      <c r="IG105"/>
+      <c r="IH105"/>
+      <c r="II105"/>
+      <c r="IJ105"/>
+      <c r="IK105"/>
+      <c r="IL105"/>
+      <c r="IM105"/>
+      <c r="IN105"/>
+      <c r="IO105"/>
+      <c r="IP105"/>
+      <c r="IQ105"/>
+      <c r="IR105"/>
+      <c r="IS105"/>
+      <c r="IT105"/>
+      <c r="IU105"/>
+      <c r="IV105"/>
     </row>
     <row r="106" ht="22.35">
       <c r="H106" s="1">
@@ -33582,252 +33582,252 @@
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
       <c r="J135" s="1"/>
-      <c r="K135" s="1"/>
-      <c r="L135" s="1"/>
-      <c r="M135" s="1"/>
-      <c r="N135" s="1"/>
-      <c r="O135" s="1"/>
-      <c r="P135" s="1"/>
-      <c r="Q135" s="1"/>
-      <c r="R135" s="1"/>
-      <c r="S135" s="1"/>
-      <c r="T135" s="1"/>
-      <c r="U135" s="1"/>
-      <c r="V135" s="1"/>
-      <c r="W135" s="1"/>
-      <c r="X135" s="1"/>
-      <c r="Y135" s="1"/>
-      <c r="Z135" s="1"/>
-      <c r="AA135" s="1"/>
-      <c r="AB135" s="1"/>
-      <c r="AC135" s="1"/>
-      <c r="AD135" s="1"/>
-      <c r="AE135" s="1"/>
-      <c r="AF135" s="1"/>
-      <c r="AG135" s="1"/>
-      <c r="AH135" s="1"/>
-      <c r="AI135" s="1"/>
-      <c r="AJ135" s="1"/>
-      <c r="AK135" s="1"/>
-      <c r="AL135" s="1"/>
-      <c r="AM135" s="1"/>
-      <c r="AN135" s="1"/>
-      <c r="AO135" s="1"/>
-      <c r="AP135" s="1"/>
-      <c r="AQ135" s="1"/>
-      <c r="AR135" s="1"/>
-      <c r="AS135" s="1"/>
-      <c r="AT135" s="1"/>
-      <c r="AU135" s="1"/>
-      <c r="AV135" s="1"/>
-      <c r="AW135" s="1"/>
-      <c r="AX135" s="1"/>
-      <c r="AY135" s="1"/>
-      <c r="AZ135" s="1"/>
-      <c r="BA135" s="1"/>
-      <c r="BB135" s="1"/>
-      <c r="BC135" s="1"/>
-      <c r="BD135" s="1"/>
-      <c r="BE135" s="1"/>
-      <c r="BF135" s="1"/>
-      <c r="BG135" s="1"/>
-      <c r="BH135" s="1"/>
-      <c r="BI135" s="1"/>
-      <c r="BJ135" s="1"/>
-      <c r="BK135" s="1"/>
-      <c r="BL135" s="1"/>
-      <c r="BM135" s="1"/>
-      <c r="BN135" s="1"/>
-      <c r="BO135" s="1"/>
-      <c r="BP135" s="1"/>
-      <c r="BQ135" s="1"/>
-      <c r="BR135" s="1"/>
-      <c r="BS135" s="1"/>
-      <c r="BT135" s="1"/>
-      <c r="BU135" s="1"/>
-      <c r="BV135" s="1"/>
-      <c r="BW135" s="1"/>
-      <c r="BX135" s="1"/>
-      <c r="BY135" s="1"/>
-      <c r="BZ135" s="1"/>
-      <c r="CA135" s="1"/>
-      <c r="CB135" s="1"/>
-      <c r="CC135" s="1"/>
-      <c r="CD135" s="1"/>
-      <c r="CE135" s="1"/>
-      <c r="CF135" s="1"/>
-      <c r="CG135" s="1"/>
-      <c r="CH135" s="1"/>
-      <c r="CI135" s="1"/>
-      <c r="CJ135" s="1"/>
-      <c r="CK135" s="1"/>
-      <c r="CL135" s="1"/>
-      <c r="CM135" s="1"/>
-      <c r="CN135" s="1"/>
-      <c r="CO135" s="1"/>
-      <c r="CP135" s="1"/>
-      <c r="CQ135" s="1"/>
-      <c r="CR135" s="1"/>
-      <c r="CS135" s="1"/>
-      <c r="CT135" s="1"/>
-      <c r="CU135" s="1"/>
-      <c r="CV135" s="1"/>
-      <c r="CW135" s="1"/>
-      <c r="CX135" s="1"/>
-      <c r="CY135" s="1"/>
-      <c r="CZ135" s="1"/>
-      <c r="DA135" s="1"/>
-      <c r="DB135" s="1"/>
-      <c r="DC135" s="1"/>
-      <c r="DD135" s="1"/>
-      <c r="DE135" s="1"/>
-      <c r="DF135" s="1"/>
-      <c r="DG135" s="1"/>
-      <c r="DH135" s="1"/>
-      <c r="DI135" s="1"/>
-      <c r="DJ135" s="1"/>
-      <c r="DK135" s="1"/>
-      <c r="DL135" s="1"/>
-      <c r="DM135" s="1"/>
-      <c r="DN135" s="1"/>
-      <c r="DO135" s="1"/>
-      <c r="DP135" s="1"/>
-      <c r="DQ135" s="1"/>
-      <c r="DR135" s="1"/>
-      <c r="DS135" s="1"/>
-      <c r="DT135" s="1"/>
-      <c r="DU135" s="1"/>
-      <c r="DV135" s="1"/>
-      <c r="DW135" s="1"/>
-      <c r="DX135" s="1"/>
-      <c r="DY135" s="1"/>
-      <c r="DZ135" s="1"/>
-      <c r="EA135" s="1"/>
-      <c r="EB135" s="1"/>
-      <c r="EC135" s="1"/>
-      <c r="ED135" s="1"/>
-      <c r="EE135" s="1"/>
-      <c r="EF135" s="1"/>
-      <c r="EG135" s="1"/>
-      <c r="EH135" s="1"/>
-      <c r="EI135" s="1"/>
-      <c r="EJ135" s="1"/>
-      <c r="EK135" s="1"/>
-      <c r="EL135" s="1"/>
-      <c r="EM135" s="1"/>
-      <c r="EN135" s="1"/>
-      <c r="EO135" s="1"/>
-      <c r="EP135" s="1"/>
-      <c r="EQ135" s="1"/>
-      <c r="ER135" s="1"/>
-      <c r="ES135" s="1"/>
-      <c r="ET135" s="1"/>
-      <c r="EU135" s="1"/>
-      <c r="EV135" s="1"/>
-      <c r="EW135" s="1"/>
-      <c r="EX135" s="1"/>
-      <c r="EY135" s="1"/>
-      <c r="EZ135" s="1"/>
-      <c r="FA135" s="1"/>
-      <c r="FB135" s="1"/>
-      <c r="FC135" s="1"/>
-      <c r="FD135" s="1"/>
-      <c r="FE135" s="1"/>
-      <c r="FF135" s="1"/>
-      <c r="FG135" s="1"/>
-      <c r="FH135" s="1"/>
-      <c r="FI135" s="1"/>
-      <c r="FJ135" s="1"/>
-      <c r="FK135" s="1"/>
-      <c r="FL135" s="1"/>
-      <c r="FM135" s="1"/>
-      <c r="FN135" s="1"/>
-      <c r="FO135" s="1"/>
-      <c r="FP135" s="1"/>
-      <c r="FQ135" s="1"/>
-      <c r="FR135" s="1"/>
-      <c r="FS135" s="1"/>
-      <c r="FT135" s="1"/>
-      <c r="FU135" s="1"/>
-      <c r="FV135" s="1"/>
-      <c r="FW135" s="1"/>
-      <c r="FX135" s="1"/>
-      <c r="FY135" s="1"/>
-      <c r="FZ135" s="1"/>
-      <c r="GA135" s="1"/>
-      <c r="GB135" s="1"/>
-      <c r="GC135" s="1"/>
-      <c r="GD135" s="1"/>
-      <c r="GE135" s="1"/>
-      <c r="GF135" s="1"/>
-      <c r="GG135" s="1"/>
-      <c r="GH135" s="1"/>
-      <c r="GI135" s="1"/>
-      <c r="GJ135" s="1"/>
-      <c r="GK135" s="1"/>
-      <c r="GL135" s="1"/>
-      <c r="GM135" s="1"/>
-      <c r="GN135" s="1"/>
-      <c r="GO135" s="1"/>
-      <c r="GP135" s="1"/>
-      <c r="GQ135" s="1"/>
-      <c r="GR135" s="1"/>
-      <c r="GS135" s="1"/>
-      <c r="GT135" s="1"/>
-      <c r="GU135" s="1"/>
-      <c r="GV135" s="1"/>
-      <c r="GW135" s="1"/>
-      <c r="GX135" s="1"/>
-      <c r="GY135" s="1"/>
-      <c r="GZ135" s="1"/>
-      <c r="HA135" s="1"/>
-      <c r="HB135" s="1"/>
-      <c r="HC135" s="1"/>
-      <c r="HD135" s="1"/>
-      <c r="HE135" s="1"/>
-      <c r="HF135" s="1"/>
-      <c r="HG135" s="1"/>
-      <c r="HH135" s="1"/>
-      <c r="HI135" s="1"/>
-      <c r="HJ135" s="1"/>
-      <c r="HK135" s="1"/>
-      <c r="HL135" s="1"/>
-      <c r="HM135" s="1"/>
-      <c r="HN135" s="1"/>
-      <c r="HO135" s="1"/>
-      <c r="HP135" s="1"/>
-      <c r="HQ135" s="1"/>
-      <c r="HR135" s="1"/>
-      <c r="HS135" s="1"/>
-      <c r="HT135" s="1"/>
-      <c r="HU135" s="1"/>
-      <c r="HV135" s="1"/>
-      <c r="HW135" s="1"/>
-      <c r="HX135" s="1"/>
-      <c r="HY135" s="1"/>
-      <c r="HZ135" s="1"/>
-      <c r="IA135" s="1"/>
-      <c r="IB135" s="1"/>
-      <c r="IC135" s="1"/>
-      <c r="ID135" s="1"/>
-      <c r="IE135" s="1"/>
-      <c r="IF135" s="1"/>
-      <c r="IG135" s="1"/>
-      <c r="IH135" s="1"/>
-      <c r="II135" s="1"/>
-      <c r="IJ135" s="1"/>
-      <c r="IK135" s="1"/>
-      <c r="IL135" s="1"/>
-      <c r="IM135" s="1"/>
-      <c r="IN135" s="1"/>
-      <c r="IO135" s="1"/>
-      <c r="IP135" s="1"/>
-      <c r="IQ135" s="1"/>
-      <c r="IR135" s="1"/>
-      <c r="IS135" s="1"/>
-      <c r="IT135" s="1"/>
-      <c r="IU135" s="1"/>
-      <c r="IV135" s="1"/>
+      <c r="K135"/>
+      <c r="L135"/>
+      <c r="M135"/>
+      <c r="N135"/>
+      <c r="O135"/>
+      <c r="P135"/>
+      <c r="Q135"/>
+      <c r="R135"/>
+      <c r="S135"/>
+      <c r="T135"/>
+      <c r="U135"/>
+      <c r="V135"/>
+      <c r="W135"/>
+      <c r="X135"/>
+      <c r="Y135"/>
+      <c r="Z135"/>
+      <c r="AA135"/>
+      <c r="AB135"/>
+      <c r="AC135"/>
+      <c r="AD135"/>
+      <c r="AE135"/>
+      <c r="AF135"/>
+      <c r="AG135"/>
+      <c r="AH135"/>
+      <c r="AI135"/>
+      <c r="AJ135"/>
+      <c r="AK135"/>
+      <c r="AL135"/>
+      <c r="AM135"/>
+      <c r="AN135"/>
+      <c r="AO135"/>
+      <c r="AP135"/>
+      <c r="AQ135"/>
+      <c r="AR135"/>
+      <c r="AS135"/>
+      <c r="AT135"/>
+      <c r="AU135"/>
+      <c r="AV135"/>
+      <c r="AW135"/>
+      <c r="AX135"/>
+      <c r="AY135"/>
+      <c r="AZ135"/>
+      <c r="BA135"/>
+      <c r="BB135"/>
+      <c r="BC135"/>
+      <c r="BD135"/>
+      <c r="BE135"/>
+      <c r="BF135"/>
+      <c r="BG135"/>
+      <c r="BH135"/>
+      <c r="BI135"/>
+      <c r="BJ135"/>
+      <c r="BK135"/>
+      <c r="BL135"/>
+      <c r="BM135"/>
+      <c r="BN135"/>
+      <c r="BO135"/>
+      <c r="BP135"/>
+      <c r="BQ135"/>
+      <c r="BR135"/>
+      <c r="BS135"/>
+      <c r="BT135"/>
+      <c r="BU135"/>
+      <c r="BV135"/>
+      <c r="BW135"/>
+      <c r="BX135"/>
+      <c r="BY135"/>
+      <c r="BZ135"/>
+      <c r="CA135"/>
+      <c r="CB135"/>
+      <c r="CC135"/>
+      <c r="CD135"/>
+      <c r="CE135"/>
+      <c r="CF135"/>
+      <c r="CG135"/>
+      <c r="CH135"/>
+      <c r="CI135"/>
+      <c r="CJ135"/>
+      <c r="CK135"/>
+      <c r="CL135"/>
+      <c r="CM135"/>
+      <c r="CN135"/>
+      <c r="CO135"/>
+      <c r="CP135"/>
+      <c r="CQ135"/>
+      <c r="CR135"/>
+      <c r="CS135"/>
+      <c r="CT135"/>
+      <c r="CU135"/>
+      <c r="CV135"/>
+      <c r="CW135"/>
+      <c r="CX135"/>
+      <c r="CY135"/>
+      <c r="CZ135"/>
+      <c r="DA135"/>
+      <c r="DB135"/>
+      <c r="DC135"/>
+      <c r="DD135"/>
+      <c r="DE135"/>
+      <c r="DF135"/>
+      <c r="DG135"/>
+      <c r="DH135"/>
+      <c r="DI135"/>
+      <c r="DJ135"/>
+      <c r="DK135"/>
+      <c r="DL135"/>
+      <c r="DM135"/>
+      <c r="DN135"/>
+      <c r="DO135"/>
+      <c r="DP135"/>
+      <c r="DQ135"/>
+      <c r="DR135"/>
+      <c r="DS135"/>
+      <c r="DT135"/>
+      <c r="DU135"/>
+      <c r="DV135"/>
+      <c r="DW135"/>
+      <c r="DX135"/>
+      <c r="DY135"/>
+      <c r="DZ135"/>
+      <c r="EA135"/>
+      <c r="EB135"/>
+      <c r="EC135"/>
+      <c r="ED135"/>
+      <c r="EE135"/>
+      <c r="EF135"/>
+      <c r="EG135"/>
+      <c r="EH135"/>
+      <c r="EI135"/>
+      <c r="EJ135"/>
+      <c r="EK135"/>
+      <c r="EL135"/>
+      <c r="EM135"/>
+      <c r="EN135"/>
+      <c r="EO135"/>
+      <c r="EP135"/>
+      <c r="EQ135"/>
+      <c r="ER135"/>
+      <c r="ES135"/>
+      <c r="ET135"/>
+      <c r="EU135"/>
+      <c r="EV135"/>
+      <c r="EW135"/>
+      <c r="EX135"/>
+      <c r="EY135"/>
+      <c r="EZ135"/>
+      <c r="FA135"/>
+      <c r="FB135"/>
+      <c r="FC135"/>
+      <c r="FD135"/>
+      <c r="FE135"/>
+      <c r="FF135"/>
+      <c r="FG135"/>
+      <c r="FH135"/>
+      <c r="FI135"/>
+      <c r="FJ135"/>
+      <c r="FK135"/>
+      <c r="FL135"/>
+      <c r="FM135"/>
+      <c r="FN135"/>
+      <c r="FO135"/>
+      <c r="FP135"/>
+      <c r="FQ135"/>
+      <c r="FR135"/>
+      <c r="FS135"/>
+      <c r="FT135"/>
+      <c r="FU135"/>
+      <c r="FV135"/>
+      <c r="FW135"/>
+      <c r="FX135"/>
+      <c r="FY135"/>
+      <c r="FZ135"/>
+      <c r="GA135"/>
+      <c r="GB135"/>
+      <c r="GC135"/>
+      <c r="GD135"/>
+      <c r="GE135"/>
+      <c r="GF135"/>
+      <c r="GG135"/>
+      <c r="GH135"/>
+      <c r="GI135"/>
+      <c r="GJ135"/>
+      <c r="GK135"/>
+      <c r="GL135"/>
+      <c r="GM135"/>
+      <c r="GN135"/>
+      <c r="GO135"/>
+      <c r="GP135"/>
+      <c r="GQ135"/>
+      <c r="GR135"/>
+      <c r="GS135"/>
+      <c r="GT135"/>
+      <c r="GU135"/>
+      <c r="GV135"/>
+      <c r="GW135"/>
+      <c r="GX135"/>
+      <c r="GY135"/>
+      <c r="GZ135"/>
+      <c r="HA135"/>
+      <c r="HB135"/>
+      <c r="HC135"/>
+      <c r="HD135"/>
+      <c r="HE135"/>
+      <c r="HF135"/>
+      <c r="HG135"/>
+      <c r="HH135"/>
+      <c r="HI135"/>
+      <c r="HJ135"/>
+      <c r="HK135"/>
+      <c r="HL135"/>
+      <c r="HM135"/>
+      <c r="HN135"/>
+      <c r="HO135"/>
+      <c r="HP135"/>
+      <c r="HQ135"/>
+      <c r="HR135"/>
+      <c r="HS135"/>
+      <c r="HT135"/>
+      <c r="HU135"/>
+      <c r="HV135"/>
+      <c r="HW135"/>
+      <c r="HX135"/>
+      <c r="HY135"/>
+      <c r="HZ135"/>
+      <c r="IA135"/>
+      <c r="IB135"/>
+      <c r="IC135"/>
+      <c r="ID135"/>
+      <c r="IE135"/>
+      <c r="IF135"/>
+      <c r="IG135"/>
+      <c r="IH135"/>
+      <c r="II135"/>
+      <c r="IJ135"/>
+      <c r="IK135"/>
+      <c r="IL135"/>
+      <c r="IM135"/>
+      <c r="IN135"/>
+      <c r="IO135"/>
+      <c r="IP135"/>
+      <c r="IQ135"/>
+      <c r="IR135"/>
+      <c r="IS135"/>
+      <c r="IT135"/>
+      <c r="IU135"/>
+      <c r="IV135"/>
     </row>
     <row r="136" ht="12.8">
       <c r="K136" s="1"/>
@@ -34877,252 +34877,252 @@
       <c r="H150" s="1"/>
       <c r="I150" s="1"/>
       <c r="J150" s="1"/>
-      <c r="K150" s="1"/>
-      <c r="L150" s="1"/>
-      <c r="M150" s="1"/>
-      <c r="N150" s="1"/>
-      <c r="O150" s="1"/>
-      <c r="P150" s="1"/>
-      <c r="Q150" s="1"/>
-      <c r="R150" s="1"/>
-      <c r="S150" s="1"/>
-      <c r="T150" s="1"/>
-      <c r="U150" s="1"/>
-      <c r="V150" s="1"/>
-      <c r="W150" s="1"/>
-      <c r="X150" s="1"/>
-      <c r="Y150" s="1"/>
-      <c r="Z150" s="1"/>
-      <c r="AA150" s="1"/>
-      <c r="AB150" s="1"/>
-      <c r="AC150" s="1"/>
-      <c r="AD150" s="1"/>
-      <c r="AE150" s="1"/>
-      <c r="AF150" s="1"/>
-      <c r="AG150" s="1"/>
-      <c r="AH150" s="1"/>
-      <c r="AI150" s="1"/>
-      <c r="AJ150" s="1"/>
-      <c r="AK150" s="1"/>
-      <c r="AL150" s="1"/>
-      <c r="AM150" s="1"/>
-      <c r="AN150" s="1"/>
-      <c r="AO150" s="1"/>
-      <c r="AP150" s="1"/>
-      <c r="AQ150" s="1"/>
-      <c r="AR150" s="1"/>
-      <c r="AS150" s="1"/>
-      <c r="AT150" s="1"/>
-      <c r="AU150" s="1"/>
-      <c r="AV150" s="1"/>
-      <c r="AW150" s="1"/>
-      <c r="AX150" s="1"/>
-      <c r="AY150" s="1"/>
-      <c r="AZ150" s="1"/>
-      <c r="BA150" s="1"/>
-      <c r="BB150" s="1"/>
-      <c r="BC150" s="1"/>
-      <c r="BD150" s="1"/>
-      <c r="BE150" s="1"/>
-      <c r="BF150" s="1"/>
-      <c r="BG150" s="1"/>
-      <c r="BH150" s="1"/>
-      <c r="BI150" s="1"/>
-      <c r="BJ150" s="1"/>
-      <c r="BK150" s="1"/>
-      <c r="BL150" s="1"/>
-      <c r="BM150" s="1"/>
-      <c r="BN150" s="1"/>
-      <c r="BO150" s="1"/>
-      <c r="BP150" s="1"/>
-      <c r="BQ150" s="1"/>
-      <c r="BR150" s="1"/>
-      <c r="BS150" s="1"/>
-      <c r="BT150" s="1"/>
-      <c r="BU150" s="1"/>
-      <c r="BV150" s="1"/>
-      <c r="BW150" s="1"/>
-      <c r="BX150" s="1"/>
-      <c r="BY150" s="1"/>
-      <c r="BZ150" s="1"/>
-      <c r="CA150" s="1"/>
-      <c r="CB150" s="1"/>
-      <c r="CC150" s="1"/>
-      <c r="CD150" s="1"/>
-      <c r="CE150" s="1"/>
-      <c r="CF150" s="1"/>
-      <c r="CG150" s="1"/>
-      <c r="CH150" s="1"/>
-      <c r="CI150" s="1"/>
-      <c r="CJ150" s="1"/>
-      <c r="CK150" s="1"/>
-      <c r="CL150" s="1"/>
-      <c r="CM150" s="1"/>
-      <c r="CN150" s="1"/>
-      <c r="CO150" s="1"/>
-      <c r="CP150" s="1"/>
-      <c r="CQ150" s="1"/>
-      <c r="CR150" s="1"/>
-      <c r="CS150" s="1"/>
-      <c r="CT150" s="1"/>
-      <c r="CU150" s="1"/>
-      <c r="CV150" s="1"/>
-      <c r="CW150" s="1"/>
-      <c r="CX150" s="1"/>
-      <c r="CY150" s="1"/>
-      <c r="CZ150" s="1"/>
-      <c r="DA150" s="1"/>
-      <c r="DB150" s="1"/>
-      <c r="DC150" s="1"/>
-      <c r="DD150" s="1"/>
-      <c r="DE150" s="1"/>
-      <c r="DF150" s="1"/>
-      <c r="DG150" s="1"/>
-      <c r="DH150" s="1"/>
-      <c r="DI150" s="1"/>
-      <c r="DJ150" s="1"/>
-      <c r="DK150" s="1"/>
-      <c r="DL150" s="1"/>
-      <c r="DM150" s="1"/>
-      <c r="DN150" s="1"/>
-      <c r="DO150" s="1"/>
-      <c r="DP150" s="1"/>
-      <c r="DQ150" s="1"/>
-      <c r="DR150" s="1"/>
-      <c r="DS150" s="1"/>
-      <c r="DT150" s="1"/>
-      <c r="DU150" s="1"/>
-      <c r="DV150" s="1"/>
-      <c r="DW150" s="1"/>
-      <c r="DX150" s="1"/>
-      <c r="DY150" s="1"/>
-      <c r="DZ150" s="1"/>
-      <c r="EA150" s="1"/>
-      <c r="EB150" s="1"/>
-      <c r="EC150" s="1"/>
-      <c r="ED150" s="1"/>
-      <c r="EE150" s="1"/>
-      <c r="EF150" s="1"/>
-      <c r="EG150" s="1"/>
-      <c r="EH150" s="1"/>
-      <c r="EI150" s="1"/>
-      <c r="EJ150" s="1"/>
-      <c r="EK150" s="1"/>
-      <c r="EL150" s="1"/>
-      <c r="EM150" s="1"/>
-      <c r="EN150" s="1"/>
-      <c r="EO150" s="1"/>
-      <c r="EP150" s="1"/>
-      <c r="EQ150" s="1"/>
-      <c r="ER150" s="1"/>
-      <c r="ES150" s="1"/>
-      <c r="ET150" s="1"/>
-      <c r="EU150" s="1"/>
-      <c r="EV150" s="1"/>
-      <c r="EW150" s="1"/>
-      <c r="EX150" s="1"/>
-      <c r="EY150" s="1"/>
-      <c r="EZ150" s="1"/>
-      <c r="FA150" s="1"/>
-      <c r="FB150" s="1"/>
-      <c r="FC150" s="1"/>
-      <c r="FD150" s="1"/>
-      <c r="FE150" s="1"/>
-      <c r="FF150" s="1"/>
-      <c r="FG150" s="1"/>
-      <c r="FH150" s="1"/>
-      <c r="FI150" s="1"/>
-      <c r="FJ150" s="1"/>
-      <c r="FK150" s="1"/>
-      <c r="FL150" s="1"/>
-      <c r="FM150" s="1"/>
-      <c r="FN150" s="1"/>
-      <c r="FO150" s="1"/>
-      <c r="FP150" s="1"/>
-      <c r="FQ150" s="1"/>
-      <c r="FR150" s="1"/>
-      <c r="FS150" s="1"/>
-      <c r="FT150" s="1"/>
-      <c r="FU150" s="1"/>
-      <c r="FV150" s="1"/>
-      <c r="FW150" s="1"/>
-      <c r="FX150" s="1"/>
-      <c r="FY150" s="1"/>
-      <c r="FZ150" s="1"/>
-      <c r="GA150" s="1"/>
-      <c r="GB150" s="1"/>
-      <c r="GC150" s="1"/>
-      <c r="GD150" s="1"/>
-      <c r="GE150" s="1"/>
-      <c r="GF150" s="1"/>
-      <c r="GG150" s="1"/>
-      <c r="GH150" s="1"/>
-      <c r="GI150" s="1"/>
-      <c r="GJ150" s="1"/>
-      <c r="GK150" s="1"/>
-      <c r="GL150" s="1"/>
-      <c r="GM150" s="1"/>
-      <c r="GN150" s="1"/>
-      <c r="GO150" s="1"/>
-      <c r="GP150" s="1"/>
-      <c r="GQ150" s="1"/>
-      <c r="GR150" s="1"/>
-      <c r="GS150" s="1"/>
-      <c r="GT150" s="1"/>
-      <c r="GU150" s="1"/>
-      <c r="GV150" s="1"/>
-      <c r="GW150" s="1"/>
-      <c r="GX150" s="1"/>
-      <c r="GY150" s="1"/>
-      <c r="GZ150" s="1"/>
-      <c r="HA150" s="1"/>
-      <c r="HB150" s="1"/>
-      <c r="HC150" s="1"/>
-      <c r="HD150" s="1"/>
-      <c r="HE150" s="1"/>
-      <c r="HF150" s="1"/>
-      <c r="HG150" s="1"/>
-      <c r="HH150" s="1"/>
-      <c r="HI150" s="1"/>
-      <c r="HJ150" s="1"/>
-      <c r="HK150" s="1"/>
-      <c r="HL150" s="1"/>
-      <c r="HM150" s="1"/>
-      <c r="HN150" s="1"/>
-      <c r="HO150" s="1"/>
-      <c r="HP150" s="1"/>
-      <c r="HQ150" s="1"/>
-      <c r="HR150" s="1"/>
-      <c r="HS150" s="1"/>
-      <c r="HT150" s="1"/>
-      <c r="HU150" s="1"/>
-      <c r="HV150" s="1"/>
-      <c r="HW150" s="1"/>
-      <c r="HX150" s="1"/>
-      <c r="HY150" s="1"/>
-      <c r="HZ150" s="1"/>
-      <c r="IA150" s="1"/>
-      <c r="IB150" s="1"/>
-      <c r="IC150" s="1"/>
-      <c r="ID150" s="1"/>
-      <c r="IE150" s="1"/>
-      <c r="IF150" s="1"/>
-      <c r="IG150" s="1"/>
-      <c r="IH150" s="1"/>
-      <c r="II150" s="1"/>
-      <c r="IJ150" s="1"/>
-      <c r="IK150" s="1"/>
-      <c r="IL150" s="1"/>
-      <c r="IM150" s="1"/>
-      <c r="IN150" s="1"/>
-      <c r="IO150" s="1"/>
-      <c r="IP150" s="1"/>
-      <c r="IQ150" s="1"/>
-      <c r="IR150" s="1"/>
-      <c r="IS150" s="1"/>
-      <c r="IT150" s="1"/>
-      <c r="IU150" s="1"/>
-      <c r="IV150" s="1"/>
+      <c r="K150"/>
+      <c r="L150"/>
+      <c r="M150"/>
+      <c r="N150"/>
+      <c r="O150"/>
+      <c r="P150"/>
+      <c r="Q150"/>
+      <c r="R150"/>
+      <c r="S150"/>
+      <c r="T150"/>
+      <c r="U150"/>
+      <c r="V150"/>
+      <c r="W150"/>
+      <c r="X150"/>
+      <c r="Y150"/>
+      <c r="Z150"/>
+      <c r="AA150"/>
+      <c r="AB150"/>
+      <c r="AC150"/>
+      <c r="AD150"/>
+      <c r="AE150"/>
+      <c r="AF150"/>
+      <c r="AG150"/>
+      <c r="AH150"/>
+      <c r="AI150"/>
+      <c r="AJ150"/>
+      <c r="AK150"/>
+      <c r="AL150"/>
+      <c r="AM150"/>
+      <c r="AN150"/>
+      <c r="AO150"/>
+      <c r="AP150"/>
+      <c r="AQ150"/>
+      <c r="AR150"/>
+      <c r="AS150"/>
+      <c r="AT150"/>
+      <c r="AU150"/>
+      <c r="AV150"/>
+      <c r="AW150"/>
+      <c r="AX150"/>
+      <c r="AY150"/>
+      <c r="AZ150"/>
+      <c r="BA150"/>
+      <c r="BB150"/>
+      <c r="BC150"/>
+      <c r="BD150"/>
+      <c r="BE150"/>
+      <c r="BF150"/>
+      <c r="BG150"/>
+      <c r="BH150"/>
+      <c r="BI150"/>
+      <c r="BJ150"/>
+      <c r="BK150"/>
+      <c r="BL150"/>
+      <c r="BM150"/>
+      <c r="BN150"/>
+      <c r="BO150"/>
+      <c r="BP150"/>
+      <c r="BQ150"/>
+      <c r="BR150"/>
+      <c r="BS150"/>
+      <c r="BT150"/>
+      <c r="BU150"/>
+      <c r="BV150"/>
+      <c r="BW150"/>
+      <c r="BX150"/>
+      <c r="BY150"/>
+      <c r="BZ150"/>
+      <c r="CA150"/>
+      <c r="CB150"/>
+      <c r="CC150"/>
+      <c r="CD150"/>
+      <c r="CE150"/>
+      <c r="CF150"/>
+      <c r="CG150"/>
+      <c r="CH150"/>
+      <c r="CI150"/>
+      <c r="CJ150"/>
+      <c r="CK150"/>
+      <c r="CL150"/>
+      <c r="CM150"/>
+      <c r="CN150"/>
+      <c r="CO150"/>
+      <c r="CP150"/>
+      <c r="CQ150"/>
+      <c r="CR150"/>
+      <c r="CS150"/>
+      <c r="CT150"/>
+      <c r="CU150"/>
+      <c r="CV150"/>
+      <c r="CW150"/>
+      <c r="CX150"/>
+      <c r="CY150"/>
+      <c r="CZ150"/>
+      <c r="DA150"/>
+      <c r="DB150"/>
+      <c r="DC150"/>
+      <c r="DD150"/>
+      <c r="DE150"/>
+      <c r="DF150"/>
+      <c r="DG150"/>
+      <c r="DH150"/>
+      <c r="DI150"/>
+      <c r="DJ150"/>
+      <c r="DK150"/>
+      <c r="DL150"/>
+      <c r="DM150"/>
+      <c r="DN150"/>
+      <c r="DO150"/>
+      <c r="DP150"/>
+      <c r="DQ150"/>
+      <c r="DR150"/>
+      <c r="DS150"/>
+      <c r="DT150"/>
+      <c r="DU150"/>
+      <c r="DV150"/>
+      <c r="DW150"/>
+      <c r="DX150"/>
+      <c r="DY150"/>
+      <c r="DZ150"/>
+      <c r="EA150"/>
+      <c r="EB150"/>
+      <c r="EC150"/>
+      <c r="ED150"/>
+      <c r="EE150"/>
+      <c r="EF150"/>
+      <c r="EG150"/>
+      <c r="EH150"/>
+      <c r="EI150"/>
+      <c r="EJ150"/>
+      <c r="EK150"/>
+      <c r="EL150"/>
+      <c r="EM150"/>
+      <c r="EN150"/>
+      <c r="EO150"/>
+      <c r="EP150"/>
+      <c r="EQ150"/>
+      <c r="ER150"/>
+      <c r="ES150"/>
+      <c r="ET150"/>
+      <c r="EU150"/>
+      <c r="EV150"/>
+      <c r="EW150"/>
+      <c r="EX150"/>
+      <c r="EY150"/>
+      <c r="EZ150"/>
+      <c r="FA150"/>
+      <c r="FB150"/>
+      <c r="FC150"/>
+      <c r="FD150"/>
+      <c r="FE150"/>
+      <c r="FF150"/>
+      <c r="FG150"/>
+      <c r="FH150"/>
+      <c r="FI150"/>
+      <c r="FJ150"/>
+      <c r="FK150"/>
+      <c r="FL150"/>
+      <c r="FM150"/>
+      <c r="FN150"/>
+      <c r="FO150"/>
+      <c r="FP150"/>
+      <c r="FQ150"/>
+      <c r="FR150"/>
+      <c r="FS150"/>
+      <c r="FT150"/>
+      <c r="FU150"/>
+      <c r="FV150"/>
+      <c r="FW150"/>
+      <c r="FX150"/>
+      <c r="FY150"/>
+      <c r="FZ150"/>
+      <c r="GA150"/>
+      <c r="GB150"/>
+      <c r="GC150"/>
+      <c r="GD150"/>
+      <c r="GE150"/>
+      <c r="GF150"/>
+      <c r="GG150"/>
+      <c r="GH150"/>
+      <c r="GI150"/>
+      <c r="GJ150"/>
+      <c r="GK150"/>
+      <c r="GL150"/>
+      <c r="GM150"/>
+      <c r="GN150"/>
+      <c r="GO150"/>
+      <c r="GP150"/>
+      <c r="GQ150"/>
+      <c r="GR150"/>
+      <c r="GS150"/>
+      <c r="GT150"/>
+      <c r="GU150"/>
+      <c r="GV150"/>
+      <c r="GW150"/>
+      <c r="GX150"/>
+      <c r="GY150"/>
+      <c r="GZ150"/>
+      <c r="HA150"/>
+      <c r="HB150"/>
+      <c r="HC150"/>
+      <c r="HD150"/>
+      <c r="HE150"/>
+      <c r="HF150"/>
+      <c r="HG150"/>
+      <c r="HH150"/>
+      <c r="HI150"/>
+      <c r="HJ150"/>
+      <c r="HK150"/>
+      <c r="HL150"/>
+      <c r="HM150"/>
+      <c r="HN150"/>
+      <c r="HO150"/>
+      <c r="HP150"/>
+      <c r="HQ150"/>
+      <c r="HR150"/>
+      <c r="HS150"/>
+      <c r="HT150"/>
+      <c r="HU150"/>
+      <c r="HV150"/>
+      <c r="HW150"/>
+      <c r="HX150"/>
+      <c r="HY150"/>
+      <c r="HZ150"/>
+      <c r="IA150"/>
+      <c r="IB150"/>
+      <c r="IC150"/>
+      <c r="ID150"/>
+      <c r="IE150"/>
+      <c r="IF150"/>
+      <c r="IG150"/>
+      <c r="IH150"/>
+      <c r="II150"/>
+      <c r="IJ150"/>
+      <c r="IK150"/>
+      <c r="IL150"/>
+      <c r="IM150"/>
+      <c r="IN150"/>
+      <c r="IO150"/>
+      <c r="IP150"/>
+      <c r="IQ150"/>
+      <c r="IR150"/>
+      <c r="IS150"/>
+      <c r="IT150"/>
+      <c r="IU150"/>
+      <c r="IV150"/>
     </row>
     <row r="151" ht="12.8">
       <c r="K151" s="1"/>
@@ -35631,252 +35631,252 @@
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
       <c r="J157" s="1"/>
-      <c r="K157" s="1"/>
-      <c r="L157" s="1"/>
-      <c r="M157" s="1"/>
-      <c r="N157" s="1"/>
-      <c r="O157" s="1"/>
-      <c r="P157" s="1"/>
-      <c r="Q157" s="1"/>
-      <c r="R157" s="1"/>
-      <c r="S157" s="1"/>
-      <c r="T157" s="1"/>
-      <c r="U157" s="1"/>
-      <c r="V157" s="1"/>
-      <c r="W157" s="1"/>
-      <c r="X157" s="1"/>
-      <c r="Y157" s="1"/>
-      <c r="Z157" s="1"/>
-      <c r="AA157" s="1"/>
-      <c r="AB157" s="1"/>
-      <c r="AC157" s="1"/>
-      <c r="AD157" s="1"/>
-      <c r="AE157" s="1"/>
-      <c r="AF157" s="1"/>
-      <c r="AG157" s="1"/>
-      <c r="AH157" s="1"/>
-      <c r="AI157" s="1"/>
-      <c r="AJ157" s="1"/>
-      <c r="AK157" s="1"/>
-      <c r="AL157" s="1"/>
-      <c r="AM157" s="1"/>
-      <c r="AN157" s="1"/>
-      <c r="AO157" s="1"/>
-      <c r="AP157" s="1"/>
-      <c r="AQ157" s="1"/>
-      <c r="AR157" s="1"/>
-      <c r="AS157" s="1"/>
-      <c r="AT157" s="1"/>
-      <c r="AU157" s="1"/>
-      <c r="AV157" s="1"/>
-      <c r="AW157" s="1"/>
-      <c r="AX157" s="1"/>
-      <c r="AY157" s="1"/>
-      <c r="AZ157" s="1"/>
-      <c r="BA157" s="1"/>
-      <c r="BB157" s="1"/>
-      <c r="BC157" s="1"/>
-      <c r="BD157" s="1"/>
-      <c r="BE157" s="1"/>
-      <c r="BF157" s="1"/>
-      <c r="BG157" s="1"/>
-      <c r="BH157" s="1"/>
-      <c r="BI157" s="1"/>
-      <c r="BJ157" s="1"/>
-      <c r="BK157" s="1"/>
-      <c r="BL157" s="1"/>
-      <c r="BM157" s="1"/>
-      <c r="BN157" s="1"/>
-      <c r="BO157" s="1"/>
-      <c r="BP157" s="1"/>
-      <c r="BQ157" s="1"/>
-      <c r="BR157" s="1"/>
-      <c r="BS157" s="1"/>
-      <c r="BT157" s="1"/>
-      <c r="BU157" s="1"/>
-      <c r="BV157" s="1"/>
-      <c r="BW157" s="1"/>
-      <c r="BX157" s="1"/>
-      <c r="BY157" s="1"/>
-      <c r="BZ157" s="1"/>
-      <c r="CA157" s="1"/>
-      <c r="CB157" s="1"/>
-      <c r="CC157" s="1"/>
-      <c r="CD157" s="1"/>
-      <c r="CE157" s="1"/>
-      <c r="CF157" s="1"/>
-      <c r="CG157" s="1"/>
-      <c r="CH157" s="1"/>
-      <c r="CI157" s="1"/>
-      <c r="CJ157" s="1"/>
-      <c r="CK157" s="1"/>
-      <c r="CL157" s="1"/>
-      <c r="CM157" s="1"/>
-      <c r="CN157" s="1"/>
-      <c r="CO157" s="1"/>
-      <c r="CP157" s="1"/>
-      <c r="CQ157" s="1"/>
-      <c r="CR157" s="1"/>
-      <c r="CS157" s="1"/>
-      <c r="CT157" s="1"/>
-      <c r="CU157" s="1"/>
-      <c r="CV157" s="1"/>
-      <c r="CW157" s="1"/>
-      <c r="CX157" s="1"/>
-      <c r="CY157" s="1"/>
-      <c r="CZ157" s="1"/>
-      <c r="DA157" s="1"/>
-      <c r="DB157" s="1"/>
-      <c r="DC157" s="1"/>
-      <c r="DD157" s="1"/>
-      <c r="DE157" s="1"/>
-      <c r="DF157" s="1"/>
-      <c r="DG157" s="1"/>
-      <c r="DH157" s="1"/>
-      <c r="DI157" s="1"/>
-      <c r="DJ157" s="1"/>
-      <c r="DK157" s="1"/>
-      <c r="DL157" s="1"/>
-      <c r="DM157" s="1"/>
-      <c r="DN157" s="1"/>
-      <c r="DO157" s="1"/>
-      <c r="DP157" s="1"/>
-      <c r="DQ157" s="1"/>
-      <c r="DR157" s="1"/>
-      <c r="DS157" s="1"/>
-      <c r="DT157" s="1"/>
-      <c r="DU157" s="1"/>
-      <c r="DV157" s="1"/>
-      <c r="DW157" s="1"/>
-      <c r="DX157" s="1"/>
-      <c r="DY157" s="1"/>
-      <c r="DZ157" s="1"/>
-      <c r="EA157" s="1"/>
-      <c r="EB157" s="1"/>
-      <c r="EC157" s="1"/>
-      <c r="ED157" s="1"/>
-      <c r="EE157" s="1"/>
-      <c r="EF157" s="1"/>
-      <c r="EG157" s="1"/>
-      <c r="EH157" s="1"/>
-      <c r="EI157" s="1"/>
-      <c r="EJ157" s="1"/>
-      <c r="EK157" s="1"/>
-      <c r="EL157" s="1"/>
-      <c r="EM157" s="1"/>
-      <c r="EN157" s="1"/>
-      <c r="EO157" s="1"/>
-      <c r="EP157" s="1"/>
-      <c r="EQ157" s="1"/>
-      <c r="ER157" s="1"/>
-      <c r="ES157" s="1"/>
-      <c r="ET157" s="1"/>
-      <c r="EU157" s="1"/>
-      <c r="EV157" s="1"/>
-      <c r="EW157" s="1"/>
-      <c r="EX157" s="1"/>
-      <c r="EY157" s="1"/>
-      <c r="EZ157" s="1"/>
-      <c r="FA157" s="1"/>
-      <c r="FB157" s="1"/>
-      <c r="FC157" s="1"/>
-      <c r="FD157" s="1"/>
-      <c r="FE157" s="1"/>
-      <c r="FF157" s="1"/>
-      <c r="FG157" s="1"/>
-      <c r="FH157" s="1"/>
-      <c r="FI157" s="1"/>
-      <c r="FJ157" s="1"/>
-      <c r="FK157" s="1"/>
-      <c r="FL157" s="1"/>
-      <c r="FM157" s="1"/>
-      <c r="FN157" s="1"/>
-      <c r="FO157" s="1"/>
-      <c r="FP157" s="1"/>
-      <c r="FQ157" s="1"/>
-      <c r="FR157" s="1"/>
-      <c r="FS157" s="1"/>
-      <c r="FT157" s="1"/>
-      <c r="FU157" s="1"/>
-      <c r="FV157" s="1"/>
-      <c r="FW157" s="1"/>
-      <c r="FX157" s="1"/>
-      <c r="FY157" s="1"/>
-      <c r="FZ157" s="1"/>
-      <c r="GA157" s="1"/>
-      <c r="GB157" s="1"/>
-      <c r="GC157" s="1"/>
-      <c r="GD157" s="1"/>
-      <c r="GE157" s="1"/>
-      <c r="GF157" s="1"/>
-      <c r="GG157" s="1"/>
-      <c r="GH157" s="1"/>
-      <c r="GI157" s="1"/>
-      <c r="GJ157" s="1"/>
-      <c r="GK157" s="1"/>
-      <c r="GL157" s="1"/>
-      <c r="GM157" s="1"/>
-      <c r="GN157" s="1"/>
-      <c r="GO157" s="1"/>
-      <c r="GP157" s="1"/>
-      <c r="GQ157" s="1"/>
-      <c r="GR157" s="1"/>
-      <c r="GS157" s="1"/>
-      <c r="GT157" s="1"/>
-      <c r="GU157" s="1"/>
-      <c r="GV157" s="1"/>
-      <c r="GW157" s="1"/>
-      <c r="GX157" s="1"/>
-      <c r="GY157" s="1"/>
-      <c r="GZ157" s="1"/>
-      <c r="HA157" s="1"/>
-      <c r="HB157" s="1"/>
-      <c r="HC157" s="1"/>
-      <c r="HD157" s="1"/>
-      <c r="HE157" s="1"/>
-      <c r="HF157" s="1"/>
-      <c r="HG157" s="1"/>
-      <c r="HH157" s="1"/>
-      <c r="HI157" s="1"/>
-      <c r="HJ157" s="1"/>
-      <c r="HK157" s="1"/>
-      <c r="HL157" s="1"/>
-      <c r="HM157" s="1"/>
-      <c r="HN157" s="1"/>
-      <c r="HO157" s="1"/>
-      <c r="HP157" s="1"/>
-      <c r="HQ157" s="1"/>
-      <c r="HR157" s="1"/>
-      <c r="HS157" s="1"/>
-      <c r="HT157" s="1"/>
-      <c r="HU157" s="1"/>
-      <c r="HV157" s="1"/>
-      <c r="HW157" s="1"/>
-      <c r="HX157" s="1"/>
-      <c r="HY157" s="1"/>
-      <c r="HZ157" s="1"/>
-      <c r="IA157" s="1"/>
-      <c r="IB157" s="1"/>
-      <c r="IC157" s="1"/>
-      <c r="ID157" s="1"/>
-      <c r="IE157" s="1"/>
-      <c r="IF157" s="1"/>
-      <c r="IG157" s="1"/>
-      <c r="IH157" s="1"/>
-      <c r="II157" s="1"/>
-      <c r="IJ157" s="1"/>
-      <c r="IK157" s="1"/>
-      <c r="IL157" s="1"/>
-      <c r="IM157" s="1"/>
-      <c r="IN157" s="1"/>
-      <c r="IO157" s="1"/>
-      <c r="IP157" s="1"/>
-      <c r="IQ157" s="1"/>
-      <c r="IR157" s="1"/>
-      <c r="IS157" s="1"/>
-      <c r="IT157" s="1"/>
-      <c r="IU157" s="1"/>
-      <c r="IV157" s="1"/>
+      <c r="K157"/>
+      <c r="L157"/>
+      <c r="M157"/>
+      <c r="N157"/>
+      <c r="O157"/>
+      <c r="P157"/>
+      <c r="Q157"/>
+      <c r="R157"/>
+      <c r="S157"/>
+      <c r="T157"/>
+      <c r="U157"/>
+      <c r="V157"/>
+      <c r="W157"/>
+      <c r="X157"/>
+      <c r="Y157"/>
+      <c r="Z157"/>
+      <c r="AA157"/>
+      <c r="AB157"/>
+      <c r="AC157"/>
+      <c r="AD157"/>
+      <c r="AE157"/>
+      <c r="AF157"/>
+      <c r="AG157"/>
+      <c r="AH157"/>
+      <c r="AI157"/>
+      <c r="AJ157"/>
+      <c r="AK157"/>
+      <c r="AL157"/>
+      <c r="AM157"/>
+      <c r="AN157"/>
+      <c r="AO157"/>
+      <c r="AP157"/>
+      <c r="AQ157"/>
+      <c r="AR157"/>
+      <c r="AS157"/>
+      <c r="AT157"/>
+      <c r="AU157"/>
+      <c r="AV157"/>
+      <c r="AW157"/>
+      <c r="AX157"/>
+      <c r="AY157"/>
+      <c r="AZ157"/>
+      <c r="BA157"/>
+      <c r="BB157"/>
+      <c r="BC157"/>
+      <c r="BD157"/>
+      <c r="BE157"/>
+      <c r="BF157"/>
+      <c r="BG157"/>
+      <c r="BH157"/>
+      <c r="BI157"/>
+      <c r="BJ157"/>
+      <c r="BK157"/>
+      <c r="BL157"/>
+      <c r="BM157"/>
+      <c r="BN157"/>
+      <c r="BO157"/>
+      <c r="BP157"/>
+      <c r="BQ157"/>
+      <c r="BR157"/>
+      <c r="BS157"/>
+      <c r="BT157"/>
+      <c r="BU157"/>
+      <c r="BV157"/>
+      <c r="BW157"/>
+      <c r="BX157"/>
+      <c r="BY157"/>
+      <c r="BZ157"/>
+      <c r="CA157"/>
+      <c r="CB157"/>
+      <c r="CC157"/>
+      <c r="CD157"/>
+      <c r="CE157"/>
+      <c r="CF157"/>
+      <c r="CG157"/>
+      <c r="CH157"/>
+      <c r="CI157"/>
+      <c r="CJ157"/>
+      <c r="CK157"/>
+      <c r="CL157"/>
+      <c r="CM157"/>
+      <c r="CN157"/>
+      <c r="CO157"/>
+      <c r="CP157"/>
+      <c r="CQ157"/>
+      <c r="CR157"/>
+      <c r="CS157"/>
+      <c r="CT157"/>
+      <c r="CU157"/>
+      <c r="CV157"/>
+      <c r="CW157"/>
+      <c r="CX157"/>
+      <c r="CY157"/>
+      <c r="CZ157"/>
+      <c r="DA157"/>
+      <c r="DB157"/>
+      <c r="DC157"/>
+      <c r="DD157"/>
+      <c r="DE157"/>
+      <c r="DF157"/>
+      <c r="DG157"/>
+      <c r="DH157"/>
+      <c r="DI157"/>
+      <c r="DJ157"/>
+      <c r="DK157"/>
+      <c r="DL157"/>
+      <c r="DM157"/>
+      <c r="DN157"/>
+      <c r="DO157"/>
+      <c r="DP157"/>
+      <c r="DQ157"/>
+      <c r="DR157"/>
+      <c r="DS157"/>
+      <c r="DT157"/>
+      <c r="DU157"/>
+      <c r="DV157"/>
+      <c r="DW157"/>
+      <c r="DX157"/>
+      <c r="DY157"/>
+      <c r="DZ157"/>
+      <c r="EA157"/>
+      <c r="EB157"/>
+      <c r="EC157"/>
+      <c r="ED157"/>
+      <c r="EE157"/>
+      <c r="EF157"/>
+      <c r="EG157"/>
+      <c r="EH157"/>
+      <c r="EI157"/>
+      <c r="EJ157"/>
+      <c r="EK157"/>
+      <c r="EL157"/>
+      <c r="EM157"/>
+      <c r="EN157"/>
+      <c r="EO157"/>
+      <c r="EP157"/>
+      <c r="EQ157"/>
+      <c r="ER157"/>
+      <c r="ES157"/>
+      <c r="ET157"/>
+      <c r="EU157"/>
+      <c r="EV157"/>
+      <c r="EW157"/>
+      <c r="EX157"/>
+      <c r="EY157"/>
+      <c r="EZ157"/>
+      <c r="FA157"/>
+      <c r="FB157"/>
+      <c r="FC157"/>
+      <c r="FD157"/>
+      <c r="FE157"/>
+      <c r="FF157"/>
+      <c r="FG157"/>
+      <c r="FH157"/>
+      <c r="FI157"/>
+      <c r="FJ157"/>
+      <c r="FK157"/>
+      <c r="FL157"/>
+      <c r="FM157"/>
+      <c r="FN157"/>
+      <c r="FO157"/>
+      <c r="FP157"/>
+      <c r="FQ157"/>
+      <c r="FR157"/>
+      <c r="FS157"/>
+      <c r="FT157"/>
+      <c r="FU157"/>
+      <c r="FV157"/>
+      <c r="FW157"/>
+      <c r="FX157"/>
+      <c r="FY157"/>
+      <c r="FZ157"/>
+      <c r="GA157"/>
+      <c r="GB157"/>
+      <c r="GC157"/>
+      <c r="GD157"/>
+      <c r="GE157"/>
+      <c r="GF157"/>
+      <c r="GG157"/>
+      <c r="GH157"/>
+      <c r="GI157"/>
+      <c r="GJ157"/>
+      <c r="GK157"/>
+      <c r="GL157"/>
+      <c r="GM157"/>
+      <c r="GN157"/>
+      <c r="GO157"/>
+      <c r="GP157"/>
+      <c r="GQ157"/>
+      <c r="GR157"/>
+      <c r="GS157"/>
+      <c r="GT157"/>
+      <c r="GU157"/>
+      <c r="GV157"/>
+      <c r="GW157"/>
+      <c r="GX157"/>
+      <c r="GY157"/>
+      <c r="GZ157"/>
+      <c r="HA157"/>
+      <c r="HB157"/>
+      <c r="HC157"/>
+      <c r="HD157"/>
+      <c r="HE157"/>
+      <c r="HF157"/>
+      <c r="HG157"/>
+      <c r="HH157"/>
+      <c r="HI157"/>
+      <c r="HJ157"/>
+      <c r="HK157"/>
+      <c r="HL157"/>
+      <c r="HM157"/>
+      <c r="HN157"/>
+      <c r="HO157"/>
+      <c r="HP157"/>
+      <c r="HQ157"/>
+      <c r="HR157"/>
+      <c r="HS157"/>
+      <c r="HT157"/>
+      <c r="HU157"/>
+      <c r="HV157"/>
+      <c r="HW157"/>
+      <c r="HX157"/>
+      <c r="HY157"/>
+      <c r="HZ157"/>
+      <c r="IA157"/>
+      <c r="IB157"/>
+      <c r="IC157"/>
+      <c r="ID157"/>
+      <c r="IE157"/>
+      <c r="IF157"/>
+      <c r="IG157"/>
+      <c r="IH157"/>
+      <c r="II157"/>
+      <c r="IJ157"/>
+      <c r="IK157"/>
+      <c r="IL157"/>
+      <c r="IM157"/>
+      <c r="IN157"/>
+      <c r="IO157"/>
+      <c r="IP157"/>
+      <c r="IQ157"/>
+      <c r="IR157"/>
+      <c r="IS157"/>
+      <c r="IT157"/>
+      <c r="IU157"/>
+      <c r="IV157"/>
     </row>
     <row r="158" ht="12.8">
       <c r="K158" s="1"/>

</xml_diff>